<commit_message>
bug correction with variables attributes type. use only string and numeric in second line of roscop file descriptor and cast with the right physical parameter type (column types) Add to short cnv file fr2599? for testing improve debug mode and error display cf-checker results: ------------------ Checking variable: DEPTH ------------------ INFO: attribute '_FillValue' is being used in a non-standard way WARNING (5): Possible incorrect declaration of a coordinate variable.
</commit_message>
<xml_diff>
--- a/roscop/code_roscop.xlsx
+++ b/roscop/code_roscop.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgrelet\go\src\github.com\jgrelet\oceano2oceansites\roscop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="90" yWindow="15" windowWidth="14505" windowHeight="8415"/>
+    <workbookView xWindow="96" yWindow="12" windowWidth="14508" windowHeight="8412"/>
   </bookViews>
   <sheets>
     <sheet name="code_roscop" sheetId="5" r:id="rId1"/>
@@ -52,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="226">
   <si>
     <t>long_name</t>
   </si>
@@ -75,9 +70,6 @@
     <t>format</t>
   </si>
   <si>
-    <t>FillValue_</t>
-  </si>
-  <si>
     <t>axis</t>
   </si>
   <si>
@@ -702,9 +694,6 @@
     <t>pss</t>
   </si>
   <si>
-    <t>none</t>
-  </si>
-  <si>
     <t>speed_of_sound_in_sea_water</t>
   </si>
   <si>
@@ -732,18 +721,21 @@
     <t>Relative julian days with decimal part (as parts of the day)</t>
   </si>
   <si>
-    <t xml:space="preserve">Depth calculated from pressure measurement </t>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>_FillValue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0E+00"/>
     <numFmt numFmtId="165" formatCode="0.E+00"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="27">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1320,7 +1312,7 @@
     <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1337,9 +1329,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1548,7 +1537,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1580,10 +1569,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1615,7 +1603,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1791,60 +1778,60 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O9" sqref="O9"/>
+      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="14"/>
+    <col min="1" max="1" width="11.5546875" style="13"/>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="34.85546875" customWidth="1"/>
-    <col min="4" max="4" width="28.85546875" style="22" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" style="18" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
-    <col min="7" max="7" width="32.85546875" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" customWidth="1"/>
-    <col min="9" max="9" width="7.5703125" style="6" customWidth="1"/>
-    <col min="10" max="10" width="8.140625" style="6" customWidth="1"/>
-    <col min="11" max="11" width="7.42578125" style="6" customWidth="1"/>
-    <col min="12" max="12" width="7.85546875" style="11" customWidth="1"/>
-    <col min="13" max="13" width="5.7109375" style="6" customWidth="1"/>
-    <col min="14" max="14" width="8.5703125" style="6" customWidth="1"/>
-    <col min="15" max="15" width="34.140625" customWidth="1"/>
-    <col min="16" max="16" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="34.88671875" customWidth="1"/>
+    <col min="4" max="4" width="28.88671875" style="21" customWidth="1"/>
+    <col min="5" max="5" width="24.109375" style="17" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" customWidth="1"/>
+    <col min="7" max="7" width="32.88671875" customWidth="1"/>
+    <col min="8" max="8" width="6.109375" customWidth="1"/>
+    <col min="9" max="9" width="7.5546875" style="6" customWidth="1"/>
+    <col min="10" max="10" width="8.109375" style="6" customWidth="1"/>
+    <col min="11" max="11" width="7.44140625" style="6" customWidth="1"/>
+    <col min="12" max="12" width="7.88671875" style="10" customWidth="1"/>
+    <col min="13" max="13" width="5.6640625" style="6" customWidth="1"/>
+    <col min="14" max="14" width="8.5546875" style="6" customWidth="1"/>
+    <col min="15" max="15" width="34.109375" customWidth="1"/>
+    <col min="16" max="16" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:21">
+      <c r="A1" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="15" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>4</v>
@@ -1856,126 +1843,126 @@
         <v>6</v>
       </c>
       <c r="L1" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="P1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="S1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="T1" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="T1" s="7" t="s">
-        <v>183</v>
-      </c>
       <c r="U1" s="8"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
-        <v>15</v>
+    <row r="2" spans="1:21">
+      <c r="A2" s="12" t="s">
+        <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>168</v>
+        <v>224</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>168</v>
+        <v>224</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>168</v>
+        <v>14</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>224</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>168</v>
+        <v>224</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>168</v>
+        <v>14</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>224</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="U2" s="2"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
-        <v>88</v>
+    <row r="3" spans="1:21">
+      <c r="A3" s="13" t="s">
+        <v>87</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="19">
+        <v>110</v>
+      </c>
+      <c r="D3" s="22"/>
+      <c r="E3" s="18">
         <v>1</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12" t="s">
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="L3" s="23">
+        <v>99999</v>
+      </c>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="L3" s="24">
-        <v>99999</v>
-      </c>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
@@ -1983,35 +1970,35 @@
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A4" s="14" t="s">
+    <row r="4" spans="1:21">
+      <c r="A4" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="19">
+      <c r="D4" s="22"/>
+      <c r="E4" s="18">
         <v>1</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12" t="s">
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4" s="23">
+        <v>99999</v>
+      </c>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="L4" s="24">
-        <v>99999</v>
-      </c>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
@@ -2019,123 +2006,117 @@
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A5" s="14" t="s">
-        <v>20</v>
+    <row r="5" spans="1:21">
+      <c r="A5" s="13" t="s">
+        <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>175</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>178</v>
+        <v>179</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>177</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M5" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="N5" s="12"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="N5" s="11"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
       <c r="S5" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="T5" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="T5" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A6" s="14" t="s">
-        <v>21</v>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6" s="13" t="s">
+        <v>20</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="D6" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="E6" s="18" t="s">
         <v>176</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>177</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M6" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="N6" s="12"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="N6" s="11"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
       <c r="S6" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="14" t="s">
-        <v>19</v>
+        <v>185</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="15">
+      <c r="A7" s="13" t="s">
+        <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D7" s="22" t="s">
         <v>173</v>
       </c>
-      <c r="D7" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="37" t="s">
-        <v>225</v>
+      <c r="E7" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="36" t="s">
+        <v>223</v>
       </c>
       <c r="G7" s="3"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="12">
+      <c r="H7" s="24"/>
+      <c r="I7" s="11">
         <v>0</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="11">
         <v>90000</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="K7" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="L7" s="27"/>
+      <c r="M7" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="L7" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M7" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="N7" s="12"/>
+      <c r="N7" s="11"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
@@ -2143,37 +2124,35 @@
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A8" s="14" t="s">
+    <row r="8" spans="1:21">
+      <c r="A8" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="19">
+      <c r="D8" s="22"/>
+      <c r="E8" s="18">
         <v>1</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="12">
+      <c r="H8" s="24"/>
+      <c r="I8" s="11">
         <v>0</v>
       </c>
-      <c r="J8" s="12">
+      <c r="J8" s="11">
         <v>90000</v>
       </c>
-      <c r="K8" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="L8" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
+      <c r="K8" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="L8" s="27"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
@@ -2181,91 +2160,89 @@
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A9" s="14" t="s">
-        <v>112</v>
+    <row r="9" spans="1:21">
+      <c r="A9" s="13" t="s">
+        <v>111</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>214</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>159</v>
+        <v>189</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>213</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>158</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I9" s="12">
+        <v>50</v>
+      </c>
+      <c r="I9" s="11">
         <v>0</v>
       </c>
-      <c r="J9" s="12">
+      <c r="J9" s="11">
         <v>9000</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="L9" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M9" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="L9" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M9" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="N9" s="12"/>
-      <c r="O9" s="3" t="s">
-        <v>226</v>
-      </c>
+      <c r="N9" s="11"/>
+      <c r="O9" s="3"/>
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
       <c r="T9" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A10" s="14" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="A10" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>213</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>221</v>
+      <c r="D10" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>219</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="11">
+        <v>0</v>
+      </c>
+      <c r="J10" s="11">
+        <v>9000</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="3" t="s">
         <v>220</v>
-      </c>
-      <c r="H10" s="3"/>
-      <c r="I10" s="12">
-        <v>0</v>
-      </c>
-      <c r="J10" s="12">
-        <v>9000</v>
-      </c>
-      <c r="K10" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="L10" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="3" t="s">
-        <v>222</v>
       </c>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
@@ -2273,45 +2250,45 @@
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A11" s="14" t="s">
-        <v>56</v>
+    <row r="11" spans="1:21">
+      <c r="A11" s="13" t="s">
+        <v>55</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>18</v>
+        <v>90</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>17</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H11" s="3"/>
-      <c r="I11" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J11" s="12">
+      <c r="I11" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11" s="11">
         <v>38</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="K11" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="L11" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="L11" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12" t="s">
-        <v>13</v>
-      </c>
       <c r="O11" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
@@ -2319,45 +2296,45 @@
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A12" s="14" t="s">
+    <row r="12" spans="1:21">
+      <c r="A12" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D12" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12" s="19">
+      <c r="E12" s="18">
         <v>1</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H12" s="3"/>
-      <c r="I12" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J12" s="12">
+      <c r="I12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" s="11">
         <v>38</v>
       </c>
-      <c r="K12" s="12" t="s">
+      <c r="K12" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="L12" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="L12" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12" t="s">
-        <v>13</v>
-      </c>
       <c r="O12" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
@@ -2365,45 +2342,45 @@
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A13" s="14" t="s">
+    <row r="13" spans="1:21">
+      <c r="A13" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>216</v>
+      </c>
+      <c r="E13" s="18" t="s">
         <v>60</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D13" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>61</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H13" s="3"/>
-      <c r="I13" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J13" s="12">
+      <c r="I13" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="J13" s="11">
         <v>38</v>
       </c>
-      <c r="K13" s="12" t="s">
+      <c r="K13" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="L13" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="L13" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12" t="s">
-        <v>13</v>
-      </c>
       <c r="O13" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
@@ -2411,45 +2388,45 @@
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A14" s="14" t="s">
+    <row r="14" spans="1:21">
+      <c r="A14" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D14" s="23" t="s">
+      <c r="E14" s="18" t="s">
         <v>64</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>65</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H14" s="3"/>
-      <c r="I14" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J14" s="12">
+      <c r="I14" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14" s="11">
         <v>38</v>
       </c>
-      <c r="K14" s="12" t="s">
+      <c r="K14" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="L14" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="L14" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12" t="s">
-        <v>13</v>
-      </c>
       <c r="O14" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
@@ -2457,45 +2434,45 @@
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A15" s="14" t="s">
-        <v>69</v>
+    <row r="15" spans="1:21">
+      <c r="A15" s="13" t="s">
+        <v>68</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D15" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>36</v>
+        <v>94</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>35</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H15" s="3"/>
-      <c r="I15" s="12">
+      <c r="I15" s="11">
         <v>1350</v>
       </c>
-      <c r="J15" s="12">
+      <c r="J15" s="11">
         <v>1600</v>
       </c>
-      <c r="K15" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="L15" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12" t="s">
-        <v>13</v>
+      <c r="K15" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="L15" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
@@ -2503,45 +2480,45 @@
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A16" s="14" t="s">
+    <row r="16" spans="1:21">
+      <c r="A16" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D16" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="D16" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16" s="19" t="s">
-        <v>18</v>
+      <c r="E16" s="18" t="s">
+        <v>17</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H16" s="3"/>
-      <c r="I16" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J16" s="12">
+      <c r="I16" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="J16" s="11">
         <v>38</v>
       </c>
-      <c r="K16" s="12" t="s">
+      <c r="K16" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="L16" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="L16" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12" t="s">
-        <v>13</v>
-      </c>
       <c r="O16" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
@@ -2549,45 +2526,45 @@
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A17" s="14" t="s">
-        <v>77</v>
+    <row r="17" spans="1:20">
+      <c r="A17" s="13" t="s">
+        <v>76</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D17" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="18" t="s">
         <v>35</v>
-      </c>
-      <c r="E17" s="19" t="s">
-        <v>36</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H17" s="3"/>
-      <c r="I17" s="12">
+      <c r="I17" s="11">
         <v>0</v>
       </c>
-      <c r="J17" s="12">
+      <c r="J17" s="11">
         <v>200</v>
       </c>
-      <c r="K17" s="12" t="s">
+      <c r="K17" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="L17" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="L17" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12" t="s">
-        <v>13</v>
-      </c>
       <c r="O17" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
@@ -2595,45 +2572,45 @@
       <c r="S17" s="3"/>
       <c r="T17" s="3"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A18" s="14" t="s">
+    <row r="18" spans="1:20">
+      <c r="A18" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D18" s="23" t="s">
+      <c r="E18" s="18" t="s">
         <v>38</v>
-      </c>
-      <c r="E18" s="19" t="s">
-        <v>39</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H18" s="3"/>
-      <c r="I18" s="12">
+      <c r="I18" s="11">
         <v>0</v>
       </c>
-      <c r="J18" s="12">
+      <c r="J18" s="11">
         <v>360</v>
       </c>
-      <c r="K18" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="L18" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12" t="s">
-        <v>13</v>
+      <c r="K18" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="L18" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
@@ -2641,45 +2618,45 @@
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A19" s="14" t="s">
+    <row r="19" spans="1:20">
+      <c r="A19" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D19" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D19" s="23" t="s">
+      <c r="E19" s="18" t="s">
         <v>41</v>
-      </c>
-      <c r="E19" s="19" t="s">
-        <v>42</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H19" s="3"/>
-      <c r="I19" s="12">
+      <c r="I19" s="11">
         <v>940</v>
       </c>
-      <c r="J19" s="12">
+      <c r="J19" s="11">
         <v>1030</v>
       </c>
-      <c r="K19" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="L19" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M19" s="12"/>
-      <c r="N19" s="12" t="s">
-        <v>13</v>
+      <c r="K19" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="L19" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
@@ -2687,45 +2664,45 @@
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A20" s="14" t="s">
-        <v>44</v>
+    <row r="20" spans="1:20">
+      <c r="A20" s="13" t="s">
+        <v>43</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D20" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="18" t="s">
         <v>46</v>
-      </c>
-      <c r="E20" s="19" t="s">
-        <v>47</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H20" s="3"/>
-      <c r="I20" s="12">
+      <c r="I20" s="11">
         <v>0</v>
       </c>
-      <c r="J20" s="12">
+      <c r="J20" s="11">
         <v>100</v>
       </c>
-      <c r="K20" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="L20" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M20" s="12"/>
-      <c r="N20" s="12" t="s">
-        <v>13</v>
+      <c r="K20" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="L20" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
@@ -2733,43 +2710,43 @@
       <c r="S20" s="3"/>
       <c r="T20" s="3"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A21" s="14" t="s">
-        <v>71</v>
+    <row r="21" spans="1:20">
+      <c r="A21" s="13" t="s">
+        <v>70</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D21" s="23"/>
-      <c r="E21" s="19" t="s">
-        <v>80</v>
+        <v>100</v>
+      </c>
+      <c r="D21" s="22"/>
+      <c r="E21" s="18" t="s">
+        <v>79</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H21" s="3"/>
-      <c r="I21" s="12">
+      <c r="I21" s="11">
         <v>-100</v>
       </c>
-      <c r="J21" s="12">
+      <c r="J21" s="11">
         <v>100</v>
       </c>
-      <c r="K21" s="12" t="s">
+      <c r="K21" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="L21" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="L21" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M21" s="12"/>
-      <c r="N21" s="12" t="s">
+      <c r="O21" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="O21" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
@@ -2777,43 +2754,43 @@
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A22" s="14" t="s">
-        <v>72</v>
+    <row r="22" spans="1:20">
+      <c r="A22" s="13" t="s">
+        <v>71</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D22" s="23"/>
-      <c r="E22" s="19" t="s">
-        <v>80</v>
+        <v>101</v>
+      </c>
+      <c r="D22" s="22"/>
+      <c r="E22" s="18" t="s">
+        <v>79</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H22" s="3"/>
-      <c r="I22" s="12">
+      <c r="I22" s="11">
         <v>-100</v>
       </c>
-      <c r="J22" s="12">
+      <c r="J22" s="11">
         <v>100</v>
       </c>
-      <c r="K22" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="L22" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M22" s="12"/>
-      <c r="N22" s="12" t="s">
-        <v>16</v>
+      <c r="K22" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="L22" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11" t="s">
+        <v>15</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="P22" s="3"/>
       <c r="Q22" s="3"/>
@@ -2821,45 +2798,45 @@
       <c r="S22" s="3"/>
       <c r="T22" s="3"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A23" s="14" t="s">
-        <v>67</v>
+    <row r="23" spans="1:20">
+      <c r="A23" s="13" t="s">
+        <v>66</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D23" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>18</v>
+        <v>102</v>
+      </c>
+      <c r="D23" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>17</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H23" s="3"/>
-      <c r="I23" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J23" s="12">
+      <c r="I23" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="J23" s="11">
         <v>38</v>
       </c>
-      <c r="K23" s="12" t="s">
+      <c r="K23" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="L23" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="L23" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M23" s="12"/>
-      <c r="N23" s="12" t="s">
-        <v>13</v>
-      </c>
       <c r="O23" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
@@ -2867,45 +2844,45 @@
       <c r="S23" s="3"/>
       <c r="T23" s="3"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A24" s="14" t="s">
-        <v>30</v>
+    <row r="24" spans="1:20">
+      <c r="A24" s="13" t="s">
+        <v>29</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D24" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" s="19" t="s">
-        <v>18</v>
+        <v>103</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>17</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H24" s="3"/>
-      <c r="I24" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J24" s="12">
+      <c r="I24" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="J24" s="11">
         <v>38</v>
       </c>
-      <c r="K24" s="12" t="s">
+      <c r="K24" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="L24" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="L24" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M24" s="12"/>
-      <c r="N24" s="12" t="s">
-        <v>13</v>
-      </c>
       <c r="O24" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
@@ -2913,45 +2890,45 @@
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A25" s="14" t="s">
-        <v>68</v>
+    <row r="25" spans="1:20">
+      <c r="A25" s="13" t="s">
+        <v>67</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D25" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>215</v>
+        <v>104</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>214</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H25" s="3"/>
-      <c r="I25" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J25" s="12">
+      <c r="I25" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="J25" s="11">
         <v>38</v>
       </c>
-      <c r="K25" s="12" t="s">
+      <c r="K25" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="L25" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="L25" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M25" s="12"/>
-      <c r="N25" s="12" t="s">
-        <v>13</v>
-      </c>
       <c r="O25" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
@@ -2959,40 +2936,40 @@
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A26" s="14" t="s">
+    <row r="26" spans="1:20">
+      <c r="A26" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D26" s="22"/>
+      <c r="E26" s="18" t="s">
         <v>81</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D26" s="23"/>
-      <c r="E26" s="19" t="s">
-        <v>82</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H26" s="3"/>
-      <c r="I26" s="12">
+      <c r="I26" s="11">
         <v>100</v>
       </c>
-      <c r="J26" s="12">
+      <c r="J26" s="11">
         <v>700</v>
       </c>
-      <c r="K26" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="L26" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M26" s="12"/>
-      <c r="N26" s="12" t="s">
-        <v>13</v>
+      <c r="K26" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="L26" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
@@ -3001,40 +2978,40 @@
       <c r="S26" s="3"/>
       <c r="T26" s="3"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A27" s="14" t="s">
+    <row r="27" spans="1:20">
+      <c r="A27" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D27" s="22"/>
+      <c r="E27" s="18" t="s">
         <v>83</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D27" s="23"/>
-      <c r="E27" s="19" t="s">
-        <v>84</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H27" s="3"/>
-      <c r="I27" s="12">
+      <c r="I27" s="11">
         <v>0</v>
       </c>
-      <c r="J27" s="12">
+      <c r="J27" s="11">
         <v>1</v>
       </c>
-      <c r="K27" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="L27" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M27" s="12"/>
-      <c r="N27" s="12" t="s">
-        <v>13</v>
+      <c r="K27" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="L27" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M27" s="11"/>
+      <c r="N27" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
@@ -3043,40 +3020,40 @@
       <c r="S27" s="3"/>
       <c r="T27" s="3"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A28" s="26" t="s">
+    <row r="28" spans="1:20">
+      <c r="A28" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C28" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C28" s="29" t="s">
+      <c r="D28" s="22"/>
+      <c r="E28" s="29" t="s">
         <v>204</v>
-      </c>
-      <c r="D28" s="23"/>
-      <c r="E28" s="30" t="s">
-        <v>205</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H28" s="3"/>
-      <c r="I28" s="31">
+      <c r="I28" s="30">
         <v>0</v>
       </c>
-      <c r="J28" s="31">
+      <c r="J28" s="30">
         <v>10</v>
       </c>
-      <c r="K28" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="L28" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M28" s="12"/>
-      <c r="N28" s="12" t="s">
-        <v>13</v>
+      <c r="K28" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="L28" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="O28" s="3"/>
       <c r="P28" s="3"/>
@@ -3085,40 +3062,40 @@
       <c r="S28" s="3"/>
       <c r="T28" s="3"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A29" s="14" t="s">
-        <v>86</v>
+    <row r="29" spans="1:20">
+      <c r="A29" s="13" t="s">
+        <v>85</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D29" s="23"/>
-      <c r="E29" s="19" t="s">
-        <v>47</v>
+        <v>107</v>
+      </c>
+      <c r="D29" s="22"/>
+      <c r="E29" s="18" t="s">
+        <v>46</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H29" s="3"/>
-      <c r="I29" s="12">
+      <c r="I29" s="11">
         <v>0</v>
       </c>
-      <c r="J29" s="12">
+      <c r="J29" s="11">
         <v>100</v>
       </c>
-      <c r="K29" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="L29" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M29" s="12"/>
-      <c r="N29" s="12" t="s">
-        <v>13</v>
+      <c r="K29" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="L29" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
@@ -3127,40 +3104,40 @@
       <c r="S29" s="3"/>
       <c r="T29" s="3"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A30" s="26" t="s">
+    <row r="30" spans="1:20">
+      <c r="A30" s="25" t="s">
+        <v>194</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C30" s="28" t="s">
         <v>195</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C30" s="29" t="s">
+      <c r="D30" s="22"/>
+      <c r="E30" s="18" t="s">
         <v>196</v>
-      </c>
-      <c r="D30" s="23"/>
-      <c r="E30" s="19" t="s">
-        <v>197</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H30" s="3"/>
-      <c r="I30" s="31">
+      <c r="I30" s="30">
         <v>0</v>
       </c>
-      <c r="J30" s="31">
+      <c r="J30" s="30">
         <v>3000</v>
       </c>
-      <c r="K30" s="31" t="s">
-        <v>198</v>
-      </c>
-      <c r="L30" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M30" s="12"/>
-      <c r="N30" s="12" t="s">
-        <v>13</v>
+      <c r="K30" s="30" t="s">
+        <v>197</v>
+      </c>
+      <c r="L30" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="O30" s="3"/>
       <c r="P30" s="3"/>
@@ -3169,40 +3146,40 @@
       <c r="S30" s="3"/>
       <c r="T30" s="3"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A31" s="26" t="s">
+    <row r="31" spans="1:20">
+      <c r="A31" s="25" t="s">
+        <v>198</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C31" s="28" t="s">
         <v>199</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C31" s="29" t="s">
-        <v>200</v>
-      </c>
-      <c r="D31" s="23"/>
-      <c r="E31" s="19" t="s">
-        <v>197</v>
+      <c r="D31" s="22"/>
+      <c r="E31" s="18" t="s">
+        <v>196</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H31" s="3"/>
-      <c r="I31" s="31">
+      <c r="I31" s="30">
         <v>0</v>
       </c>
-      <c r="J31" s="31">
+      <c r="J31" s="30">
         <v>4000</v>
       </c>
-      <c r="K31" s="31" t="s">
-        <v>198</v>
-      </c>
-      <c r="L31" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M31" s="12"/>
-      <c r="N31" s="12" t="s">
-        <v>13</v>
+      <c r="K31" s="30" t="s">
+        <v>197</v>
+      </c>
+      <c r="L31" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M31" s="11"/>
+      <c r="N31" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="O31" s="3"/>
       <c r="P31" s="3"/>
@@ -3211,40 +3188,40 @@
       <c r="S31" s="3"/>
       <c r="T31" s="3"/>
     </row>
-    <row r="32" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="26" t="s">
+    <row r="32" spans="1:20" ht="12.6" customHeight="1">
+      <c r="A32" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C32" s="28" t="s">
         <v>201</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C32" s="29" t="s">
-        <v>202</v>
-      </c>
-      <c r="D32" s="23"/>
-      <c r="E32" s="19" t="s">
-        <v>197</v>
+      <c r="D32" s="22"/>
+      <c r="E32" s="18" t="s">
+        <v>196</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H32" s="3"/>
-      <c r="I32" s="31">
+      <c r="I32" s="30">
         <v>0</v>
       </c>
-      <c r="J32" s="31">
+      <c r="J32" s="30">
         <v>3000</v>
       </c>
-      <c r="K32" s="31" t="s">
-        <v>198</v>
-      </c>
-      <c r="L32" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M32" s="12"/>
-      <c r="N32" s="12" t="s">
-        <v>13</v>
+      <c r="K32" s="30" t="s">
+        <v>197</v>
+      </c>
+      <c r="L32" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M32" s="11"/>
+      <c r="N32" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="O32" s="3"/>
       <c r="P32" s="3"/>
@@ -3253,40 +3230,40 @@
       <c r="S32" s="3"/>
       <c r="T32" s="3"/>
     </row>
-    <row r="33" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="27" t="s">
+    <row r="33" spans="1:20" ht="12.6" customHeight="1">
+      <c r="A33" s="26" t="s">
+        <v>205</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C33" s="31" t="s">
         <v>206</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C33" s="32" t="s">
+      <c r="D33" s="22"/>
+      <c r="E33" s="32" t="s">
         <v>207</v>
-      </c>
-      <c r="D33" s="23"/>
-      <c r="E33" s="33" t="s">
-        <v>208</v>
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H33" s="3"/>
-      <c r="I33" s="32">
+      <c r="I33" s="31">
         <v>0</v>
       </c>
-      <c r="J33" s="34">
+      <c r="J33" s="33">
         <v>999999</v>
       </c>
-      <c r="K33" s="34" t="s">
-        <v>209</v>
-      </c>
-      <c r="L33" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M33" s="12"/>
-      <c r="N33" s="12" t="s">
-        <v>13</v>
+      <c r="K33" s="33" t="s">
+        <v>208</v>
+      </c>
+      <c r="L33" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M33" s="11"/>
+      <c r="N33" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
@@ -3295,40 +3272,40 @@
       <c r="S33" s="3"/>
       <c r="T33" s="3"/>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A34" s="14" t="s">
-        <v>67</v>
+    <row r="34" spans="1:20">
+      <c r="A34" s="13" t="s">
+        <v>66</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D34" s="23"/>
-      <c r="E34" s="19" t="s">
-        <v>18</v>
+        <v>102</v>
+      </c>
+      <c r="D34" s="22"/>
+      <c r="E34" s="18" t="s">
+        <v>17</v>
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H34" s="3"/>
-      <c r="I34" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J34" s="12">
+      <c r="I34" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="J34" s="11">
         <v>38</v>
       </c>
-      <c r="K34" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="L34" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M34" s="12"/>
-      <c r="N34" s="12" t="s">
-        <v>13</v>
+      <c r="K34" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="L34" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M34" s="11"/>
+      <c r="N34" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="O34" s="3"/>
       <c r="P34" s="3"/>
@@ -3337,40 +3314,40 @@
       <c r="S34" s="3"/>
       <c r="T34" s="3"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A35" s="14" t="s">
+    <row r="35" spans="1:20">
+      <c r="A35" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D35" s="23"/>
-      <c r="E35" s="19" t="s">
-        <v>216</v>
+      <c r="D35" s="22"/>
+      <c r="E35" s="18">
+        <v>1</v>
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H35" s="3"/>
-      <c r="I35" s="12" t="s">
+      <c r="I35" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="J35" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="J35" s="12" t="s">
+      <c r="K35" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="K35" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="L35" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M35" s="12"/>
-      <c r="N35" s="12" t="s">
-        <v>13</v>
+      <c r="L35" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M35" s="11"/>
+      <c r="N35" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="O35" s="3"/>
       <c r="P35" s="3"/>
@@ -3379,40 +3356,40 @@
       <c r="S35" s="3"/>
       <c r="T35" s="3"/>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A36" s="14" t="s">
+    <row r="36" spans="1:20">
+      <c r="A36" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="D36" s="23"/>
-      <c r="E36" s="19" t="s">
-        <v>18</v>
+      <c r="D36" s="22"/>
+      <c r="E36" s="18" t="s">
+        <v>17</v>
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H36" s="3"/>
-      <c r="I36" s="12">
+      <c r="I36" s="11">
         <v>-2</v>
       </c>
-      <c r="J36" s="12">
+      <c r="J36" s="11">
         <v>32</v>
       </c>
-      <c r="K36" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="L36" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M36" s="12"/>
-      <c r="N36" s="12" t="s">
-        <v>13</v>
+      <c r="K36" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="L36" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M36" s="11"/>
+      <c r="N36" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="O36" s="3"/>
       <c r="P36" s="3"/>
@@ -3421,40 +3398,40 @@
       <c r="S36" s="3"/>
       <c r="T36" s="3"/>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A37" s="14" t="s">
+    <row r="37" spans="1:20">
+      <c r="A37" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="D37" s="23"/>
-      <c r="E37" s="19" t="s">
-        <v>18</v>
+      <c r="D37" s="22"/>
+      <c r="E37" s="18" t="s">
+        <v>17</v>
       </c>
       <c r="F37" s="3"/>
       <c r="G37" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H37" s="3"/>
-      <c r="I37" s="12">
+      <c r="I37" s="11">
         <v>-2</v>
       </c>
-      <c r="J37" s="12">
+      <c r="J37" s="11">
         <v>32</v>
       </c>
-      <c r="K37" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="L37" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M37" s="12"/>
-      <c r="N37" s="12" t="s">
-        <v>13</v>
+      <c r="K37" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="L37" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M37" s="11"/>
+      <c r="N37" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="O37" s="3"/>
       <c r="P37" s="3"/>
@@ -3463,40 +3440,40 @@
       <c r="S37" s="3"/>
       <c r="T37" s="3"/>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A38" s="14" t="s">
+    <row r="38" spans="1:20">
+      <c r="A38" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="D38" s="23"/>
-      <c r="E38" s="19" t="s">
-        <v>215</v>
+      <c r="D38" s="22"/>
+      <c r="E38" s="18" t="s">
+        <v>214</v>
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H38" s="3"/>
-      <c r="I38" s="12">
+      <c r="I38" s="11">
         <v>33</v>
       </c>
-      <c r="J38" s="12">
+      <c r="J38" s="11">
         <v>37</v>
       </c>
-      <c r="K38" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="L38" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M38" s="12"/>
-      <c r="N38" s="12" t="s">
-        <v>13</v>
+      <c r="K38" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="L38" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M38" s="11"/>
+      <c r="N38" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="O38" s="3"/>
       <c r="P38" s="3"/>
@@ -3505,40 +3482,40 @@
       <c r="S38" s="3"/>
       <c r="T38" s="3"/>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A39" s="14" t="s">
+    <row r="39" spans="1:20">
+      <c r="A39" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="D39" s="23"/>
-      <c r="E39" s="19" t="s">
-        <v>215</v>
+      <c r="D39" s="22"/>
+      <c r="E39" s="18" t="s">
+        <v>214</v>
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H39" s="3"/>
-      <c r="I39" s="12">
+      <c r="I39" s="11">
         <v>33</v>
       </c>
-      <c r="J39" s="12">
+      <c r="J39" s="11">
         <v>37</v>
       </c>
-      <c r="K39" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="L39" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M39" s="12"/>
-      <c r="N39" s="12" t="s">
-        <v>13</v>
+      <c r="K39" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="L39" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M39" s="11"/>
+      <c r="N39" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="O39" s="3"/>
       <c r="P39" s="3"/>
@@ -3547,40 +3524,40 @@
       <c r="S39" s="3"/>
       <c r="T39" s="3"/>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A40" s="14" t="s">
+    <row r="40" spans="1:20">
+      <c r="A40" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B40" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C40" s="3" t="s">
+      <c r="D40" s="22"/>
+      <c r="E40" s="18" t="s">
         <v>128</v>
-      </c>
-      <c r="D40" s="23"/>
-      <c r="E40" s="19" t="s">
-        <v>129</v>
       </c>
       <c r="F40" s="3"/>
       <c r="G40" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H40" s="3"/>
-      <c r="I40" s="12">
+      <c r="I40" s="11">
         <v>3</v>
       </c>
-      <c r="J40" s="12">
+      <c r="J40" s="11">
         <v>7</v>
       </c>
-      <c r="K40" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="L40" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M40" s="12"/>
-      <c r="N40" s="12" t="s">
-        <v>13</v>
+      <c r="K40" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="L40" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M40" s="11"/>
+      <c r="N40" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="O40" s="3"/>
       <c r="P40" s="3"/>
@@ -3589,40 +3566,40 @@
       <c r="S40" s="3"/>
       <c r="T40" s="3"/>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A41" s="14" t="s">
+    <row r="41" spans="1:20">
+      <c r="A41" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="D41" s="23"/>
-      <c r="E41" s="19" t="s">
-        <v>129</v>
+      <c r="D41" s="22"/>
+      <c r="E41" s="18" t="s">
+        <v>128</v>
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H41" s="3"/>
-      <c r="I41" s="12">
+      <c r="I41" s="11">
         <v>3</v>
       </c>
-      <c r="J41" s="12">
+      <c r="J41" s="11">
         <v>7</v>
       </c>
-      <c r="K41" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="L41" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M41" s="12"/>
-      <c r="N41" s="12" t="s">
-        <v>13</v>
+      <c r="K41" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="L41" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M41" s="11"/>
+      <c r="N41" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="O41" s="3"/>
       <c r="P41" s="3"/>
@@ -3631,40 +3608,40 @@
       <c r="S41" s="3"/>
       <c r="T41" s="3"/>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A42" s="14" t="s">
+    <row r="42" spans="1:20">
+      <c r="A42" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B42" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C42" s="3" t="s">
+      <c r="D42" s="22"/>
+      <c r="E42" s="18" t="s">
         <v>134</v>
-      </c>
-      <c r="D42" s="23"/>
-      <c r="E42" s="19" t="s">
-        <v>135</v>
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H42" s="3"/>
-      <c r="I42" s="12">
+      <c r="I42" s="11">
         <v>0</v>
       </c>
-      <c r="J42" s="12">
+      <c r="J42" s="11">
         <v>10</v>
       </c>
-      <c r="K42" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="L42" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M42" s="12"/>
-      <c r="N42" s="12" t="s">
-        <v>13</v>
+      <c r="K42" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="L42" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M42" s="11"/>
+      <c r="N42" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="O42" s="3"/>
       <c r="P42" s="3"/>
@@ -3673,40 +3650,40 @@
       <c r="S42" s="3"/>
       <c r="T42" s="3"/>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A43" s="14" t="s">
+    <row r="43" spans="1:20">
+      <c r="A43" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B43" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D43" s="23"/>
-      <c r="E43" s="19" t="s">
-        <v>135</v>
+      <c r="D43" s="22"/>
+      <c r="E43" s="18" t="s">
+        <v>134</v>
       </c>
       <c r="F43" s="3"/>
       <c r="G43" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H43" s="3"/>
-      <c r="I43" s="12">
+      <c r="I43" s="11">
         <v>0</v>
       </c>
-      <c r="J43" s="12">
+      <c r="J43" s="11">
         <v>10</v>
       </c>
-      <c r="K43" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="L43" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M43" s="12"/>
-      <c r="N43" s="12" t="s">
-        <v>13</v>
+      <c r="K43" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="L43" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M43" s="11"/>
+      <c r="N43" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="O43" s="3"/>
       <c r="P43" s="3"/>
@@ -3715,40 +3692,40 @@
       <c r="S43" s="3"/>
       <c r="T43" s="3"/>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A44" s="14" t="s">
-        <v>139</v>
+    <row r="44" spans="1:20">
+      <c r="A44" s="13" t="s">
+        <v>138</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="D44" s="23"/>
-      <c r="E44" s="19" t="s">
-        <v>61</v>
+        <v>133</v>
+      </c>
+      <c r="D44" s="22"/>
+      <c r="E44" s="18" t="s">
+        <v>60</v>
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H44" s="3"/>
-      <c r="I44" s="12">
+      <c r="I44" s="11">
         <v>0</v>
       </c>
-      <c r="J44" s="12">
+      <c r="J44" s="11">
         <v>450</v>
       </c>
-      <c r="K44" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="L44" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M44" s="12"/>
-      <c r="N44" s="12" t="s">
-        <v>13</v>
+      <c r="K44" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="L44" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M44" s="11"/>
+      <c r="N44" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="O44" s="3"/>
       <c r="P44" s="3"/>
@@ -3757,40 +3734,40 @@
       <c r="S44" s="3"/>
       <c r="T44" s="3"/>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A45" s="14" t="s">
-        <v>141</v>
+    <row r="45" spans="1:20">
+      <c r="A45" s="13" t="s">
+        <v>140</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D45" s="23"/>
-      <c r="E45" s="19" t="s">
-        <v>61</v>
+        <v>137</v>
+      </c>
+      <c r="D45" s="22"/>
+      <c r="E45" s="18" t="s">
+        <v>60</v>
       </c>
       <c r="F45" s="3"/>
       <c r="G45" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H45" s="3"/>
-      <c r="I45" s="12">
+      <c r="I45" s="11">
         <v>0</v>
       </c>
-      <c r="J45" s="12">
+      <c r="J45" s="11">
         <v>450</v>
       </c>
-      <c r="K45" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="L45" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M45" s="12"/>
-      <c r="N45" s="12" t="s">
-        <v>13</v>
+      <c r="K45" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="L45" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M45" s="11"/>
+      <c r="N45" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="O45" s="3"/>
       <c r="P45" s="3"/>
@@ -3799,40 +3776,40 @@
       <c r="S45" s="3"/>
       <c r="T45" s="3"/>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A46" s="14" t="s">
+    <row r="46" spans="1:20">
+      <c r="A46" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C46" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B46" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C46" s="3" t="s">
+      <c r="D46" s="22"/>
+      <c r="E46" s="18" t="s">
         <v>143</v>
-      </c>
-      <c r="D46" s="23"/>
-      <c r="E46" s="19" t="s">
-        <v>144</v>
       </c>
       <c r="F46" s="3"/>
       <c r="G46" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H46" s="3"/>
-      <c r="I46" s="12">
+      <c r="I46" s="11">
         <v>0</v>
       </c>
-      <c r="J46" s="12">
+      <c r="J46" s="11">
         <v>10</v>
       </c>
-      <c r="K46" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="L46" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M46" s="12"/>
-      <c r="N46" s="12" t="s">
-        <v>13</v>
+      <c r="K46" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="L46" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M46" s="11"/>
+      <c r="N46" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="O46" s="3"/>
       <c r="P46" s="3"/>
@@ -3841,40 +3818,40 @@
       <c r="S46" s="3"/>
       <c r="T46" s="3"/>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A47" s="14" t="s">
+    <row r="47" spans="1:20">
+      <c r="A47" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D47" s="23"/>
-      <c r="E47" s="19" t="s">
-        <v>144</v>
+      <c r="D47" s="22"/>
+      <c r="E47" s="18" t="s">
+        <v>143</v>
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H47" s="3"/>
-      <c r="I47" s="12">
+      <c r="I47" s="11">
         <v>0</v>
       </c>
-      <c r="J47" s="12">
+      <c r="J47" s="11">
         <v>10</v>
       </c>
-      <c r="K47" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="L47" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M47" s="12"/>
-      <c r="N47" s="12" t="s">
-        <v>13</v>
+      <c r="K47" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="L47" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M47" s="11"/>
+      <c r="N47" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="O47" s="3"/>
       <c r="P47" s="3"/>
@@ -3883,40 +3860,40 @@
       <c r="S47" s="3"/>
       <c r="T47" s="3"/>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A48" s="14" t="s">
+    <row r="48" spans="1:20">
+      <c r="A48" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C48" s="3" t="s">
+      <c r="D48" s="22"/>
+      <c r="E48" s="18" t="s">
         <v>149</v>
-      </c>
-      <c r="D48" s="23"/>
-      <c r="E48" s="19" t="s">
-        <v>150</v>
       </c>
       <c r="F48" s="3"/>
       <c r="G48" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H48" s="3"/>
-      <c r="I48" s="12">
+      <c r="I48" s="11">
         <v>-1</v>
       </c>
-      <c r="J48" s="12">
+      <c r="J48" s="11">
         <v>1</v>
       </c>
-      <c r="K48" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="L48" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M48" s="12"/>
-      <c r="N48" s="12" t="s">
-        <v>13</v>
+      <c r="K48" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="L48" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M48" s="11"/>
+      <c r="N48" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="O48" s="3"/>
       <c r="P48" s="3"/>
@@ -3925,40 +3902,40 @@
       <c r="S48" s="3"/>
       <c r="T48" s="3"/>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A49" s="14" t="s">
+    <row r="49" spans="1:20">
+      <c r="A49" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C49" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="B49" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="D49" s="23"/>
-      <c r="E49" s="19" t="s">
-        <v>150</v>
+      <c r="D49" s="22"/>
+      <c r="E49" s="18" t="s">
+        <v>149</v>
       </c>
       <c r="F49" s="3"/>
       <c r="G49" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H49" s="3"/>
-      <c r="I49" s="12">
+      <c r="I49" s="11">
         <v>-1</v>
       </c>
-      <c r="J49" s="12">
+      <c r="J49" s="11">
         <v>1</v>
       </c>
-      <c r="K49" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="L49" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M49" s="12"/>
-      <c r="N49" s="12" t="s">
-        <v>13</v>
+      <c r="K49" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="L49" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M49" s="11"/>
+      <c r="N49" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="O49" s="3"/>
       <c r="P49" s="3"/>
@@ -3967,40 +3944,40 @@
       <c r="S49" s="3"/>
       <c r="T49" s="3"/>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A50" s="14" t="s">
+    <row r="50" spans="1:20">
+      <c r="A50" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C50" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="B50" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="D50" s="23"/>
-      <c r="E50" s="19" t="s">
-        <v>18</v>
+      <c r="D50" s="22"/>
+      <c r="E50" s="18" t="s">
+        <v>17</v>
       </c>
       <c r="F50" s="3"/>
       <c r="G50" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H50" s="3"/>
-      <c r="I50" s="12">
+      <c r="I50" s="11">
         <v>0</v>
       </c>
-      <c r="J50" s="12">
+      <c r="J50" s="11">
         <v>90</v>
       </c>
-      <c r="K50" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="L50" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M50" s="12"/>
-      <c r="N50" s="12" t="s">
-        <v>13</v>
+      <c r="K50" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="L50" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M50" s="11"/>
+      <c r="N50" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="O50" s="3"/>
       <c r="P50" s="3"/>
@@ -4009,42 +3986,42 @@
       <c r="S50" s="3"/>
       <c r="T50" s="3"/>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A51" s="14" t="s">
+    <row r="51" spans="1:20">
+      <c r="A51" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C51" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="B51" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C51" s="3" t="s">
+      <c r="D51" s="22"/>
+      <c r="E51" s="18" t="s">
         <v>158</v>
-      </c>
-      <c r="D51" s="23"/>
-      <c r="E51" s="19" t="s">
-        <v>159</v>
       </c>
       <c r="F51" s="3"/>
       <c r="G51" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="I51" s="12">
+        <v>47</v>
+      </c>
+      <c r="I51" s="11">
         <v>0</v>
       </c>
-      <c r="J51" s="12">
+      <c r="J51" s="11">
         <v>40000</v>
       </c>
-      <c r="K51" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="L51" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M51" s="12"/>
-      <c r="N51" s="12" t="s">
-        <v>194</v>
+      <c r="K51" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="L51" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M51" s="11"/>
+      <c r="N51" s="11" t="s">
+        <v>193</v>
       </c>
       <c r="O51" s="3"/>
       <c r="P51" s="3"/>
@@ -4052,40 +4029,40 @@
       <c r="R51" s="3"/>
       <c r="S51" s="3"/>
       <c r="T51" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A52" s="15" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20">
+      <c r="A52" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C52" s="34" t="s">
         <v>210</v>
       </c>
-      <c r="B52" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C52" s="35" t="s">
+      <c r="D52" s="22"/>
+      <c r="E52" s="18">
+        <v>1</v>
+      </c>
+      <c r="F52" s="34"/>
+      <c r="G52" s="34"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="34">
+        <v>0</v>
+      </c>
+      <c r="J52" s="35">
+        <v>999</v>
+      </c>
+      <c r="K52" s="35" t="s">
         <v>211</v>
       </c>
-      <c r="D52" s="23"/>
-      <c r="E52" s="19">
-        <v>1</v>
-      </c>
-      <c r="F52" s="35"/>
-      <c r="G52" s="35"/>
-      <c r="H52" s="3"/>
-      <c r="I52" s="35">
-        <v>0</v>
-      </c>
-      <c r="J52" s="36">
-        <v>999</v>
-      </c>
-      <c r="K52" s="36" t="s">
-        <v>212</v>
-      </c>
-      <c r="L52" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M52" s="12"/>
-      <c r="N52" s="12"/>
+      <c r="L52" s="23">
+        <v>99999</v>
+      </c>
+      <c r="M52" s="11"/>
+      <c r="N52" s="11"/>
       <c r="O52" s="3"/>
       <c r="P52" s="3"/>
       <c r="Q52" s="3"/>
@@ -4093,37 +4070,37 @@
       <c r="S52" s="3"/>
       <c r="T52" s="3"/>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A53" s="14" t="s">
+    <row r="53" spans="1:20">
+      <c r="A53" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C53" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="B53" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="D53" s="23"/>
-      <c r="E53" s="19">
+      <c r="D53" s="22"/>
+      <c r="E53" s="18">
         <v>1</v>
       </c>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
-      <c r="I53" s="12">
+      <c r="I53" s="11">
         <v>1</v>
       </c>
-      <c r="J53" s="12">
+      <c r="J53" s="11">
         <v>36</v>
       </c>
-      <c r="K53" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="L53" s="24">
+      <c r="K53" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="L53" s="23">
         <v>99999</v>
       </c>
-      <c r="M53" s="12"/>
-      <c r="N53" s="12"/>
+      <c r="M53" s="11"/>
+      <c r="N53" s="11"/>
       <c r="O53" s="3"/>
       <c r="P53" s="3"/>
       <c r="Q53" s="3"/>
@@ -4131,37 +4108,37 @@
       <c r="S53" s="3"/>
       <c r="T53" s="3"/>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A54" s="14" t="s">
+    <row r="54" spans="1:20">
+      <c r="A54" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C54" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="B54" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="D54" s="23"/>
-      <c r="E54" s="19">
+      <c r="D54" s="22"/>
+      <c r="E54" s="18">
         <v>1</v>
       </c>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
-      <c r="I54" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="J54" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="K54" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="L54" s="24">
+      <c r="I54" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="J54" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="K54" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="L54" s="23">
         <v>99999</v>
       </c>
-      <c r="M54" s="12"/>
-      <c r="N54" s="12"/>
+      <c r="M54" s="11"/>
+      <c r="N54" s="11"/>
       <c r="O54" s="3"/>
       <c r="P54" s="3"/>
       <c r="Q54" s="3"/>
@@ -4169,38 +4146,38 @@
       <c r="S54" s="3"/>
       <c r="T54" s="3"/>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A55" s="14" t="s">
+    <row r="55" spans="1:20">
+      <c r="A55" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C55" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="B55" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D55" s="23"/>
-      <c r="E55" s="19" t="s">
-        <v>159</v>
+      <c r="D55" s="22"/>
+      <c r="E55" s="18" t="s">
+        <v>158</v>
       </c>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
-      <c r="I55" s="12">
+      <c r="I55" s="11">
         <v>0</v>
       </c>
-      <c r="J55" s="12">
+      <c r="J55" s="11">
         <v>11000</v>
       </c>
-      <c r="K55" s="12" t="s">
+      <c r="K55" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="L55" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M55" s="11"/>
+      <c r="N55" s="11" t="s">
         <v>193</v>
-      </c>
-      <c r="L55" s="28">
-        <v>1E+36</v>
-      </c>
-      <c r="M55" s="12"/>
-      <c r="N55" s="12" t="s">
-        <v>194</v>
       </c>
       <c r="O55" s="3"/>
       <c r="P55" s="3"/>

</xml_diff>

<commit_message>
add Density primary and secondary DEN1, DEN2
</commit_message>
<xml_diff>
--- a/roscop/code_roscop.xlsx
+++ b/roscop/code_roscop.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="225">
   <si>
     <t>long_name</t>
   </si>
@@ -82,9 +82,6 @@
     <t>%1d</t>
   </si>
   <si>
-    <t>%6.3lf</t>
-  </si>
-  <si>
     <t>0.001</t>
   </si>
   <si>
@@ -118,9 +115,6 @@
     <t>days since 1950-01-01T00:00:00Z</t>
   </si>
   <si>
-    <t>%7.2lf</t>
-  </si>
-  <si>
     <t>Z</t>
   </si>
   <si>
@@ -175,9 +169,6 @@
     <t>hectoPascal</t>
   </si>
   <si>
-    <t>%6.1lf</t>
-  </si>
-  <si>
     <t>RELH</t>
   </si>
   <si>
@@ -265,9 +256,6 @@
     <t>EWCT</t>
   </si>
   <si>
-    <t>%7.3lf</t>
-  </si>
-  <si>
     <t>0.01</t>
   </si>
   <si>
@@ -280,12 +268,6 @@
     <t>WMSP</t>
   </si>
   <si>
-    <t>%5.1lf</t>
-  </si>
-  <si>
-    <t>%8.3lf</t>
-  </si>
-  <si>
     <t>cm/second</t>
   </si>
   <si>
@@ -301,15 +283,9 @@
     <t>milligram/m3</t>
   </si>
   <si>
-    <t>%8.4lf</t>
-  </si>
-  <si>
     <t>TUR3</t>
   </si>
   <si>
-    <t>%6.2lf</t>
-  </si>
-  <si>
     <t>PRLF</t>
   </si>
   <si>
@@ -725,6 +701,27 @@
   </si>
   <si>
     <t>_FillValue</t>
+  </si>
+  <si>
+    <t>%7.2f</t>
+  </si>
+  <si>
+    <t>%8.4f</t>
+  </si>
+  <si>
+    <t>%6.2f</t>
+  </si>
+  <si>
+    <t>DEN1</t>
+  </si>
+  <si>
+    <t>DEN2</t>
+  </si>
+  <si>
+    <t>density primary sensor</t>
+  </si>
+  <si>
+    <t>density secondary sensor</t>
   </si>
 </sst>
 </file>
@@ -1779,13 +1776,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U55"/>
+  <dimension ref="A1:U57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
@@ -1810,10 +1807,10 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="15" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C1" s="19" t="s">
         <v>0</v>
@@ -1828,10 +1825,10 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>4</v>
@@ -1843,7 +1840,7 @@
         <v>6</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>7</v>
@@ -1855,94 +1852,94 @@
         <v>9</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="T1" s="7" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="U1" s="8"/>
     </row>
     <row r="2" spans="1:21">
       <c r="A2" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U2" s="2"/>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" s="13" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="18">
@@ -1954,7 +1951,7 @@
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
       <c r="K3" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="L3" s="23">
         <v>99999</v>
@@ -1962,7 +1959,7 @@
       <c r="M3" s="11"/>
       <c r="N3" s="11"/>
       <c r="O3" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
@@ -1972,13 +1969,13 @@
     </row>
     <row r="4" spans="1:21">
       <c r="A4" s="13" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D4" s="22"/>
       <c r="E4" s="18">
@@ -1990,7 +1987,7 @@
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
       <c r="K4" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="L4" s="23">
         <v>99999</v>
@@ -1998,7 +1995,7 @@
       <c r="M4" s="11"/>
       <c r="N4" s="11"/>
       <c r="O4" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
@@ -2008,19 +2005,19 @@
     </row>
     <row r="5" spans="1:21">
       <c r="A5" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D5" s="22" t="s">
         <v>166</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>174</v>
-      </c>
       <c r="E5" s="18" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -2030,7 +2027,7 @@
       <c r="K5" s="11"/>
       <c r="L5" s="27"/>
       <c r="M5" s="11" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="N5" s="11"/>
       <c r="O5" s="3"/>
@@ -2038,27 +2035,27 @@
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
       <c r="S5" s="3" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:21">
       <c r="A6" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -2068,7 +2065,7 @@
       <c r="K6" s="11"/>
       <c r="L6" s="27"/>
       <c r="M6" s="11" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="N6" s="11"/>
       <c r="O6" s="3"/>
@@ -2076,30 +2073,30 @@
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
       <c r="S6" s="3" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="15">
       <c r="A7" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F7" s="36" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="24"/>
@@ -2110,11 +2107,11 @@
         <v>90000</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="L7" s="27"/>
       <c r="M7" s="11" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="N7" s="11"/>
       <c r="O7" s="3"/>
@@ -2126,13 +2123,13 @@
     </row>
     <row r="8" spans="1:21">
       <c r="A8" s="13" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="D8" s="22"/>
       <c r="E8" s="18">
@@ -2148,7 +2145,7 @@
         <v>90000</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="L8" s="27"/>
       <c r="M8" s="11"/>
@@ -2162,24 +2159,24 @@
     </row>
     <row r="9" spans="1:21">
       <c r="A9" s="13" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I9" s="11">
         <v>0</v>
@@ -2188,13 +2185,13 @@
         <v>9000</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>23</v>
+        <v>218</v>
       </c>
       <c r="L9" s="27">
         <v>1E+36</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="N9" s="11"/>
       <c r="O9" s="3"/>
@@ -2203,28 +2200,28 @@
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
       <c r="T9" s="3" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:21">
       <c r="A10" s="13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="11">
@@ -2234,7 +2231,7 @@
         <v>9000</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>23</v>
+        <v>218</v>
       </c>
       <c r="L10" s="27">
         <v>1E+36</v>
@@ -2242,7 +2239,7 @@
       <c r="M10" s="11"/>
       <c r="N10" s="11"/>
       <c r="O10" s="3" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
@@ -2252,43 +2249,43 @@
     </row>
     <row r="11" spans="1:21">
       <c r="A11" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J11" s="11">
         <v>38</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>11</v>
+        <v>104</v>
       </c>
       <c r="L11" s="27">
         <v>1E+36</v>
       </c>
       <c r="M11" s="11"/>
       <c r="N11" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
@@ -2298,43 +2295,43 @@
     </row>
     <row r="12" spans="1:21">
       <c r="A12" s="13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E12" s="18">
         <v>1</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J12" s="11">
         <v>38</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>11</v>
+        <v>104</v>
       </c>
       <c r="L12" s="27">
         <v>1E+36</v>
       </c>
       <c r="M12" s="11"/>
       <c r="N12" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
@@ -2344,43 +2341,43 @@
     </row>
     <row r="13" spans="1:21">
       <c r="A13" s="13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J13" s="11">
         <v>38</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>11</v>
+        <v>104</v>
       </c>
       <c r="L13" s="27">
         <v>1E+36</v>
       </c>
       <c r="M13" s="11"/>
       <c r="N13" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
@@ -2390,43 +2387,43 @@
     </row>
     <row r="14" spans="1:21">
       <c r="A14" s="13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J14" s="11">
         <v>38</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>11</v>
+        <v>104</v>
       </c>
       <c r="L14" s="27">
         <v>1E+36</v>
       </c>
       <c r="M14" s="11"/>
       <c r="N14" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
@@ -2436,23 +2433,23 @@
     </row>
     <row r="15" spans="1:21">
       <c r="A15" s="13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="11">
@@ -2462,17 +2459,17 @@
         <v>1600</v>
       </c>
       <c r="K15" s="11" t="s">
-        <v>23</v>
+        <v>218</v>
       </c>
       <c r="L15" s="27">
         <v>1E+36</v>
       </c>
       <c r="M15" s="11"/>
       <c r="N15" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
@@ -2482,43 +2479,43 @@
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J16" s="11">
         <v>38</v>
       </c>
       <c r="K16" s="11" t="s">
-        <v>11</v>
+        <v>104</v>
       </c>
       <c r="L16" s="27">
         <v>1E+36</v>
       </c>
       <c r="M16" s="11"/>
       <c r="N16" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
@@ -2528,23 +2525,23 @@
     </row>
     <row r="17" spans="1:20">
       <c r="A17" s="13" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="11">
@@ -2554,17 +2551,17 @@
         <v>200</v>
       </c>
       <c r="K17" s="11" t="s">
-        <v>11</v>
+        <v>104</v>
       </c>
       <c r="L17" s="27">
         <v>1E+36</v>
       </c>
       <c r="M17" s="11"/>
       <c r="N17" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
@@ -2574,23 +2571,23 @@
     </row>
     <row r="18" spans="1:20">
       <c r="A18" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="18" t="s">
         <v>36</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D18" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>38</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="11">
@@ -2600,17 +2597,17 @@
         <v>360</v>
       </c>
       <c r="K18" s="11" t="s">
-        <v>77</v>
+        <v>147</v>
       </c>
       <c r="L18" s="27">
         <v>1E+36</v>
       </c>
       <c r="M18" s="11"/>
       <c r="N18" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
@@ -2620,23 +2617,23 @@
     </row>
     <row r="19" spans="1:20">
       <c r="A19" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="18" t="s">
         <v>39</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D19" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>41</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="11">
@@ -2646,17 +2643,17 @@
         <v>1030</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>78</v>
+        <v>189</v>
       </c>
       <c r="L19" s="27">
         <v>1E+36</v>
       </c>
       <c r="M19" s="11"/>
       <c r="N19" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
@@ -2666,23 +2663,23 @@
     </row>
     <row r="20" spans="1:20">
       <c r="A20" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" s="18" t="s">
         <v>43</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D20" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>46</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="11">
@@ -2692,17 +2689,17 @@
         <v>100</v>
       </c>
       <c r="K20" s="11" t="s">
-        <v>42</v>
+        <v>184</v>
       </c>
       <c r="L20" s="27">
         <v>1E+36</v>
       </c>
       <c r="M20" s="11"/>
       <c r="N20" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
@@ -2712,21 +2709,21 @@
     </row>
     <row r="21" spans="1:20">
       <c r="A21" s="13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D21" s="22"/>
       <c r="E21" s="18" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="11">
@@ -2736,17 +2733,17 @@
         <v>100</v>
       </c>
       <c r="K21" s="11" t="s">
-        <v>72</v>
+        <v>131</v>
       </c>
       <c r="L21" s="27">
         <v>1E+36</v>
       </c>
       <c r="M21" s="11"/>
       <c r="N21" s="11" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="O21" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
@@ -2756,21 +2753,21 @@
     </row>
     <row r="22" spans="1:20">
       <c r="A22" s="13" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D22" s="22"/>
       <c r="E22" s="18" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="11">
@@ -2780,17 +2777,17 @@
         <v>100</v>
       </c>
       <c r="K22" s="11" t="s">
-        <v>72</v>
+        <v>131</v>
       </c>
       <c r="L22" s="27">
         <v>1E+36</v>
       </c>
       <c r="M22" s="11"/>
       <c r="N22" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="P22" s="3"/>
       <c r="Q22" s="3"/>
@@ -2800,43 +2797,43 @@
     </row>
     <row r="23" spans="1:20">
       <c r="A23" s="13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J23" s="11">
         <v>38</v>
       </c>
       <c r="K23" s="11" t="s">
-        <v>11</v>
+        <v>104</v>
       </c>
       <c r="L23" s="27">
         <v>1E+36</v>
       </c>
       <c r="M23" s="11"/>
       <c r="N23" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O23" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
@@ -2846,43 +2843,43 @@
     </row>
     <row r="24" spans="1:20">
       <c r="A24" s="13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J24" s="11">
         <v>38</v>
       </c>
       <c r="K24" s="11" t="s">
-        <v>11</v>
+        <v>104</v>
       </c>
       <c r="L24" s="27">
         <v>1E+36</v>
       </c>
       <c r="M24" s="11"/>
       <c r="N24" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O24" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
@@ -2892,43 +2889,43 @@
     </row>
     <row r="25" spans="1:20">
       <c r="A25" s="13" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H25" s="3"/>
       <c r="I25" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J25" s="11">
         <v>38</v>
       </c>
       <c r="K25" s="11" t="s">
-        <v>11</v>
+        <v>104</v>
       </c>
       <c r="L25" s="27">
         <v>1E+36</v>
       </c>
       <c r="M25" s="11"/>
       <c r="N25" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O25" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
@@ -2938,21 +2935,21 @@
     </row>
     <row r="26" spans="1:20">
       <c r="A26" s="13" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D26" s="22"/>
       <c r="E26" s="18" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H26" s="3"/>
       <c r="I26" s="11">
@@ -2962,14 +2959,14 @@
         <v>700</v>
       </c>
       <c r="K26" s="11" t="s">
-        <v>72</v>
+        <v>131</v>
       </c>
       <c r="L26" s="27">
         <v>1E+36</v>
       </c>
       <c r="M26" s="11"/>
       <c r="N26" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
@@ -2980,21 +2977,21 @@
     </row>
     <row r="27" spans="1:20">
       <c r="A27" s="13" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D27" s="22"/>
       <c r="E27" s="18" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H27" s="3"/>
       <c r="I27" s="11">
@@ -3004,14 +3001,14 @@
         <v>1</v>
       </c>
       <c r="K27" s="11" t="s">
-        <v>84</v>
+        <v>219</v>
       </c>
       <c r="L27" s="27">
         <v>1E+36</v>
       </c>
       <c r="M27" s="11"/>
       <c r="N27" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
@@ -3022,21 +3019,21 @@
     </row>
     <row r="28" spans="1:20">
       <c r="A28" s="25" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="29" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H28" s="3"/>
       <c r="I28" s="30">
@@ -3046,14 +3043,14 @@
         <v>10</v>
       </c>
       <c r="K28" s="30" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="L28" s="27">
         <v>1E+36</v>
       </c>
       <c r="M28" s="11"/>
       <c r="N28" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O28" s="3"/>
       <c r="P28" s="3"/>
@@ -3064,21 +3061,21 @@
     </row>
     <row r="29" spans="1:20">
       <c r="A29" s="13" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D29" s="22"/>
       <c r="E29" s="18" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H29" s="3"/>
       <c r="I29" s="11">
@@ -3088,14 +3085,14 @@
         <v>100</v>
       </c>
       <c r="K29" s="11" t="s">
-        <v>86</v>
+        <v>220</v>
       </c>
       <c r="L29" s="27">
         <v>1E+36</v>
       </c>
       <c r="M29" s="11"/>
       <c r="N29" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
@@ -3106,21 +3103,21 @@
     </row>
     <row r="30" spans="1:20">
       <c r="A30" s="25" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="18" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H30" s="3"/>
       <c r="I30" s="30">
@@ -3130,14 +3127,14 @@
         <v>3000</v>
       </c>
       <c r="K30" s="30" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="L30" s="27">
         <v>1E+36</v>
       </c>
       <c r="M30" s="11"/>
       <c r="N30" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O30" s="3"/>
       <c r="P30" s="3"/>
@@ -3148,21 +3145,21 @@
     </row>
     <row r="31" spans="1:20">
       <c r="A31" s="25" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="18" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H31" s="3"/>
       <c r="I31" s="30">
@@ -3172,14 +3169,14 @@
         <v>4000</v>
       </c>
       <c r="K31" s="30" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="L31" s="27">
         <v>1E+36</v>
       </c>
       <c r="M31" s="11"/>
       <c r="N31" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O31" s="3"/>
       <c r="P31" s="3"/>
@@ -3190,21 +3187,21 @@
     </row>
     <row r="32" spans="1:20" ht="12.6" customHeight="1">
       <c r="A32" s="25" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="D32" s="22"/>
       <c r="E32" s="18" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H32" s="3"/>
       <c r="I32" s="30">
@@ -3214,14 +3211,14 @@
         <v>3000</v>
       </c>
       <c r="K32" s="30" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="L32" s="27">
         <v>1E+36</v>
       </c>
       <c r="M32" s="11"/>
       <c r="N32" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O32" s="3"/>
       <c r="P32" s="3"/>
@@ -3232,21 +3229,21 @@
     </row>
     <row r="33" spans="1:20" ht="12.6" customHeight="1">
       <c r="A33" s="26" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="D33" s="22"/>
       <c r="E33" s="32" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="31">
@@ -3256,14 +3253,14 @@
         <v>999999</v>
       </c>
       <c r="K33" s="33" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="L33" s="27">
         <v>1E+36</v>
       </c>
       <c r="M33" s="11"/>
       <c r="N33" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
@@ -3274,38 +3271,38 @@
     </row>
     <row r="34" spans="1:20">
       <c r="A34" s="13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D34" s="22"/>
       <c r="E34" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H34" s="3"/>
       <c r="I34" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J34" s="11">
         <v>38</v>
       </c>
       <c r="K34" s="11" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="L34" s="27">
         <v>1E+36</v>
       </c>
       <c r="M34" s="11"/>
       <c r="N34" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O34" s="3"/>
       <c r="P34" s="3"/>
@@ -3316,13 +3313,13 @@
     </row>
     <row r="35" spans="1:20">
       <c r="A35" s="13" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D35" s="22"/>
       <c r="E35" s="18">
@@ -3330,24 +3327,24 @@
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H35" s="3"/>
       <c r="I35" s="11" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="J35" s="11" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="K35" s="11" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="L35" s="27">
         <v>1E+36</v>
       </c>
       <c r="M35" s="11"/>
       <c r="N35" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O35" s="3"/>
       <c r="P35" s="3"/>
@@ -3358,21 +3355,21 @@
     </row>
     <row r="36" spans="1:20">
       <c r="A36" s="13" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D36" s="22"/>
       <c r="E36" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H36" s="3"/>
       <c r="I36" s="11">
@@ -3382,14 +3379,14 @@
         <v>32</v>
       </c>
       <c r="K36" s="11" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="L36" s="27">
         <v>1E+36</v>
       </c>
       <c r="M36" s="11"/>
       <c r="N36" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O36" s="3"/>
       <c r="P36" s="3"/>
@@ -3400,21 +3397,21 @@
     </row>
     <row r="37" spans="1:20">
       <c r="A37" s="13" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D37" s="22"/>
       <c r="E37" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F37" s="3"/>
       <c r="G37" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H37" s="3"/>
       <c r="I37" s="11">
@@ -3424,14 +3421,14 @@
         <v>32</v>
       </c>
       <c r="K37" s="11" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="L37" s="27">
         <v>1E+36</v>
       </c>
       <c r="M37" s="11"/>
       <c r="N37" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O37" s="3"/>
       <c r="P37" s="3"/>
@@ -3442,21 +3439,21 @@
     </row>
     <row r="38" spans="1:20">
       <c r="A38" s="13" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D38" s="22"/>
       <c r="E38" s="18" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H38" s="3"/>
       <c r="I38" s="11">
@@ -3466,14 +3463,14 @@
         <v>37</v>
       </c>
       <c r="K38" s="11" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="L38" s="27">
         <v>1E+36</v>
       </c>
       <c r="M38" s="11"/>
       <c r="N38" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O38" s="3"/>
       <c r="P38" s="3"/>
@@ -3484,21 +3481,21 @@
     </row>
     <row r="39" spans="1:20">
       <c r="A39" s="13" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="D39" s="22"/>
       <c r="E39" s="18" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H39" s="3"/>
       <c r="I39" s="11">
@@ -3508,14 +3505,14 @@
         <v>37</v>
       </c>
       <c r="K39" s="11" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="L39" s="27">
         <v>1E+36</v>
       </c>
       <c r="M39" s="11"/>
       <c r="N39" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O39" s="3"/>
       <c r="P39" s="3"/>
@@ -3526,21 +3523,21 @@
     </row>
     <row r="40" spans="1:20">
       <c r="A40" s="13" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="D40" s="22"/>
       <c r="E40" s="18" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="F40" s="3"/>
       <c r="G40" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H40" s="3"/>
       <c r="I40" s="11">
@@ -3550,14 +3547,14 @@
         <v>7</v>
       </c>
       <c r="K40" s="11" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="L40" s="27">
         <v>1E+36</v>
       </c>
       <c r="M40" s="11"/>
       <c r="N40" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O40" s="3"/>
       <c r="P40" s="3"/>
@@ -3568,21 +3565,21 @@
     </row>
     <row r="41" spans="1:20">
       <c r="A41" s="13" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="D41" s="22"/>
       <c r="E41" s="18" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H41" s="3"/>
       <c r="I41" s="11">
@@ -3592,14 +3589,14 @@
         <v>7</v>
       </c>
       <c r="K41" s="11" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="L41" s="27">
         <v>1E+36</v>
       </c>
       <c r="M41" s="11"/>
       <c r="N41" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O41" s="3"/>
       <c r="P41" s="3"/>
@@ -3610,40 +3607,44 @@
     </row>
     <row r="42" spans="1:20">
       <c r="A42" s="13" t="s">
-        <v>132</v>
+        <v>221</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="D42" s="22"/>
+        <v>223</v>
+      </c>
+      <c r="D42" s="22" t="s">
+        <v>60</v>
+      </c>
       <c r="E42" s="18" t="s">
-        <v>134</v>
+        <v>61</v>
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H42" s="3"/>
-      <c r="I42" s="11">
-        <v>0</v>
+      <c r="I42" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="J42" s="11">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="K42" s="11" t="s">
-        <v>135</v>
+        <v>104</v>
       </c>
       <c r="L42" s="27">
         <v>1E+36</v>
       </c>
       <c r="M42" s="11"/>
       <c r="N42" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="O42" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="O42" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="P42" s="3"/>
       <c r="Q42" s="3"/>
       <c r="R42" s="3"/>
@@ -3652,40 +3653,44 @@
     </row>
     <row r="43" spans="1:20">
       <c r="A43" s="13" t="s">
-        <v>136</v>
+        <v>222</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="D43" s="22"/>
+        <v>224</v>
+      </c>
+      <c r="D43" s="22" t="s">
+        <v>60</v>
+      </c>
       <c r="E43" s="18" t="s">
-        <v>134</v>
+        <v>61</v>
       </c>
       <c r="F43" s="3"/>
       <c r="G43" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H43" s="3"/>
-      <c r="I43" s="11">
-        <v>0</v>
+      <c r="I43" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="J43" s="11">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="K43" s="11" t="s">
-        <v>135</v>
+        <v>104</v>
       </c>
       <c r="L43" s="27">
         <v>1E+36</v>
       </c>
       <c r="M43" s="11"/>
       <c r="N43" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="O43" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="O43" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="P43" s="3"/>
       <c r="Q43" s="3"/>
       <c r="R43" s="3"/>
@@ -3694,38 +3699,38 @@
     </row>
     <row r="44" spans="1:20">
       <c r="A44" s="13" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="D44" s="22"/>
       <c r="E44" s="18" t="s">
-        <v>60</v>
+        <v>126</v>
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H44" s="3"/>
       <c r="I44" s="11">
         <v>0</v>
       </c>
       <c r="J44" s="11">
-        <v>450</v>
+        <v>10</v>
       </c>
       <c r="K44" s="11" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="L44" s="27">
         <v>1E+36</v>
       </c>
       <c r="M44" s="11"/>
       <c r="N44" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O44" s="3"/>
       <c r="P44" s="3"/>
@@ -3736,38 +3741,38 @@
     </row>
     <row r="45" spans="1:20">
       <c r="A45" s="13" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="D45" s="22"/>
       <c r="E45" s="18" t="s">
-        <v>60</v>
+        <v>126</v>
       </c>
       <c r="F45" s="3"/>
       <c r="G45" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H45" s="3"/>
       <c r="I45" s="11">
         <v>0</v>
       </c>
       <c r="J45" s="11">
-        <v>450</v>
+        <v>10</v>
       </c>
       <c r="K45" s="11" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="L45" s="27">
         <v>1E+36</v>
       </c>
       <c r="M45" s="11"/>
       <c r="N45" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O45" s="3"/>
       <c r="P45" s="3"/>
@@ -3778,38 +3783,38 @@
     </row>
     <row r="46" spans="1:20">
       <c r="A46" s="13" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="D46" s="22"/>
       <c r="E46" s="18" t="s">
-        <v>143</v>
+        <v>57</v>
       </c>
       <c r="F46" s="3"/>
       <c r="G46" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H46" s="3"/>
       <c r="I46" s="11">
         <v>0</v>
       </c>
       <c r="J46" s="11">
-        <v>10</v>
+        <v>450</v>
       </c>
       <c r="K46" s="11" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="L46" s="27">
         <v>1E+36</v>
       </c>
       <c r="M46" s="11"/>
       <c r="N46" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O46" s="3"/>
       <c r="P46" s="3"/>
@@ -3820,38 +3825,38 @@
     </row>
     <row r="47" spans="1:20">
       <c r="A47" s="13" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="D47" s="22"/>
       <c r="E47" s="18" t="s">
-        <v>143</v>
+        <v>57</v>
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H47" s="3"/>
       <c r="I47" s="11">
         <v>0</v>
       </c>
       <c r="J47" s="11">
-        <v>10</v>
+        <v>450</v>
       </c>
       <c r="K47" s="11" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="L47" s="27">
         <v>1E+36</v>
       </c>
       <c r="M47" s="11"/>
       <c r="N47" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O47" s="3"/>
       <c r="P47" s="3"/>
@@ -3862,38 +3867,38 @@
     </row>
     <row r="48" spans="1:20">
       <c r="A48" s="13" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="D48" s="22"/>
       <c r="E48" s="18" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="F48" s="3"/>
       <c r="G48" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H48" s="3"/>
       <c r="I48" s="11">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J48" s="11">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K48" s="11" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="L48" s="27">
         <v>1E+36</v>
       </c>
       <c r="M48" s="11"/>
       <c r="N48" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O48" s="3"/>
       <c r="P48" s="3"/>
@@ -3904,38 +3909,38 @@
     </row>
     <row r="49" spans="1:20">
       <c r="A49" s="13" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="D49" s="22"/>
       <c r="E49" s="18" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="F49" s="3"/>
       <c r="G49" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H49" s="3"/>
       <c r="I49" s="11">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J49" s="11">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K49" s="11" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="L49" s="27">
         <v>1E+36</v>
       </c>
       <c r="M49" s="11"/>
       <c r="N49" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O49" s="3"/>
       <c r="P49" s="3"/>
@@ -3946,38 +3951,38 @@
     </row>
     <row r="50" spans="1:20">
       <c r="A50" s="13" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="D50" s="22"/>
       <c r="E50" s="18" t="s">
-        <v>17</v>
+        <v>141</v>
       </c>
       <c r="F50" s="3"/>
       <c r="G50" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H50" s="3"/>
       <c r="I50" s="11">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J50" s="11">
-        <v>90</v>
+        <v>1</v>
       </c>
       <c r="K50" s="11" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="L50" s="27">
         <v>1E+36</v>
       </c>
       <c r="M50" s="11"/>
       <c r="N50" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O50" s="3"/>
       <c r="P50" s="3"/>
@@ -3988,81 +3993,81 @@
     </row>
     <row r="51" spans="1:20">
       <c r="A51" s="13" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="D51" s="22"/>
       <c r="E51" s="18" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="F51" s="3"/>
       <c r="G51" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="H51" s="3" t="s">
-        <v>47</v>
-      </c>
+        <v>210</v>
+      </c>
+      <c r="H51" s="3"/>
       <c r="I51" s="11">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J51" s="11">
-        <v>40000</v>
+        <v>1</v>
       </c>
       <c r="K51" s="11" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="L51" s="27">
         <v>1E+36</v>
       </c>
       <c r="M51" s="11"/>
       <c r="N51" s="11" t="s">
-        <v>193</v>
+        <v>11</v>
       </c>
       <c r="O51" s="3"/>
       <c r="P51" s="3"/>
       <c r="Q51" s="3"/>
       <c r="R51" s="3"/>
       <c r="S51" s="3"/>
-      <c r="T51" s="3" t="s">
-        <v>188</v>
-      </c>
+      <c r="T51" s="3"/>
     </row>
     <row r="52" spans="1:20">
-      <c r="A52" s="14" t="s">
-        <v>209</v>
+      <c r="A52" s="13" t="s">
+        <v>145</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C52" s="34" t="s">
-        <v>210</v>
+        <v>158</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>146</v>
       </c>
       <c r="D52" s="22"/>
-      <c r="E52" s="18">
-        <v>1</v>
-      </c>
-      <c r="F52" s="34"/>
-      <c r="G52" s="34"/>
+      <c r="E52" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3" t="s">
+        <v>210</v>
+      </c>
       <c r="H52" s="3"/>
-      <c r="I52" s="34">
+      <c r="I52" s="11">
         <v>0</v>
       </c>
-      <c r="J52" s="35">
-        <v>999</v>
-      </c>
-      <c r="K52" s="35" t="s">
-        <v>211</v>
-      </c>
-      <c r="L52" s="23">
-        <v>99999</v>
+      <c r="J52" s="11">
+        <v>90</v>
+      </c>
+      <c r="K52" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="L52" s="27">
+        <v>1E+36</v>
       </c>
       <c r="M52" s="11"/>
-      <c r="N52" s="11"/>
+      <c r="N52" s="11" t="s">
+        <v>11</v>
+      </c>
       <c r="O52" s="3"/>
       <c r="P52" s="3"/>
       <c r="Q52" s="3"/>
@@ -4072,67 +4077,75 @@
     </row>
     <row r="53" spans="1:20">
       <c r="A53" s="13" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>108</v>
+        <v>158</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="D53" s="22"/>
-      <c r="E53" s="18">
-        <v>1</v>
+      <c r="E53" s="18" t="s">
+        <v>150</v>
       </c>
       <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
+      <c r="G53" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="I53" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J53" s="11">
-        <v>36</v>
+        <v>40000</v>
       </c>
       <c r="K53" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="L53" s="23">
-        <v>99999</v>
+        <v>151</v>
+      </c>
+      <c r="L53" s="27">
+        <v>1E+36</v>
       </c>
       <c r="M53" s="11"/>
-      <c r="N53" s="11"/>
+      <c r="N53" s="11" t="s">
+        <v>185</v>
+      </c>
       <c r="O53" s="3"/>
       <c r="P53" s="3"/>
       <c r="Q53" s="3"/>
       <c r="R53" s="3"/>
       <c r="S53" s="3"/>
-      <c r="T53" s="3"/>
+      <c r="T53" s="3" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="54" spans="1:20">
-      <c r="A54" s="13" t="s">
-        <v>163</v>
+      <c r="A54" s="14" t="s">
+        <v>201</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>164</v>
+        <v>100</v>
+      </c>
+      <c r="C54" s="34" t="s">
+        <v>202</v>
       </c>
       <c r="D54" s="22"/>
       <c r="E54" s="18">
         <v>1</v>
       </c>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
+      <c r="F54" s="34"/>
+      <c r="G54" s="34"/>
       <c r="H54" s="3"/>
-      <c r="I54" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="J54" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="K54" s="11" t="s">
-        <v>10</v>
+      <c r="I54" s="34">
+        <v>0</v>
+      </c>
+      <c r="J54" s="35">
+        <v>999</v>
+      </c>
+      <c r="K54" s="35" t="s">
+        <v>203</v>
       </c>
       <c r="L54" s="23">
         <v>99999</v>
@@ -4148,43 +4161,119 @@
     </row>
     <row r="55" spans="1:20">
       <c r="A55" s="13" t="s">
-        <v>190</v>
+        <v>152</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>166</v>
+        <v>100</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>191</v>
+        <v>153</v>
       </c>
       <c r="D55" s="22"/>
-      <c r="E55" s="18" t="s">
-        <v>158</v>
+      <c r="E55" s="18">
+        <v>1</v>
       </c>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
       <c r="I55" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J55" s="11">
-        <v>11000</v>
+        <v>36</v>
       </c>
       <c r="K55" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="L55" s="27">
-        <v>1E+36</v>
+        <v>154</v>
+      </c>
+      <c r="L55" s="23">
+        <v>99999</v>
       </c>
       <c r="M55" s="11"/>
-      <c r="N55" s="11" t="s">
-        <v>193</v>
-      </c>
+      <c r="N55" s="11"/>
       <c r="O55" s="3"/>
       <c r="P55" s="3"/>
       <c r="Q55" s="3"/>
       <c r="R55" s="3"/>
       <c r="S55" s="3"/>
       <c r="T55" s="3"/>
+    </row>
+    <row r="56" spans="1:20">
+      <c r="A56" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D56" s="22"/>
+      <c r="E56" s="18">
+        <v>1</v>
+      </c>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="J56" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="K56" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="L56" s="23">
+        <v>99999</v>
+      </c>
+      <c r="M56" s="11"/>
+      <c r="N56" s="11"/>
+      <c r="O56" s="3"/>
+      <c r="P56" s="3"/>
+      <c r="Q56" s="3"/>
+      <c r="R56" s="3"/>
+      <c r="S56" s="3"/>
+      <c r="T56" s="3"/>
+    </row>
+    <row r="57" spans="1:20">
+      <c r="A57" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D57" s="22"/>
+      <c r="E57" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
+      <c r="H57" s="3"/>
+      <c r="I57" s="11">
+        <v>0</v>
+      </c>
+      <c r="J57" s="11">
+        <v>11000</v>
+      </c>
+      <c r="K57" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="L57" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M57" s="11"/>
+      <c r="N57" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="O57" s="3"/>
+      <c r="P57" s="3"/>
+      <c r="Q57" s="3"/>
+      <c r="R57" s="3"/>
+      <c r="S57" s="3"/>
+      <c r="T57" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
change configuration ini files for toml
</commit_message>
<xml_diff>
--- a/roscop/code_roscop.xlsx
+++ b/roscop/code_roscop.xlsx
@@ -10,7 +10,7 @@
     <sheet name="code_roscop" sheetId="5" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="tsg_ncvar_1" localSheetId="0">code_roscop!$A$1:$P$9</definedName>
+    <definedName name="tsg_ncvar_1" localSheetId="0">code_roscop!$A$1:$O$9</definedName>
   </definedNames>
   <calcPr calcId="125725" refMode="R1C1"/>
 </workbook>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="223">
   <si>
     <t>long_name</t>
   </si>
@@ -493,9 +493,6 @@
     <t>%5.1f</t>
   </si>
   <si>
-    <t>HEIG</t>
-  </si>
-  <si>
     <t>atmospheric height</t>
   </si>
   <si>
@@ -676,12 +673,6 @@
     <t>moles_of_oxygen_per_unit_mass_in_sea_water</t>
   </si>
   <si>
-    <t>coordinates</t>
-  </si>
-  <si>
-    <t>TIME DEPTH LATITUDE LONGITUDE</t>
-  </si>
-  <si>
     <t>decibar</t>
   </si>
   <si>
@@ -722,6 +713,9 @@
   </si>
   <si>
     <t>density secondary sensor</t>
+  </si>
+  <si>
+    <t>HEIGHT</t>
   </si>
 </sst>
 </file>
@@ -1776,13 +1770,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U57"/>
+  <dimension ref="A1:T57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B43" sqref="B43"/>
+      <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
@@ -1793,19 +1787,18 @@
     <col min="4" max="4" width="28.88671875" style="21" customWidth="1"/>
     <col min="5" max="5" width="24.109375" style="17" customWidth="1"/>
     <col min="6" max="6" width="15.5546875" customWidth="1"/>
-    <col min="7" max="7" width="32.88671875" customWidth="1"/>
-    <col min="8" max="8" width="6.109375" customWidth="1"/>
-    <col min="9" max="9" width="7.5546875" style="6" customWidth="1"/>
-    <col min="10" max="10" width="8.109375" style="6" customWidth="1"/>
-    <col min="11" max="11" width="7.44140625" style="6" customWidth="1"/>
-    <col min="12" max="12" width="7.88671875" style="10" customWidth="1"/>
-    <col min="13" max="13" width="5.6640625" style="6" customWidth="1"/>
-    <col min="14" max="14" width="8.5546875" style="6" customWidth="1"/>
-    <col min="15" max="15" width="34.109375" customWidth="1"/>
-    <col min="16" max="16" width="11.44140625" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" customWidth="1"/>
+    <col min="8" max="8" width="7.5546875" style="6" customWidth="1"/>
+    <col min="9" max="9" width="8.109375" style="6" customWidth="1"/>
+    <col min="10" max="10" width="7.44140625" style="6" customWidth="1"/>
+    <col min="11" max="11" width="7.88671875" style="10" customWidth="1"/>
+    <col min="12" max="12" width="5.6640625" style="6" customWidth="1"/>
+    <col min="13" max="13" width="8.5546875" style="6" customWidth="1"/>
+    <col min="14" max="14" width="34.109375" customWidth="1"/>
+    <col min="15" max="15" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:20">
       <c r="A1" s="15" t="s">
         <v>80</v>
       </c>
@@ -1825,50 +1818,47 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="H1" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="H1" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="I1" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="9" t="s">
-        <v>217</v>
+      <c r="K1" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="N1" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="O1" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="S1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="S1" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="T1" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="U1" s="8"/>
-    </row>
-    <row r="2" spans="1:21">
+      <c r="T1" s="8"/>
+    </row>
+    <row r="2" spans="1:20">
       <c r="A2" s="12" t="s">
         <v>13</v>
       </c>
@@ -1890,32 +1880,32 @@
       <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>216</v>
-      </c>
       <c r="K2" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="5" t="s">
-        <v>216</v>
-      </c>
       <c r="M2" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>216</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>13</v>
@@ -1926,12 +1916,9 @@
       <c r="S2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="T2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="U2" s="2"/>
-    </row>
-    <row r="3" spans="1:21">
+      <c r="T2" s="2"/>
+    </row>
+    <row r="3" spans="1:20">
       <c r="A3" s="13" t="s">
         <v>79</v>
       </c>
@@ -1947,27 +1934,26 @@
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="H3" s="11"/>
       <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11" t="s">
+      <c r="J3" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="L3" s="23">
+      <c r="K3" s="23">
         <v>99999</v>
       </c>
+      <c r="L3" s="11"/>
       <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>49</v>
       </c>
+      <c r="O3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-    </row>
-    <row r="4" spans="1:21">
+    </row>
+    <row r="4" spans="1:20">
       <c r="A4" s="13" t="s">
         <v>101</v>
       </c>
@@ -1983,873 +1969,829 @@
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+      <c r="H4" s="11"/>
       <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11" t="s">
+      <c r="J4" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="L4" s="23">
+      <c r="K4" s="23">
         <v>99999</v>
       </c>
+      <c r="L4" s="11"/>
       <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>49</v>
       </c>
+      <c r="O4" s="3"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
       <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-    </row>
-    <row r="5" spans="1:21">
+    </row>
+    <row r="5" spans="1:20">
       <c r="A5" s="13" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+      <c r="H5" s="11"/>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="27"/>
-      <c r="M5" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="N5" s="11"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="M5" s="11"/>
+      <c r="N5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
+      <c r="R5" s="3" t="s">
+        <v>174</v>
+      </c>
       <c r="S5" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="T5" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21">
+    </row>
+    <row r="6" spans="1:20">
       <c r="A6" s="13" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D6" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="E6" s="18" t="s">
         <v>167</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>168</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="N6" s="11"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="M6" s="11"/>
+      <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
+      <c r="R6" s="3" t="s">
+        <v>174</v>
+      </c>
       <c r="S6" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="T6" s="3" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="15">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="15">
       <c r="A7" s="13" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D7" s="22" t="s">
         <v>164</v>
-      </c>
-      <c r="D7" s="22" t="s">
-        <v>165</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>21</v>
       </c>
       <c r="F7" s="36" t="s">
-        <v>215</v>
-      </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="24"/>
+        <v>212</v>
+      </c>
+      <c r="G7" s="24"/>
+      <c r="H7" s="11">
+        <v>0</v>
+      </c>
       <c r="I7" s="11">
-        <v>0</v>
-      </c>
-      <c r="J7" s="11">
         <v>90000</v>
       </c>
-      <c r="K7" s="11" t="s">
+      <c r="J7" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="K7" s="27"/>
+      <c r="L7" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="L7" s="27"/>
-      <c r="M7" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="N7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
       <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-    </row>
-    <row r="8" spans="1:21">
+    </row>
+    <row r="8" spans="1:20">
       <c r="A8" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>161</v>
       </c>
       <c r="D8" s="22"/>
       <c r="E8" s="18">
         <v>1</v>
       </c>
       <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="11">
+        <v>0</v>
+      </c>
       <c r="I8" s="11">
-        <v>0</v>
-      </c>
-      <c r="J8" s="11">
         <v>90000</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="J8" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="L8" s="27"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="11"/>
       <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
+      <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
       <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-    </row>
-    <row r="9" spans="1:21">
+    </row>
+    <row r="9" spans="1:20">
       <c r="A9" s="13" t="s">
         <v>103</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>47</v>
       </c>
+      <c r="H9" s="11">
+        <v>0</v>
+      </c>
       <c r="I9" s="11">
-        <v>0</v>
-      </c>
-      <c r="J9" s="11">
         <v>9000</v>
       </c>
-      <c r="K9" s="11" t="s">
-        <v>218</v>
-      </c>
-      <c r="L9" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M9" s="11" t="s">
+      <c r="J9" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="K9" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L9" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="N9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="3"/>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21">
+      <c r="S9" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
       <c r="A10" s="13" t="s">
         <v>45</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>46</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F10" s="3"/>
-      <c r="G10" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="11">
+        <v>0</v>
+      </c>
       <c r="I10" s="11">
-        <v>0</v>
-      </c>
-      <c r="J10" s="11">
         <v>9000</v>
       </c>
-      <c r="K10" s="11" t="s">
-        <v>218</v>
-      </c>
-      <c r="L10" s="27">
-        <v>1E+36</v>
+      <c r="J10" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="K10" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="3" t="s">
-        <v>212</v>
-      </c>
+      <c r="N10" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="O10" s="3"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
       <c r="S10" s="3"/>
-      <c r="T10" s="3"/>
-    </row>
-    <row r="11" spans="1:21">
+    </row>
+    <row r="11" spans="1:20">
       <c r="A11" s="13" t="s">
-        <v>52</v>
+        <v>222</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D11" s="22" t="s">
-        <v>23</v>
-      </c>
+        <v>148</v>
+      </c>
+      <c r="D11" s="22"/>
       <c r="E11" s="18" t="s">
-        <v>16</v>
+        <v>149</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H11" s="3"/>
-      <c r="I11" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="J11" s="11">
-        <v>38</v>
-      </c>
-      <c r="K11" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="L11" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="O11" s="3" t="s">
-        <v>213</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="H11" s="11">
+        <v>0</v>
+      </c>
+      <c r="I11" s="11">
+        <v>40000</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="K11" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L11" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="M11" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
       <c r="R11" s="3"/>
-      <c r="S11" s="3"/>
-      <c r="T11" s="3"/>
-    </row>
-    <row r="12" spans="1:21">
+      <c r="S11" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20">
       <c r="A12" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" s="18">
-        <v>1</v>
+        <v>23</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>16</v>
       </c>
       <c r="F12" s="3"/>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="3"/>
+      <c r="H12" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="11">
+        <v>38</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="K12" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="N12" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="J12" s="11">
-        <v>38</v>
-      </c>
-      <c r="K12" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="L12" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="O12" s="3" t="s">
-        <v>214</v>
-      </c>
+      <c r="O12" s="3"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
       <c r="R12" s="3"/>
       <c r="S12" s="3"/>
-      <c r="T12" s="3"/>
-    </row>
-    <row r="13" spans="1:21">
+    </row>
+    <row r="13" spans="1:20">
       <c r="A13" s="13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>57</v>
+        <v>54</v>
+      </c>
+      <c r="E13" s="18">
+        <v>1</v>
       </c>
       <c r="F13" s="3"/>
-      <c r="G13" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H13" s="3"/>
-      <c r="I13" s="11" t="s">
+      <c r="G13" s="3"/>
+      <c r="H13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="J13" s="11">
+      <c r="I13" s="11">
         <v>38</v>
       </c>
-      <c r="K13" s="11" t="s">
+      <c r="J13" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="L13" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11" t="s">
+      <c r="K13" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="O13" s="3" t="s">
-        <v>58</v>
-      </c>
+      <c r="N13" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="O13" s="3"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
       <c r="S13" s="3"/>
-      <c r="T13" s="3"/>
-    </row>
-    <row r="14" spans="1:21">
+    </row>
+    <row r="14" spans="1:20">
       <c r="A14" s="13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>60</v>
+        <v>207</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F14" s="3"/>
-      <c r="G14" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H14" s="3"/>
-      <c r="I14" s="11" t="s">
+      <c r="G14" s="3"/>
+      <c r="H14" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="J14" s="11">
+      <c r="I14" s="11">
         <v>38</v>
       </c>
-      <c r="K14" s="11" t="s">
+      <c r="J14" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="L14" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M14" s="11"/>
-      <c r="N14" s="11" t="s">
+      <c r="K14" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="O14" s="3" t="s">
-        <v>62</v>
-      </c>
+      <c r="N14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O14" s="3"/>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
       <c r="R14" s="3"/>
       <c r="S14" s="3"/>
-      <c r="T14" s="3"/>
-    </row>
-    <row r="15" spans="1:21">
+    </row>
+    <row r="15" spans="1:20">
       <c r="A15" s="13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>207</v>
+        <v>60</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="F15" s="3"/>
-      <c r="G15" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="I15" s="11">
-        <v>1350</v>
-      </c>
-      <c r="J15" s="11">
-        <v>1600</v>
-      </c>
-      <c r="K15" s="11" t="s">
-        <v>218</v>
-      </c>
-      <c r="L15" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="K15" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="O15" s="3" t="s">
-        <v>66</v>
-      </c>
+      <c r="N15" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="O15" s="3"/>
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
       <c r="S15" s="3"/>
-      <c r="T15" s="3"/>
-    </row>
-    <row r="16" spans="1:21">
+    </row>
+    <row r="16" spans="1:20">
       <c r="A16" s="13" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>29</v>
+        <v>206</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="F16" s="3"/>
-      <c r="G16" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H16" s="3"/>
-      <c r="I16" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="J16" s="11">
-        <v>38</v>
-      </c>
-      <c r="K16" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="L16" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M16" s="11"/>
-      <c r="N16" s="11" t="s">
+      <c r="G16" s="3"/>
+      <c r="H16" s="11">
+        <v>1350</v>
+      </c>
+      <c r="I16" s="11">
+        <v>1600</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="K16" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="O16" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="N16" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="O16" s="3"/>
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
       <c r="S16" s="3"/>
-      <c r="T16" s="3"/>
-    </row>
-    <row r="17" spans="1:20">
+    </row>
+    <row r="17" spans="1:19">
       <c r="A17" s="13" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="F17" s="3"/>
-      <c r="G17" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="I17" s="11">
-        <v>0</v>
-      </c>
-      <c r="J17" s="11">
-        <v>200</v>
-      </c>
-      <c r="K17" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="J17" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="L17" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M17" s="11"/>
-      <c r="N17" s="11" t="s">
+      <c r="K17" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="O17" s="3" t="s">
-        <v>31</v>
-      </c>
+      <c r="N17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="O17" s="3"/>
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
       <c r="R17" s="3"/>
       <c r="S17" s="3"/>
-      <c r="T17" s="3"/>
-    </row>
-    <row r="18" spans="1:20">
+    </row>
+    <row r="18" spans="1:19">
       <c r="A18" s="13" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F18" s="3"/>
-      <c r="G18" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="11">
+        <v>0</v>
+      </c>
       <c r="I18" s="11">
-        <v>0</v>
-      </c>
-      <c r="J18" s="11">
-        <v>360</v>
-      </c>
-      <c r="K18" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="L18" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M18" s="11"/>
-      <c r="N18" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="K18" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="O18" s="3" t="s">
+      <c r="N18" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="O18" s="3"/>
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
       <c r="R18" s="3"/>
       <c r="S18" s="3"/>
-      <c r="T18" s="3"/>
-    </row>
-    <row r="19" spans="1:20">
+    </row>
+    <row r="19" spans="1:19">
       <c r="A19" s="13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F19" s="3"/>
-      <c r="G19" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="11">
+        <v>0</v>
+      </c>
       <c r="I19" s="11">
-        <v>940</v>
-      </c>
-      <c r="J19" s="11">
-        <v>1030</v>
-      </c>
-      <c r="K19" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="L19" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M19" s="11"/>
-      <c r="N19" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="J19" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="K19" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="O19" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="N19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O19" s="3"/>
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
       <c r="R19" s="3"/>
       <c r="S19" s="3"/>
-      <c r="T19" s="3"/>
-    </row>
-    <row r="20" spans="1:20">
+    </row>
+    <row r="20" spans="1:19">
       <c r="A20" s="13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F20" s="3"/>
-      <c r="G20" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="11">
+        <v>940</v>
+      </c>
       <c r="I20" s="11">
-        <v>0</v>
-      </c>
-      <c r="J20" s="11">
-        <v>100</v>
-      </c>
-      <c r="K20" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="L20" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M20" s="11"/>
-      <c r="N20" s="11" t="s">
+        <v>1030</v>
+      </c>
+      <c r="J20" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="K20" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="O20" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="N20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="O20" s="3"/>
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
       <c r="R20" s="3"/>
       <c r="S20" s="3"/>
-      <c r="T20" s="3"/>
-    </row>
-    <row r="21" spans="1:20">
+    </row>
+    <row r="21" spans="1:19">
       <c r="A21" s="13" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D21" s="22"/>
+        <v>91</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>42</v>
+      </c>
       <c r="E21" s="18" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="F21" s="3"/>
-      <c r="G21" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="11">
+        <v>0</v>
+      </c>
       <c r="I21" s="11">
-        <v>-100</v>
-      </c>
-      <c r="J21" s="11">
         <v>100</v>
       </c>
-      <c r="K21" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="L21" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M21" s="11"/>
-      <c r="N21" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="O21" s="3" t="s">
-        <v>70</v>
-      </c>
+      <c r="J21" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="K21" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="N21" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O21" s="3"/>
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
       <c r="R21" s="3"/>
       <c r="S21" s="3"/>
-      <c r="T21" s="3"/>
-    </row>
-    <row r="22" spans="1:20">
+    </row>
+    <row r="22" spans="1:19">
       <c r="A22" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D22" s="22"/>
       <c r="E22" s="18" t="s">
         <v>73</v>
       </c>
       <c r="F22" s="3"/>
-      <c r="G22" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="11">
+        <v>-100</v>
+      </c>
       <c r="I22" s="11">
-        <v>-100</v>
-      </c>
-      <c r="J22" s="11">
         <v>100</v>
       </c>
-      <c r="K22" s="11" t="s">
+      <c r="J22" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="L22" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M22" s="11"/>
-      <c r="N22" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="O22" s="3" t="s">
-        <v>71</v>
-      </c>
+      <c r="K22" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="N22" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="O22" s="3"/>
       <c r="P22" s="3"/>
       <c r="Q22" s="3"/>
       <c r="R22" s="3"/>
       <c r="S22" s="3"/>
-      <c r="T22" s="3"/>
-    </row>
-    <row r="23" spans="1:20">
+    </row>
+    <row r="23" spans="1:19">
       <c r="A23" s="13" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D23" s="22" t="s">
-        <v>23</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="D23" s="22"/>
       <c r="E23" s="18" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="F23" s="3"/>
-      <c r="G23" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H23" s="3"/>
-      <c r="I23" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="J23" s="11">
-        <v>38</v>
-      </c>
-      <c r="K23" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="L23" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M23" s="11"/>
-      <c r="N23" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="O23" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="G23" s="3"/>
+      <c r="H23" s="11">
+        <v>-100</v>
+      </c>
+      <c r="I23" s="11">
+        <v>100</v>
+      </c>
+      <c r="J23" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="K23" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="N23" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="O23" s="3"/>
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
       <c r="R23" s="3"/>
       <c r="S23" s="3"/>
-      <c r="T23" s="3"/>
-    </row>
-    <row r="24" spans="1:20">
+    </row>
+    <row r="24" spans="1:19">
       <c r="A24" s="13" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D24" s="22" t="s">
         <v>23</v>
@@ -2858,808 +2800,751 @@
         <v>16</v>
       </c>
       <c r="F24" s="3"/>
-      <c r="G24" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H24" s="3"/>
-      <c r="I24" s="11" t="s">
+      <c r="G24" s="3"/>
+      <c r="H24" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="J24" s="11">
+      <c r="I24" s="11">
         <v>38</v>
       </c>
-      <c r="K24" s="11" t="s">
+      <c r="J24" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="L24" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M24" s="11"/>
-      <c r="N24" s="11" t="s">
+      <c r="K24" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="O24" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="N24" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O24" s="3"/>
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
       <c r="R24" s="3"/>
       <c r="S24" s="3"/>
-      <c r="T24" s="3"/>
-    </row>
-    <row r="25" spans="1:20">
+    </row>
+    <row r="25" spans="1:19">
       <c r="A25" s="13" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>54</v>
+        <v>23</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>206</v>
+        <v>16</v>
       </c>
       <c r="F25" s="3"/>
-      <c r="G25" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H25" s="3"/>
-      <c r="I25" s="11" t="s">
+      <c r="G25" s="3"/>
+      <c r="H25" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="J25" s="11">
+      <c r="I25" s="11">
         <v>38</v>
       </c>
-      <c r="K25" s="11" t="s">
+      <c r="J25" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="L25" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M25" s="11"/>
-      <c r="N25" s="11" t="s">
+      <c r="K25" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="O25" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="N25" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="O25" s="3"/>
       <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
       <c r="R25" s="3"/>
       <c r="S25" s="3"/>
-      <c r="T25" s="3"/>
-    </row>
-    <row r="26" spans="1:20">
+    </row>
+    <row r="26" spans="1:19">
       <c r="A26" s="13" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D26" s="22"/>
+        <v>96</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>54</v>
+      </c>
       <c r="E26" s="18" t="s">
-        <v>75</v>
+        <v>205</v>
       </c>
       <c r="F26" s="3"/>
-      <c r="G26" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="I26" s="11">
-        <v>100</v>
-      </c>
-      <c r="J26" s="11">
-        <v>700</v>
-      </c>
-      <c r="K26" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="L26" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M26" s="11"/>
-      <c r="N26" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="J26" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="K26" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11" t="s">
         <v>11</v>
+      </c>
+      <c r="N26" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
       <c r="R26" s="3"/>
       <c r="S26" s="3"/>
-      <c r="T26" s="3"/>
-    </row>
-    <row r="27" spans="1:20">
+    </row>
+    <row r="27" spans="1:19">
       <c r="A27" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D27" s="22"/>
       <c r="E27" s="18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F27" s="3"/>
-      <c r="G27" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="11">
+        <v>100</v>
+      </c>
       <c r="I27" s="11">
-        <v>0</v>
-      </c>
-      <c r="J27" s="11">
-        <v>1</v>
-      </c>
-      <c r="K27" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="L27" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M27" s="11"/>
-      <c r="N27" s="11" t="s">
+        <v>700</v>
+      </c>
+      <c r="J27" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="K27" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="N27" s="3"/>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
       <c r="Q27" s="3"/>
       <c r="R27" s="3"/>
       <c r="S27" s="3"/>
-      <c r="T27" s="3"/>
-    </row>
-    <row r="28" spans="1:20">
-      <c r="A28" s="25" t="s">
-        <v>194</v>
+    </row>
+    <row r="28" spans="1:19">
+      <c r="A28" s="13" t="s">
+        <v>76</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C28" s="28" t="s">
-        <v>195</v>
+        <v>157</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="D28" s="22"/>
-      <c r="E28" s="29" t="s">
-        <v>196</v>
+      <c r="E28" s="18" t="s">
+        <v>77</v>
       </c>
       <c r="F28" s="3"/>
-      <c r="G28" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H28" s="3"/>
-      <c r="I28" s="30">
+      <c r="G28" s="3"/>
+      <c r="H28" s="11">
         <v>0</v>
       </c>
-      <c r="J28" s="30">
-        <v>10</v>
-      </c>
-      <c r="K28" s="30" t="s">
-        <v>104</v>
-      </c>
-      <c r="L28" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M28" s="11"/>
-      <c r="N28" s="11" t="s">
+      <c r="I28" s="11">
+        <v>1</v>
+      </c>
+      <c r="J28" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="K28" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="N28" s="3"/>
       <c r="O28" s="3"/>
       <c r="P28" s="3"/>
       <c r="Q28" s="3"/>
       <c r="R28" s="3"/>
       <c r="S28" s="3"/>
-      <c r="T28" s="3"/>
-    </row>
-    <row r="29" spans="1:20">
-      <c r="A29" s="13" t="s">
-        <v>78</v>
+    </row>
+    <row r="29" spans="1:19">
+      <c r="A29" s="25" t="s">
+        <v>193</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>99</v>
+        <v>157</v>
+      </c>
+      <c r="C29" s="28" t="s">
+        <v>194</v>
       </c>
       <c r="D29" s="22"/>
-      <c r="E29" s="18" t="s">
-        <v>43</v>
+      <c r="E29" s="29" t="s">
+        <v>195</v>
       </c>
       <c r="F29" s="3"/>
-      <c r="G29" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H29" s="3"/>
-      <c r="I29" s="11">
+      <c r="G29" s="3"/>
+      <c r="H29" s="30">
         <v>0</v>
       </c>
-      <c r="J29" s="11">
-        <v>100</v>
-      </c>
-      <c r="K29" s="11" t="s">
-        <v>220</v>
-      </c>
-      <c r="L29" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M29" s="11"/>
-      <c r="N29" s="11" t="s">
+      <c r="I29" s="30">
+        <v>10</v>
+      </c>
+      <c r="J29" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="K29" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="N29" s="3"/>
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
       <c r="Q29" s="3"/>
       <c r="R29" s="3"/>
       <c r="S29" s="3"/>
-      <c r="T29" s="3"/>
-    </row>
-    <row r="30" spans="1:20">
-      <c r="A30" s="25" t="s">
-        <v>186</v>
+    </row>
+    <row r="30" spans="1:19">
+      <c r="A30" s="13" t="s">
+        <v>78</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C30" s="28" t="s">
-        <v>187</v>
+        <v>157</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="18" t="s">
-        <v>188</v>
+        <v>43</v>
       </c>
       <c r="F30" s="3"/>
-      <c r="G30" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H30" s="3"/>
-      <c r="I30" s="30">
+      <c r="G30" s="3"/>
+      <c r="H30" s="11">
         <v>0</v>
       </c>
-      <c r="J30" s="30">
-        <v>3000</v>
-      </c>
-      <c r="K30" s="30" t="s">
-        <v>189</v>
-      </c>
-      <c r="L30" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M30" s="11"/>
-      <c r="N30" s="11" t="s">
+      <c r="I30" s="11">
+        <v>100</v>
+      </c>
+      <c r="J30" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="K30" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="N30" s="3"/>
       <c r="O30" s="3"/>
       <c r="P30" s="3"/>
       <c r="Q30" s="3"/>
       <c r="R30" s="3"/>
       <c r="S30" s="3"/>
-      <c r="T30" s="3"/>
-    </row>
-    <row r="31" spans="1:20">
+    </row>
+    <row r="31" spans="1:19">
       <c r="A31" s="25" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="30">
+        <v>0</v>
+      </c>
+      <c r="I31" s="30">
+        <v>3000</v>
+      </c>
+      <c r="J31" s="30" t="s">
         <v>188</v>
       </c>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H31" s="3"/>
-      <c r="I31" s="30">
-        <v>0</v>
-      </c>
-      <c r="J31" s="30">
-        <v>4000</v>
-      </c>
-      <c r="K31" s="30" t="s">
-        <v>189</v>
-      </c>
-      <c r="L31" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M31" s="11"/>
-      <c r="N31" s="11" t="s">
+      <c r="K31" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="N31" s="3"/>
       <c r="O31" s="3"/>
       <c r="P31" s="3"/>
       <c r="Q31" s="3"/>
       <c r="R31" s="3"/>
       <c r="S31" s="3"/>
-      <c r="T31" s="3"/>
-    </row>
-    <row r="32" spans="1:20" ht="12.6" customHeight="1">
+    </row>
+    <row r="32" spans="1:19">
       <c r="A32" s="25" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D32" s="22"/>
       <c r="E32" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="30">
+        <v>0</v>
+      </c>
+      <c r="I32" s="30">
+        <v>4000</v>
+      </c>
+      <c r="J32" s="30" t="s">
         <v>188</v>
       </c>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H32" s="3"/>
-      <c r="I32" s="30">
-        <v>0</v>
-      </c>
-      <c r="J32" s="30">
-        <v>3000</v>
-      </c>
-      <c r="K32" s="30" t="s">
-        <v>189</v>
-      </c>
-      <c r="L32" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M32" s="11"/>
-      <c r="N32" s="11" t="s">
+      <c r="K32" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="N32" s="3"/>
       <c r="O32" s="3"/>
       <c r="P32" s="3"/>
       <c r="Q32" s="3"/>
       <c r="R32" s="3"/>
       <c r="S32" s="3"/>
-      <c r="T32" s="3"/>
-    </row>
-    <row r="33" spans="1:20" ht="12.6" customHeight="1">
-      <c r="A33" s="26" t="s">
-        <v>197</v>
+    </row>
+    <row r="33" spans="1:19" ht="12.6" customHeight="1">
+      <c r="A33" s="25" t="s">
+        <v>191</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C33" s="31" t="s">
-        <v>198</v>
+        <v>157</v>
+      </c>
+      <c r="C33" s="28" t="s">
+        <v>192</v>
       </c>
       <c r="D33" s="22"/>
-      <c r="E33" s="32" t="s">
-        <v>199</v>
+      <c r="E33" s="18" t="s">
+        <v>187</v>
       </c>
       <c r="F33" s="3"/>
-      <c r="G33" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H33" s="3"/>
-      <c r="I33" s="31">
+      <c r="G33" s="3"/>
+      <c r="H33" s="30">
         <v>0</v>
       </c>
-      <c r="J33" s="33">
-        <v>999999</v>
-      </c>
-      <c r="K33" s="33" t="s">
-        <v>200</v>
-      </c>
-      <c r="L33" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M33" s="11"/>
-      <c r="N33" s="11" t="s">
+      <c r="I33" s="30">
+        <v>3000</v>
+      </c>
+      <c r="J33" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="K33" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="N33" s="3"/>
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
       <c r="Q33" s="3"/>
       <c r="R33" s="3"/>
       <c r="S33" s="3"/>
-      <c r="T33" s="3"/>
-    </row>
-    <row r="34" spans="1:20">
-      <c r="A34" s="13" t="s">
-        <v>63</v>
+    </row>
+    <row r="34" spans="1:19" ht="12.6" customHeight="1">
+      <c r="A34" s="26" t="s">
+        <v>196</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>94</v>
+        <v>157</v>
+      </c>
+      <c r="C34" s="31" t="s">
+        <v>197</v>
       </c>
       <c r="D34" s="22"/>
-      <c r="E34" s="18" t="s">
-        <v>16</v>
+      <c r="E34" s="32" t="s">
+        <v>198</v>
       </c>
       <c r="F34" s="3"/>
-      <c r="G34" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H34" s="3"/>
-      <c r="I34" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="J34" s="11">
-        <v>38</v>
-      </c>
-      <c r="K34" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="L34" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M34" s="11"/>
-      <c r="N34" s="11" t="s">
+      <c r="G34" s="3"/>
+      <c r="H34" s="31">
+        <v>0</v>
+      </c>
+      <c r="I34" s="33">
+        <v>999999</v>
+      </c>
+      <c r="J34" s="33" t="s">
+        <v>199</v>
+      </c>
+      <c r="K34" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="N34" s="3"/>
       <c r="O34" s="3"/>
       <c r="P34" s="3"/>
       <c r="Q34" s="3"/>
       <c r="R34" s="3"/>
       <c r="S34" s="3"/>
-      <c r="T34" s="3"/>
-    </row>
-    <row r="35" spans="1:20">
+    </row>
+    <row r="35" spans="1:19">
       <c r="A35" s="13" t="s">
-        <v>105</v>
+        <v>63</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="D35" s="22"/>
-      <c r="E35" s="18">
-        <v>1</v>
+      <c r="E35" s="18" t="s">
+        <v>16</v>
       </c>
       <c r="F35" s="3"/>
-      <c r="G35" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H35" s="3"/>
-      <c r="I35" s="11" t="s">
-        <v>107</v>
+      <c r="G35" s="3"/>
+      <c r="H35" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I35" s="11">
+        <v>38</v>
       </c>
       <c r="J35" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="K35" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="L35" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M35" s="11"/>
-      <c r="N35" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="K35" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L35" s="11"/>
+      <c r="M35" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="N35" s="3"/>
       <c r="O35" s="3"/>
       <c r="P35" s="3"/>
       <c r="Q35" s="3"/>
       <c r="R35" s="3"/>
       <c r="S35" s="3"/>
-      <c r="T35" s="3"/>
-    </row>
-    <row r="36" spans="1:20">
+    </row>
+    <row r="36" spans="1:19">
       <c r="A36" s="13" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D36" s="22"/>
-      <c r="E36" s="18" t="s">
-        <v>16</v>
+      <c r="E36" s="18">
+        <v>1</v>
       </c>
       <c r="F36" s="3"/>
-      <c r="G36" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H36" s="3"/>
-      <c r="I36" s="11">
-        <v>-2</v>
-      </c>
-      <c r="J36" s="11">
-        <v>32</v>
-      </c>
-      <c r="K36" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="L36" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M36" s="11"/>
-      <c r="N36" s="11" t="s">
+      <c r="G36" s="3"/>
+      <c r="H36" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="I36" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="J36" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="K36" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="N36" s="3"/>
       <c r="O36" s="3"/>
       <c r="P36" s="3"/>
       <c r="Q36" s="3"/>
       <c r="R36" s="3"/>
       <c r="S36" s="3"/>
-      <c r="T36" s="3"/>
-    </row>
-    <row r="37" spans="1:20">
+    </row>
+    <row r="37" spans="1:19">
       <c r="A37" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D37" s="22"/>
       <c r="E37" s="18" t="s">
         <v>16</v>
       </c>
       <c r="F37" s="3"/>
-      <c r="G37" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="11">
+        <v>-2</v>
+      </c>
       <c r="I37" s="11">
-        <v>-2</v>
-      </c>
-      <c r="J37" s="11">
         <v>32</v>
       </c>
-      <c r="K37" s="11" t="s">
+      <c r="J37" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="L37" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M37" s="11"/>
-      <c r="N37" s="11" t="s">
+      <c r="K37" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L37" s="11"/>
+      <c r="M37" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="N37" s="3"/>
       <c r="O37" s="3"/>
       <c r="P37" s="3"/>
       <c r="Q37" s="3"/>
       <c r="R37" s="3"/>
       <c r="S37" s="3"/>
-      <c r="T37" s="3"/>
-    </row>
-    <row r="38" spans="1:20">
+    </row>
+    <row r="38" spans="1:19">
       <c r="A38" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D38" s="22"/>
       <c r="E38" s="18" t="s">
-        <v>206</v>
+        <v>16</v>
       </c>
       <c r="F38" s="3"/>
-      <c r="G38" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="11">
+        <v>-2</v>
+      </c>
       <c r="I38" s="11">
-        <v>33</v>
-      </c>
-      <c r="J38" s="11">
-        <v>37</v>
-      </c>
-      <c r="K38" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="J38" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="L38" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M38" s="11"/>
-      <c r="N38" s="11" t="s">
+      <c r="K38" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L38" s="11"/>
+      <c r="M38" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="N38" s="3"/>
       <c r="O38" s="3"/>
       <c r="P38" s="3"/>
       <c r="Q38" s="3"/>
       <c r="R38" s="3"/>
       <c r="S38" s="3"/>
-      <c r="T38" s="3"/>
-    </row>
-    <row r="39" spans="1:20">
+    </row>
+    <row r="39" spans="1:19">
       <c r="A39" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D39" s="22"/>
       <c r="E39" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F39" s="3"/>
-      <c r="G39" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="11">
+        <v>33</v>
+      </c>
       <c r="I39" s="11">
-        <v>33</v>
-      </c>
-      <c r="J39" s="11">
         <v>37</v>
       </c>
-      <c r="K39" s="11" t="s">
+      <c r="J39" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="L39" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M39" s="11"/>
-      <c r="N39" s="11" t="s">
+      <c r="K39" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L39" s="11"/>
+      <c r="M39" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="N39" s="3"/>
       <c r="O39" s="3"/>
       <c r="P39" s="3"/>
       <c r="Q39" s="3"/>
       <c r="R39" s="3"/>
       <c r="S39" s="3"/>
-      <c r="T39" s="3"/>
-    </row>
-    <row r="40" spans="1:20">
+    </row>
+    <row r="40" spans="1:19">
       <c r="A40" s="13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D40" s="22"/>
       <c r="E40" s="18" t="s">
-        <v>120</v>
+        <v>205</v>
       </c>
       <c r="F40" s="3"/>
-      <c r="G40" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="11">
+        <v>33</v>
+      </c>
       <c r="I40" s="11">
-        <v>3</v>
-      </c>
-      <c r="J40" s="11">
-        <v>7</v>
-      </c>
-      <c r="K40" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="L40" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M40" s="11"/>
-      <c r="N40" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="J40" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="K40" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L40" s="11"/>
+      <c r="M40" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="N40" s="3"/>
       <c r="O40" s="3"/>
       <c r="P40" s="3"/>
       <c r="Q40" s="3"/>
       <c r="R40" s="3"/>
       <c r="S40" s="3"/>
-      <c r="T40" s="3"/>
-    </row>
-    <row r="41" spans="1:20">
+    </row>
+    <row r="41" spans="1:19">
       <c r="A41" s="13" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D41" s="22"/>
       <c r="E41" s="18" t="s">
         <v>120</v>
       </c>
       <c r="F41" s="3"/>
-      <c r="G41" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="11">
+        <v>3</v>
+      </c>
       <c r="I41" s="11">
-        <v>3</v>
-      </c>
-      <c r="J41" s="11">
         <v>7</v>
       </c>
-      <c r="K41" s="11" t="s">
+      <c r="J41" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="L41" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M41" s="11"/>
-      <c r="N41" s="11" t="s">
+      <c r="K41" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L41" s="11"/>
+      <c r="M41" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="N41" s="3"/>
       <c r="O41" s="3"/>
       <c r="P41" s="3"/>
       <c r="Q41" s="3"/>
       <c r="R41" s="3"/>
       <c r="S41" s="3"/>
-      <c r="T41" s="3"/>
-    </row>
-    <row r="42" spans="1:20">
+    </row>
+    <row r="42" spans="1:19">
       <c r="A42" s="13" t="s">
-        <v>221</v>
+        <v>122</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="D42" s="22" t="s">
-        <v>60</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="D42" s="22"/>
       <c r="E42" s="18" t="s">
-        <v>61</v>
+        <v>120</v>
       </c>
       <c r="F42" s="3"/>
-      <c r="G42" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H42" s="3"/>
-      <c r="I42" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="J42" s="11">
-        <v>38</v>
-      </c>
-      <c r="K42" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="L42" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M42" s="11"/>
-      <c r="N42" s="11" t="s">
+      <c r="G42" s="3"/>
+      <c r="H42" s="11">
+        <v>3</v>
+      </c>
+      <c r="I42" s="11">
+        <v>7</v>
+      </c>
+      <c r="J42" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="K42" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L42" s="11"/>
+      <c r="M42" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="O42" s="3" t="s">
-        <v>62</v>
-      </c>
+      <c r="N42" s="3"/>
+      <c r="O42" s="3"/>
       <c r="P42" s="3"/>
       <c r="Q42" s="3"/>
       <c r="R42" s="3"/>
       <c r="S42" s="3"/>
-      <c r="T42" s="3"/>
-    </row>
-    <row r="43" spans="1:20">
+    </row>
+    <row r="43" spans="1:19">
       <c r="A43" s="13" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D43" s="22" t="s">
         <v>60</v>
@@ -3668,506 +3553,472 @@
         <v>61</v>
       </c>
       <c r="F43" s="3"/>
-      <c r="G43" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H43" s="3"/>
-      <c r="I43" s="11" t="s">
+      <c r="G43" s="3"/>
+      <c r="H43" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="J43" s="11">
+      <c r="I43" s="11">
         <v>38</v>
       </c>
-      <c r="K43" s="11" t="s">
+      <c r="J43" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="L43" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M43" s="11"/>
-      <c r="N43" s="11" t="s">
+      <c r="K43" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L43" s="11"/>
+      <c r="M43" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="O43" s="3" t="s">
+      <c r="N43" s="3" t="s">
         <v>62</v>
       </c>
+      <c r="O43" s="3"/>
       <c r="P43" s="3"/>
       <c r="Q43" s="3"/>
       <c r="R43" s="3"/>
       <c r="S43" s="3"/>
-      <c r="T43" s="3"/>
-    </row>
-    <row r="44" spans="1:20">
+    </row>
+    <row r="44" spans="1:19">
       <c r="A44" s="13" t="s">
-        <v>124</v>
+        <v>219</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="D44" s="22"/>
+        <v>221</v>
+      </c>
+      <c r="D44" s="22" t="s">
+        <v>60</v>
+      </c>
       <c r="E44" s="18" t="s">
-        <v>126</v>
+        <v>61</v>
       </c>
       <c r="F44" s="3"/>
-      <c r="G44" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="I44" s="11">
-        <v>0</v>
-      </c>
-      <c r="J44" s="11">
-        <v>10</v>
-      </c>
-      <c r="K44" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="L44" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M44" s="11"/>
-      <c r="N44" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="J44" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="K44" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L44" s="11"/>
+      <c r="M44" s="11" t="s">
         <v>11</v>
+      </c>
+      <c r="N44" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="O44" s="3"/>
       <c r="P44" s="3"/>
       <c r="Q44" s="3"/>
       <c r="R44" s="3"/>
       <c r="S44" s="3"/>
-      <c r="T44" s="3"/>
-    </row>
-    <row r="45" spans="1:20">
+    </row>
+    <row r="45" spans="1:19">
       <c r="A45" s="13" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D45" s="22"/>
       <c r="E45" s="18" t="s">
         <v>126</v>
       </c>
       <c r="F45" s="3"/>
-      <c r="G45" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="11">
+        <v>0</v>
+      </c>
       <c r="I45" s="11">
-        <v>0</v>
-      </c>
-      <c r="J45" s="11">
         <v>10</v>
       </c>
-      <c r="K45" s="11" t="s">
+      <c r="J45" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="L45" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M45" s="11"/>
-      <c r="N45" s="11" t="s">
+      <c r="K45" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L45" s="11"/>
+      <c r="M45" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="N45" s="3"/>
       <c r="O45" s="3"/>
       <c r="P45" s="3"/>
       <c r="Q45" s="3"/>
       <c r="R45" s="3"/>
       <c r="S45" s="3"/>
-      <c r="T45" s="3"/>
-    </row>
-    <row r="46" spans="1:20">
+    </row>
+    <row r="46" spans="1:19">
       <c r="A46" s="13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D46" s="22"/>
       <c r="E46" s="18" t="s">
-        <v>57</v>
+        <v>126</v>
       </c>
       <c r="F46" s="3"/>
-      <c r="G46" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="11">
+        <v>0</v>
+      </c>
       <c r="I46" s="11">
-        <v>0</v>
-      </c>
-      <c r="J46" s="11">
-        <v>450</v>
-      </c>
-      <c r="K46" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="L46" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M46" s="11"/>
-      <c r="N46" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J46" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="K46" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L46" s="11"/>
+      <c r="M46" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="N46" s="3"/>
       <c r="O46" s="3"/>
       <c r="P46" s="3"/>
       <c r="Q46" s="3"/>
       <c r="R46" s="3"/>
       <c r="S46" s="3"/>
-      <c r="T46" s="3"/>
-    </row>
-    <row r="47" spans="1:20">
+    </row>
+    <row r="47" spans="1:19">
       <c r="A47" s="13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D47" s="22"/>
       <c r="E47" s="18" t="s">
         <v>57</v>
       </c>
       <c r="F47" s="3"/>
-      <c r="G47" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="11">
+        <v>0</v>
+      </c>
       <c r="I47" s="11">
-        <v>0</v>
-      </c>
-      <c r="J47" s="11">
         <v>450</v>
       </c>
-      <c r="K47" s="11" t="s">
+      <c r="J47" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="L47" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M47" s="11"/>
-      <c r="N47" s="11" t="s">
+      <c r="K47" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L47" s="11"/>
+      <c r="M47" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="N47" s="3"/>
       <c r="O47" s="3"/>
       <c r="P47" s="3"/>
       <c r="Q47" s="3"/>
       <c r="R47" s="3"/>
       <c r="S47" s="3"/>
-      <c r="T47" s="3"/>
-    </row>
-    <row r="48" spans="1:20">
+    </row>
+    <row r="48" spans="1:19">
       <c r="A48" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D48" s="22"/>
       <c r="E48" s="18" t="s">
-        <v>135</v>
+        <v>57</v>
       </c>
       <c r="F48" s="3"/>
-      <c r="G48" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="11">
+        <v>0</v>
+      </c>
       <c r="I48" s="11">
-        <v>0</v>
-      </c>
-      <c r="J48" s="11">
-        <v>10</v>
-      </c>
-      <c r="K48" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="L48" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M48" s="11"/>
-      <c r="N48" s="11" t="s">
+        <v>450</v>
+      </c>
+      <c r="J48" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="K48" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L48" s="11"/>
+      <c r="M48" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="N48" s="3"/>
       <c r="O48" s="3"/>
       <c r="P48" s="3"/>
       <c r="Q48" s="3"/>
       <c r="R48" s="3"/>
       <c r="S48" s="3"/>
-      <c r="T48" s="3"/>
-    </row>
-    <row r="49" spans="1:20">
+    </row>
+    <row r="49" spans="1:19">
       <c r="A49" s="13" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D49" s="22"/>
       <c r="E49" s="18" t="s">
         <v>135</v>
       </c>
       <c r="F49" s="3"/>
-      <c r="G49" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="11">
+        <v>0</v>
+      </c>
       <c r="I49" s="11">
-        <v>0</v>
-      </c>
-      <c r="J49" s="11">
         <v>10</v>
       </c>
-      <c r="K49" s="11" t="s">
+      <c r="J49" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="L49" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M49" s="11"/>
-      <c r="N49" s="11" t="s">
+      <c r="K49" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L49" s="11"/>
+      <c r="M49" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="N49" s="3"/>
       <c r="O49" s="3"/>
       <c r="P49" s="3"/>
       <c r="Q49" s="3"/>
       <c r="R49" s="3"/>
       <c r="S49" s="3"/>
-      <c r="T49" s="3"/>
-    </row>
-    <row r="50" spans="1:20">
+    </row>
+    <row r="50" spans="1:19">
       <c r="A50" s="13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D50" s="22"/>
       <c r="E50" s="18" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="F50" s="3"/>
-      <c r="G50" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="11">
+        <v>0</v>
+      </c>
       <c r="I50" s="11">
-        <v>-1</v>
-      </c>
-      <c r="J50" s="11">
-        <v>1</v>
-      </c>
-      <c r="K50" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="L50" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M50" s="11"/>
-      <c r="N50" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J50" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="K50" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L50" s="11"/>
+      <c r="M50" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="N50" s="3"/>
       <c r="O50" s="3"/>
       <c r="P50" s="3"/>
       <c r="Q50" s="3"/>
       <c r="R50" s="3"/>
       <c r="S50" s="3"/>
-      <c r="T50" s="3"/>
-    </row>
-    <row r="51" spans="1:20">
+    </row>
+    <row r="51" spans="1:19">
       <c r="A51" s="13" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D51" s="22"/>
       <c r="E51" s="18" t="s">
         <v>141</v>
       </c>
       <c r="F51" s="3"/>
-      <c r="G51" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="11">
+        <v>-1</v>
+      </c>
       <c r="I51" s="11">
-        <v>-1</v>
-      </c>
-      <c r="J51" s="11">
         <v>1</v>
       </c>
-      <c r="K51" s="11" t="s">
+      <c r="J51" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="L51" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M51" s="11"/>
-      <c r="N51" s="11" t="s">
+      <c r="K51" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L51" s="11"/>
+      <c r="M51" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="N51" s="3"/>
       <c r="O51" s="3"/>
       <c r="P51" s="3"/>
       <c r="Q51" s="3"/>
       <c r="R51" s="3"/>
       <c r="S51" s="3"/>
-      <c r="T51" s="3"/>
-    </row>
-    <row r="52" spans="1:20">
+    </row>
+    <row r="52" spans="1:19">
       <c r="A52" s="13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D52" s="22"/>
       <c r="E52" s="18" t="s">
-        <v>16</v>
+        <v>141</v>
       </c>
       <c r="F52" s="3"/>
-      <c r="G52" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="11">
+        <v>-1</v>
+      </c>
       <c r="I52" s="11">
-        <v>0</v>
-      </c>
-      <c r="J52" s="11">
-        <v>90</v>
-      </c>
-      <c r="K52" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="L52" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M52" s="11"/>
-      <c r="N52" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="J52" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="K52" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L52" s="11"/>
+      <c r="M52" s="11" t="s">
         <v>11</v>
       </c>
+      <c r="N52" s="3"/>
       <c r="O52" s="3"/>
       <c r="P52" s="3"/>
       <c r="Q52" s="3"/>
       <c r="R52" s="3"/>
       <c r="S52" s="3"/>
-      <c r="T52" s="3"/>
-    </row>
-    <row r="53" spans="1:20">
+    </row>
+    <row r="53" spans="1:19">
       <c r="A53" s="13" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D53" s="22"/>
       <c r="E53" s="18" t="s">
-        <v>150</v>
+        <v>16</v>
       </c>
       <c r="F53" s="3"/>
-      <c r="G53" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H53" s="3" t="s">
-        <v>44</v>
+      <c r="G53" s="3"/>
+      <c r="H53" s="11">
+        <v>0</v>
       </c>
       <c r="I53" s="11">
-        <v>0</v>
-      </c>
-      <c r="J53" s="11">
-        <v>40000</v>
-      </c>
-      <c r="K53" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="L53" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M53" s="11"/>
-      <c r="N53" s="11" t="s">
-        <v>185</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="J53" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="K53" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L53" s="11"/>
+      <c r="M53" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="N53" s="3"/>
       <c r="O53" s="3"/>
       <c r="P53" s="3"/>
       <c r="Q53" s="3"/>
       <c r="R53" s="3"/>
       <c r="S53" s="3"/>
-      <c r="T53" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="54" spans="1:20">
+    </row>
+    <row r="54" spans="1:19">
       <c r="A54" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>100</v>
       </c>
       <c r="C54" s="34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D54" s="22"/>
       <c r="E54" s="18">
         <v>1</v>
       </c>
       <c r="F54" s="34"/>
-      <c r="G54" s="34"/>
-      <c r="H54" s="3"/>
-      <c r="I54" s="34">
+      <c r="G54" s="3"/>
+      <c r="H54" s="34">
         <v>0</v>
       </c>
-      <c r="J54" s="35">
+      <c r="I54" s="35">
         <v>999</v>
       </c>
-      <c r="K54" s="35" t="s">
-        <v>203</v>
-      </c>
-      <c r="L54" s="23">
+      <c r="J54" s="35" t="s">
+        <v>202</v>
+      </c>
+      <c r="K54" s="23">
         <v>99999</v>
       </c>
+      <c r="L54" s="11"/>
       <c r="M54" s="11"/>
-      <c r="N54" s="11"/>
+      <c r="N54" s="3"/>
       <c r="O54" s="3"/>
       <c r="P54" s="3"/>
       <c r="Q54" s="3"/>
       <c r="R54" s="3"/>
       <c r="S54" s="3"/>
-      <c r="T54" s="3"/>
-    </row>
-    <row r="55" spans="1:20">
+    </row>
+    <row r="55" spans="1:19">
       <c r="A55" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>100</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D55" s="22"/>
       <c r="E55" s="18">
@@ -4175,37 +4026,36 @@
       </c>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
-      <c r="H55" s="3"/>
+      <c r="H55" s="11">
+        <v>1</v>
+      </c>
       <c r="I55" s="11">
-        <v>1</v>
-      </c>
-      <c r="J55" s="11">
         <v>36</v>
       </c>
-      <c r="K55" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="L55" s="23">
+      <c r="J55" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="K55" s="23">
         <v>99999</v>
       </c>
+      <c r="L55" s="11"/>
       <c r="M55" s="11"/>
-      <c r="N55" s="11"/>
+      <c r="N55" s="3"/>
       <c r="O55" s="3"/>
       <c r="P55" s="3"/>
       <c r="Q55" s="3"/>
       <c r="R55" s="3"/>
       <c r="S55" s="3"/>
-      <c r="T55" s="3"/>
-    </row>
-    <row r="56" spans="1:20">
+    </row>
+    <row r="56" spans="1:19">
       <c r="A56" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>100</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D56" s="22"/>
       <c r="E56" s="18">
@@ -4213,67 +4063,65 @@
       </c>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
-      <c r="H56" s="3"/>
+      <c r="H56" s="11" t="s">
+        <v>107</v>
+      </c>
       <c r="I56" s="11" t="s">
-        <v>107</v>
+        <v>156</v>
       </c>
       <c r="J56" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="K56" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="L56" s="23">
+      <c r="K56" s="23">
         <v>99999</v>
       </c>
+      <c r="L56" s="11"/>
       <c r="M56" s="11"/>
-      <c r="N56" s="11"/>
+      <c r="N56" s="3"/>
       <c r="O56" s="3"/>
       <c r="P56" s="3"/>
       <c r="Q56" s="3"/>
       <c r="R56" s="3"/>
       <c r="S56" s="3"/>
-      <c r="T56" s="3"/>
-    </row>
-    <row r="57" spans="1:20">
+    </row>
+    <row r="57" spans="1:19">
       <c r="A57" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C57" s="3" t="s">
         <v>182</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>183</v>
       </c>
       <c r="D57" s="22"/>
       <c r="E57" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
-      <c r="H57" s="3"/>
+      <c r="H57" s="11">
+        <v>0</v>
+      </c>
       <c r="I57" s="11">
-        <v>0</v>
-      </c>
-      <c r="J57" s="11">
         <v>11000</v>
       </c>
-      <c r="K57" s="11" t="s">
+      <c r="J57" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="K57" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="L57" s="11"/>
+      <c r="M57" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="L57" s="27">
-        <v>1E+36</v>
-      </c>
-      <c r="M57" s="11"/>
-      <c r="N57" s="11" t="s">
-        <v>185</v>
-      </c>
+      <c r="N57" s="3"/>
       <c r="O57" s="3"/>
       <c r="P57" s="3"/>
       <c r="Q57" s="3"/>
       <c r="R57" s="3"/>
       <c r="S57" s="3"/>
-      <c r="T57" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
2D slice is now initialize with fillValue from roscop.csv, and not with 1e36 cmd line option display version and date remove code_roscop.csv form main directory
</commit_message>
<xml_diff>
--- a/roscop/code_roscop.xlsx
+++ b/roscop/code_roscop.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgrelet\go\src\github.com\jgrelet\oceano2oceansites\roscop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="96" yWindow="12" windowWidth="14508" windowHeight="8412"/>
+    <workbookView xWindow="90" yWindow="15" windowWidth="14505" windowHeight="8415"/>
   </bookViews>
   <sheets>
     <sheet name="code_roscop" sheetId="5" r:id="rId1"/>
@@ -47,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="235">
   <si>
     <t>long_name</t>
   </si>
@@ -725,17 +730,44 @@
   </si>
   <si>
     <t>_FillValue</t>
+  </si>
+  <si>
+    <t>COND1</t>
+  </si>
+  <si>
+    <t>COND2</t>
+  </si>
+  <si>
+    <t>mS/cm</t>
+  </si>
+  <si>
+    <t>CNDC</t>
+  </si>
+  <si>
+    <t>float33</t>
+  </si>
+  <si>
+    <t>electrical conductivity</t>
+  </si>
+  <si>
+    <t>0.002</t>
+  </si>
+  <si>
+    <t>COND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">electrical conductivity </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0E+00"/>
     <numFmt numFmtId="165" formatCode="0.E+00"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1537,7 +1569,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1569,9 +1601,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1603,6 +1636,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1778,37 +1812,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="13"/>
+    <col min="1" max="1" width="11.5703125" style="13"/>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="34.88671875" customWidth="1"/>
-    <col min="4" max="4" width="28.88671875" style="21" customWidth="1"/>
-    <col min="5" max="5" width="24.109375" style="17" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" customWidth="1"/>
-    <col min="7" max="7" width="32.88671875" customWidth="1"/>
-    <col min="8" max="8" width="6.109375" customWidth="1"/>
-    <col min="9" max="9" width="7.5546875" style="6" customWidth="1"/>
-    <col min="10" max="10" width="8.109375" style="6" customWidth="1"/>
-    <col min="11" max="11" width="7.44140625" style="6" customWidth="1"/>
-    <col min="12" max="12" width="7.88671875" style="10" customWidth="1"/>
-    <col min="13" max="13" width="5.6640625" style="6" customWidth="1"/>
-    <col min="14" max="14" width="8.5546875" style="6" customWidth="1"/>
-    <col min="15" max="15" width="34.109375" customWidth="1"/>
-    <col min="16" max="16" width="11.44140625" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" style="21" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" style="17" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="32.85546875" customWidth="1"/>
+    <col min="8" max="8" width="6.140625" customWidth="1"/>
+    <col min="9" max="9" width="7.5703125" style="6" customWidth="1"/>
+    <col min="10" max="10" width="8.140625" style="6" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" style="6" customWidth="1"/>
+    <col min="12" max="12" width="7.85546875" style="10" customWidth="1"/>
+    <col min="13" max="13" width="5.7109375" style="6" customWidth="1"/>
+    <col min="14" max="14" width="8.5703125" style="6" customWidth="1"/>
+    <col min="15" max="15" width="34.140625" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>88</v>
       </c>
@@ -1871,7 +1905,7 @@
       </c>
       <c r="U1" s="8"/>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>14</v>
       </c>
@@ -1934,7 +1968,7 @@
       </c>
       <c r="U2" s="2"/>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>87</v>
       </c>
@@ -1970,7 +2004,7 @@
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>109</v>
       </c>
@@ -2006,7 +2040,7 @@
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>19</v>
       </c>
@@ -2044,7 +2078,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
@@ -2082,7 +2116,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="15">
+    <row r="7" spans="1:21" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>18</v>
       </c>
@@ -2124,7 +2158,7 @@
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>168</v>
       </c>
@@ -2160,7 +2194,7 @@
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>111</v>
       </c>
@@ -2206,7 +2240,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>48</v>
       </c>
@@ -2250,7 +2284,7 @@
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
         <v>55</v>
       </c>
@@ -2296,7 +2330,7 @@
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
         <v>56</v>
       </c>
@@ -2342,32 +2376,30 @@
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>59</v>
+        <v>229</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>166</v>
+        <v>230</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D13" s="22" t="s">
-        <v>216</v>
-      </c>
+        <v>231</v>
+      </c>
+      <c r="D13" s="22"/>
       <c r="E13" s="18" t="s">
-        <v>60</v>
+        <v>228</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3" t="s">
         <v>218</v>
       </c>
       <c r="H13" s="3"/>
-      <c r="I13" s="11" t="s">
-        <v>13</v>
+      <c r="I13" s="11">
+        <v>30</v>
       </c>
       <c r="J13" s="11">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="K13" s="11" t="s">
         <v>11</v>
@@ -2377,32 +2409,30 @@
       </c>
       <c r="M13" s="11"/>
       <c r="N13" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="O13" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>232</v>
+      </c>
+      <c r="O13" s="3"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>166</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>63</v>
+        <v>216</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3" t="s">
@@ -2426,7 +2456,7 @@
         <v>12</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
@@ -2434,35 +2464,35 @@
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>166</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>215</v>
+        <v>63</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3" t="s">
         <v>218</v>
       </c>
       <c r="H15" s="3"/>
-      <c r="I15" s="11">
-        <v>1350</v>
+      <c r="I15" s="11" t="s">
+        <v>13</v>
       </c>
       <c r="J15" s="11">
-        <v>1600</v>
+        <v>38</v>
       </c>
       <c r="K15" s="11" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="L15" s="27">
         <v>1E+36</v>
@@ -2472,7 +2502,7 @@
         <v>12</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
@@ -2480,35 +2510,35 @@
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>166</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>31</v>
+        <v>215</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
         <v>218</v>
       </c>
       <c r="H16" s="3"/>
-      <c r="I16" s="11" t="s">
-        <v>13</v>
+      <c r="I16" s="11">
+        <v>1350</v>
       </c>
       <c r="J16" s="11">
-        <v>38</v>
+        <v>1600</v>
       </c>
       <c r="K16" s="11" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="L16" s="27">
         <v>1E+36</v>
@@ -2518,7 +2548,7 @@
         <v>12</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
@@ -2526,32 +2556,32 @@
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
-        <v>76</v>
+        <v>30</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>166</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3" t="s">
         <v>218</v>
       </c>
       <c r="H17" s="3"/>
-      <c r="I17" s="11">
-        <v>0</v>
+      <c r="I17" s="11" t="s">
+        <v>13</v>
       </c>
       <c r="J17" s="11">
-        <v>200</v>
+        <v>38</v>
       </c>
       <c r="K17" s="11" t="s">
         <v>11</v>
@@ -2564,7 +2594,7 @@
         <v>12</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
@@ -2572,21 +2602,21 @@
       <c r="S17" s="3"/>
       <c r="T17" s="3"/>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>166</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3" t="s">
@@ -2597,10 +2627,10 @@
         <v>0</v>
       </c>
       <c r="J18" s="11">
-        <v>360</v>
+        <v>200</v>
       </c>
       <c r="K18" s="11" t="s">
-        <v>77</v>
+        <v>11</v>
       </c>
       <c r="L18" s="27">
         <v>1E+36</v>
@@ -2618,21 +2648,21 @@
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>166</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3" t="s">
@@ -2640,13 +2670,13 @@
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="11">
-        <v>940</v>
+        <v>0</v>
       </c>
       <c r="J19" s="11">
-        <v>1030</v>
+        <v>360</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L19" s="27">
         <v>1E+36</v>
@@ -2656,7 +2686,7 @@
         <v>12</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
@@ -2664,21 +2694,21 @@
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>166</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3" t="s">
@@ -2686,13 +2716,13 @@
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="11">
-        <v>0</v>
+        <v>940</v>
       </c>
       <c r="J20" s="11">
-        <v>100</v>
+        <v>1030</v>
       </c>
       <c r="K20" s="11" t="s">
-        <v>42</v>
+        <v>78</v>
       </c>
       <c r="L20" s="27">
         <v>1E+36</v>
@@ -2702,7 +2732,7 @@
         <v>12</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
@@ -2710,19 +2740,21 @@
       <c r="S20" s="3"/>
       <c r="T20" s="3"/>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>166</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D21" s="22"/>
+        <v>99</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>45</v>
+      </c>
       <c r="E21" s="18" t="s">
-        <v>79</v>
+        <v>46</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3" t="s">
@@ -2730,23 +2762,23 @@
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="11">
-        <v>-100</v>
+        <v>0</v>
       </c>
       <c r="J21" s="11">
         <v>100</v>
       </c>
       <c r="K21" s="11" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="L21" s="27">
         <v>1E+36</v>
       </c>
       <c r="M21" s="11"/>
       <c r="N21" s="11" t="s">
-        <v>73</v>
+        <v>12</v>
       </c>
       <c r="O21" s="3" t="s">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
@@ -2754,15 +2786,15 @@
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>166</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D22" s="22"/>
       <c r="E22" s="18" t="s">
@@ -2787,10 +2819,10 @@
       </c>
       <c r="M22" s="11"/>
       <c r="N22" s="11" t="s">
-        <v>15</v>
+        <v>73</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P22" s="3"/>
       <c r="Q22" s="3"/>
@@ -2798,45 +2830,43 @@
       <c r="S22" s="3"/>
       <c r="T22" s="3"/>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>166</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D23" s="22" t="s">
-        <v>25</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="D23" s="22"/>
       <c r="E23" s="18" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3" t="s">
         <v>218</v>
       </c>
       <c r="H23" s="3"/>
-      <c r="I23" s="11" t="s">
-        <v>13</v>
+      <c r="I23" s="11">
+        <v>-100</v>
       </c>
       <c r="J23" s="11">
-        <v>38</v>
+        <v>100</v>
       </c>
       <c r="K23" s="11" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="L23" s="27">
         <v>1E+36</v>
       </c>
       <c r="M23" s="11"/>
       <c r="N23" s="11" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="O23" s="3" t="s">
-        <v>21</v>
+        <v>75</v>
       </c>
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
@@ -2844,15 +2874,15 @@
       <c r="S23" s="3"/>
       <c r="T23" s="3"/>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" s="13" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>166</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D24" s="22" t="s">
         <v>25</v>
@@ -2882,7 +2912,7 @@
         <v>12</v>
       </c>
       <c r="O24" s="3" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
@@ -2890,21 +2920,21 @@
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" s="13" t="s">
-        <v>67</v>
+        <v>29</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>166</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>214</v>
+        <v>17</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3" t="s">
@@ -2928,7 +2958,7 @@
         <v>12</v>
       </c>
       <c r="O25" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
@@ -2936,33 +2966,35 @@
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="13" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>166</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D26" s="22"/>
+        <v>104</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>57</v>
+      </c>
       <c r="E26" s="18" t="s">
-        <v>81</v>
+        <v>214</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3" t="s">
         <v>218</v>
       </c>
       <c r="H26" s="3"/>
-      <c r="I26" s="11">
-        <v>100</v>
+      <c r="I26" s="11" t="s">
+        <v>13</v>
       </c>
       <c r="J26" s="11">
-        <v>700</v>
+        <v>38</v>
       </c>
       <c r="K26" s="11" t="s">
-        <v>72</v>
+        <v>11</v>
       </c>
       <c r="L26" s="27">
         <v>1E+36</v>
@@ -2971,26 +3003,28 @@
       <c r="N26" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="O26" s="3"/>
+      <c r="O26" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
       <c r="R26" s="3"/>
       <c r="S26" s="3"/>
       <c r="T26" s="3"/>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" s="13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>166</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D27" s="22"/>
       <c r="E27" s="18" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3" t="s">
@@ -2998,13 +3032,13 @@
       </c>
       <c r="H27" s="3"/>
       <c r="I27" s="11">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J27" s="11">
-        <v>1</v>
+        <v>700</v>
       </c>
       <c r="K27" s="11" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="L27" s="27">
         <v>1E+36</v>
@@ -3020,33 +3054,33 @@
       <c r="S27" s="3"/>
       <c r="T27" s="3"/>
     </row>
-    <row r="28" spans="1:20">
-      <c r="A28" s="25" t="s">
-        <v>202</v>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A28" s="13" t="s">
+        <v>82</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C28" s="28" t="s">
-        <v>203</v>
+      <c r="C28" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="D28" s="22"/>
-      <c r="E28" s="29" t="s">
-        <v>204</v>
+      <c r="E28" s="18" t="s">
+        <v>83</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3" t="s">
         <v>218</v>
       </c>
       <c r="H28" s="3"/>
-      <c r="I28" s="30">
+      <c r="I28" s="11">
         <v>0</v>
       </c>
-      <c r="J28" s="30">
-        <v>10</v>
-      </c>
-      <c r="K28" s="30" t="s">
-        <v>112</v>
+      <c r="J28" s="11">
+        <v>1</v>
+      </c>
+      <c r="K28" s="11" t="s">
+        <v>84</v>
       </c>
       <c r="L28" s="27">
         <v>1E+36</v>
@@ -3062,33 +3096,33 @@
       <c r="S28" s="3"/>
       <c r="T28" s="3"/>
     </row>
-    <row r="29" spans="1:20">
-      <c r="A29" s="13" t="s">
-        <v>85</v>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A29" s="25" t="s">
+        <v>202</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>107</v>
+      <c r="C29" s="28" t="s">
+        <v>203</v>
       </c>
       <c r="D29" s="22"/>
-      <c r="E29" s="18" t="s">
-        <v>46</v>
+      <c r="E29" s="29" t="s">
+        <v>204</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3" t="s">
         <v>218</v>
       </c>
       <c r="H29" s="3"/>
-      <c r="I29" s="11">
+      <c r="I29" s="30">
         <v>0</v>
       </c>
-      <c r="J29" s="11">
-        <v>100</v>
-      </c>
-      <c r="K29" s="11" t="s">
-        <v>86</v>
+      <c r="J29" s="30">
+        <v>10</v>
+      </c>
+      <c r="K29" s="30" t="s">
+        <v>112</v>
       </c>
       <c r="L29" s="27">
         <v>1E+36</v>
@@ -3104,33 +3138,33 @@
       <c r="S29" s="3"/>
       <c r="T29" s="3"/>
     </row>
-    <row r="30" spans="1:20">
-      <c r="A30" s="25" t="s">
-        <v>194</v>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A30" s="13" t="s">
+        <v>85</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C30" s="28" t="s">
-        <v>195</v>
+      <c r="C30" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="18" t="s">
-        <v>196</v>
+        <v>46</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3" t="s">
         <v>218</v>
       </c>
       <c r="H30" s="3"/>
-      <c r="I30" s="30">
+      <c r="I30" s="11">
         <v>0</v>
       </c>
-      <c r="J30" s="30">
-        <v>3000</v>
-      </c>
-      <c r="K30" s="30" t="s">
-        <v>197</v>
+      <c r="J30" s="11">
+        <v>100</v>
+      </c>
+      <c r="K30" s="11" t="s">
+        <v>86</v>
       </c>
       <c r="L30" s="27">
         <v>1E+36</v>
@@ -3146,15 +3180,15 @@
       <c r="S30" s="3"/>
       <c r="T30" s="3"/>
     </row>
-    <row r="31" spans="1:20">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" s="25" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>166</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="18" t="s">
@@ -3169,7 +3203,7 @@
         <v>0</v>
       </c>
       <c r="J31" s="30">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="K31" s="30" t="s">
         <v>197</v>
@@ -3188,15 +3222,15 @@
       <c r="S31" s="3"/>
       <c r="T31" s="3"/>
     </row>
-    <row r="32" spans="1:20" ht="12.6" customHeight="1">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" s="25" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>166</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D32" s="22"/>
       <c r="E32" s="18" t="s">
@@ -3211,7 +3245,7 @@
         <v>0</v>
       </c>
       <c r="J32" s="30">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="K32" s="30" t="s">
         <v>197</v>
@@ -3230,33 +3264,33 @@
       <c r="S32" s="3"/>
       <c r="T32" s="3"/>
     </row>
-    <row r="33" spans="1:20" ht="12.6" customHeight="1">
-      <c r="A33" s="26" t="s">
-        <v>205</v>
+    <row r="33" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="25" t="s">
+        <v>200</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C33" s="31" t="s">
-        <v>206</v>
+      <c r="C33" s="28" t="s">
+        <v>201</v>
       </c>
       <c r="D33" s="22"/>
-      <c r="E33" s="32" t="s">
-        <v>207</v>
+      <c r="E33" s="18" t="s">
+        <v>196</v>
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3" t="s">
         <v>218</v>
       </c>
       <c r="H33" s="3"/>
-      <c r="I33" s="31">
+      <c r="I33" s="30">
         <v>0</v>
       </c>
-      <c r="J33" s="33">
-        <v>999999</v>
-      </c>
-      <c r="K33" s="33" t="s">
-        <v>208</v>
+      <c r="J33" s="30">
+        <v>3000</v>
+      </c>
+      <c r="K33" s="30" t="s">
+        <v>197</v>
       </c>
       <c r="L33" s="27">
         <v>1E+36</v>
@@ -3272,33 +3306,33 @@
       <c r="S33" s="3"/>
       <c r="T33" s="3"/>
     </row>
-    <row r="34" spans="1:20">
-      <c r="A34" s="13" t="s">
-        <v>66</v>
+    <row r="34" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="26" t="s">
+        <v>205</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>102</v>
+      <c r="C34" s="31" t="s">
+        <v>206</v>
       </c>
       <c r="D34" s="22"/>
-      <c r="E34" s="18" t="s">
-        <v>17</v>
+      <c r="E34" s="32" t="s">
+        <v>207</v>
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="3" t="s">
         <v>218</v>
       </c>
       <c r="H34" s="3"/>
-      <c r="I34" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="J34" s="11">
-        <v>38</v>
-      </c>
-      <c r="K34" s="11" t="s">
-        <v>112</v>
+      <c r="I34" s="31">
+        <v>0</v>
+      </c>
+      <c r="J34" s="33">
+        <v>999999</v>
+      </c>
+      <c r="K34" s="33" t="s">
+        <v>208</v>
       </c>
       <c r="L34" s="27">
         <v>1E+36</v>
@@ -3314,19 +3348,19 @@
       <c r="S34" s="3"/>
       <c r="T34" s="3"/>
     </row>
-    <row r="35" spans="1:20">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" s="13" t="s">
-        <v>113</v>
+        <v>66</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>166</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="D35" s="22"/>
-      <c r="E35" s="18">
-        <v>1</v>
+      <c r="E35" s="18" t="s">
+        <v>17</v>
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3" t="s">
@@ -3334,13 +3368,13 @@
       </c>
       <c r="H35" s="3"/>
       <c r="I35" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="J35" s="11" t="s">
-        <v>116</v>
+        <v>13</v>
+      </c>
+      <c r="J35" s="11">
+        <v>38</v>
       </c>
       <c r="K35" s="11" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="L35" s="27">
         <v>1E+36</v>
@@ -3356,33 +3390,33 @@
       <c r="S35" s="3"/>
       <c r="T35" s="3"/>
     </row>
-    <row r="36" spans="1:20">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36" s="13" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>166</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D36" s="22"/>
-      <c r="E36" s="18" t="s">
-        <v>17</v>
+      <c r="E36" s="18">
+        <v>1</v>
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3" t="s">
         <v>218</v>
       </c>
       <c r="H36" s="3"/>
-      <c r="I36" s="11">
-        <v>-2</v>
-      </c>
-      <c r="J36" s="11">
-        <v>32</v>
+      <c r="I36" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="J36" s="11" t="s">
+        <v>116</v>
       </c>
       <c r="K36" s="11" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="L36" s="27">
         <v>1E+36</v>
@@ -3398,15 +3432,15 @@
       <c r="S36" s="3"/>
       <c r="T36" s="3"/>
     </row>
-    <row r="37" spans="1:20">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>166</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D37" s="22"/>
       <c r="E37" s="18" t="s">
@@ -3440,19 +3474,19 @@
       <c r="S37" s="3"/>
       <c r="T37" s="3"/>
     </row>
-    <row r="38" spans="1:20">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" s="13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>166</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D38" s="22"/>
       <c r="E38" s="18" t="s">
-        <v>214</v>
+        <v>17</v>
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3" t="s">
@@ -3460,10 +3494,10 @@
       </c>
       <c r="H38" s="3"/>
       <c r="I38" s="11">
-        <v>33</v>
+        <v>-2</v>
       </c>
       <c r="J38" s="11">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="K38" s="11" t="s">
         <v>112</v>
@@ -3482,15 +3516,15 @@
       <c r="S38" s="3"/>
       <c r="T38" s="3"/>
     </row>
-    <row r="39" spans="1:20">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" s="13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>166</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D39" s="22"/>
       <c r="E39" s="18" t="s">
@@ -3524,19 +3558,19 @@
       <c r="S39" s="3"/>
       <c r="T39" s="3"/>
     </row>
-    <row r="40" spans="1:20">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40" s="13" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>166</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D40" s="22"/>
       <c r="E40" s="18" t="s">
-        <v>128</v>
+        <v>214</v>
       </c>
       <c r="F40" s="3"/>
       <c r="G40" s="3" t="s">
@@ -3544,13 +3578,13 @@
       </c>
       <c r="H40" s="3"/>
       <c r="I40" s="11">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="J40" s="11">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="K40" s="11" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="L40" s="27">
         <v>1E+36</v>
@@ -3566,15 +3600,15 @@
       <c r="S40" s="3"/>
       <c r="T40" s="3"/>
     </row>
-    <row r="41" spans="1:20">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41" s="13" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>166</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D41" s="22"/>
       <c r="E41" s="18" t="s">
@@ -3608,19 +3642,19 @@
       <c r="S41" s="3"/>
       <c r="T41" s="3"/>
     </row>
-    <row r="42" spans="1:20">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42" s="13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>166</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D42" s="22"/>
       <c r="E42" s="18" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3" t="s">
@@ -3628,13 +3662,13 @@
       </c>
       <c r="H42" s="3"/>
       <c r="I42" s="11">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J42" s="11">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="K42" s="11" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="L42" s="27">
         <v>1E+36</v>
@@ -3650,15 +3684,15 @@
       <c r="S42" s="3"/>
       <c r="T42" s="3"/>
     </row>
-    <row r="43" spans="1:20">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" s="13" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>166</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D43" s="22"/>
       <c r="E43" s="18" t="s">
@@ -3692,19 +3726,19 @@
       <c r="S43" s="3"/>
       <c r="T43" s="3"/>
     </row>
-    <row r="44" spans="1:20">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A44" s="13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>166</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D44" s="22"/>
       <c r="E44" s="18" t="s">
-        <v>60</v>
+        <v>134</v>
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3" t="s">
@@ -3715,10 +3749,10 @@
         <v>0</v>
       </c>
       <c r="J44" s="11">
-        <v>450</v>
+        <v>10</v>
       </c>
       <c r="K44" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="L44" s="27">
         <v>1E+36</v>
@@ -3734,15 +3768,15 @@
       <c r="S44" s="3"/>
       <c r="T44" s="3"/>
     </row>
-    <row r="45" spans="1:20">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A45" s="13" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>166</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D45" s="22"/>
       <c r="E45" s="18" t="s">
@@ -3776,19 +3810,19 @@
       <c r="S45" s="3"/>
       <c r="T45" s="3"/>
     </row>
-    <row r="46" spans="1:20">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>166</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D46" s="22"/>
       <c r="E46" s="18" t="s">
-        <v>143</v>
+        <v>60</v>
       </c>
       <c r="F46" s="3"/>
       <c r="G46" s="3" t="s">
@@ -3799,10 +3833,10 @@
         <v>0</v>
       </c>
       <c r="J46" s="11">
-        <v>10</v>
+        <v>450</v>
       </c>
       <c r="K46" s="11" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="L46" s="27">
         <v>1E+36</v>
@@ -3818,15 +3852,15 @@
       <c r="S46" s="3"/>
       <c r="T46" s="3"/>
     </row>
-    <row r="47" spans="1:20">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47" s="13" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>166</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D47" s="22"/>
       <c r="E47" s="18" t="s">
@@ -3860,19 +3894,19 @@
       <c r="S47" s="3"/>
       <c r="T47" s="3"/>
     </row>
-    <row r="48" spans="1:20">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>166</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D48" s="22"/>
       <c r="E48" s="18" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="F48" s="3"/>
       <c r="G48" s="3" t="s">
@@ -3880,13 +3914,13 @@
       </c>
       <c r="H48" s="3"/>
       <c r="I48" s="11">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J48" s="11">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K48" s="11" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="L48" s="27">
         <v>1E+36</v>
@@ -3902,15 +3936,15 @@
       <c r="S48" s="3"/>
       <c r="T48" s="3"/>
     </row>
-    <row r="49" spans="1:20">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A49" s="13" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>166</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D49" s="22"/>
       <c r="E49" s="18" t="s">
@@ -3944,19 +3978,19 @@
       <c r="S49" s="3"/>
       <c r="T49" s="3"/>
     </row>
-    <row r="50" spans="1:20">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50" s="13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>166</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D50" s="22"/>
       <c r="E50" s="18" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="F50" s="3"/>
       <c r="G50" s="3" t="s">
@@ -3964,13 +3998,13 @@
       </c>
       <c r="H50" s="3"/>
       <c r="I50" s="11">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J50" s="11">
-        <v>90</v>
+        <v>1</v>
       </c>
       <c r="K50" s="11" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="L50" s="27">
         <v>1E+36</v>
@@ -3986,115 +4020,119 @@
       <c r="S50" s="3"/>
       <c r="T50" s="3"/>
     </row>
-    <row r="51" spans="1:20">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A51" s="13" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>166</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D51" s="22"/>
       <c r="E51" s="18" t="s">
-        <v>158</v>
+        <v>17</v>
       </c>
       <c r="F51" s="3"/>
       <c r="G51" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="H51" s="3" t="s">
-        <v>47</v>
-      </c>
+      <c r="H51" s="3"/>
       <c r="I51" s="11">
         <v>0</v>
       </c>
       <c r="J51" s="11">
-        <v>40000</v>
+        <v>90</v>
       </c>
       <c r="K51" s="11" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="L51" s="27">
         <v>1E+36</v>
       </c>
       <c r="M51" s="11"/>
       <c r="N51" s="11" t="s">
-        <v>193</v>
+        <v>12</v>
       </c>
       <c r="O51" s="3"/>
       <c r="P51" s="3"/>
       <c r="Q51" s="3"/>
       <c r="R51" s="3"/>
       <c r="S51" s="3"/>
-      <c r="T51" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="52" spans="1:20">
-      <c r="A52" s="14" t="s">
-        <v>209</v>
+      <c r="T51" s="3"/>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A52" s="13" t="s">
+        <v>156</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C52" s="34" t="s">
-        <v>210</v>
+        <v>166</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="D52" s="22"/>
-      <c r="E52" s="18">
-        <v>1</v>
-      </c>
-      <c r="F52" s="34"/>
-      <c r="G52" s="34"/>
-      <c r="H52" s="3"/>
-      <c r="I52" s="34">
+      <c r="E52" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I52" s="11">
         <v>0</v>
       </c>
-      <c r="J52" s="35">
-        <v>999</v>
-      </c>
-      <c r="K52" s="35" t="s">
-        <v>211</v>
-      </c>
-      <c r="L52" s="23">
-        <v>99999</v>
+      <c r="J52" s="11">
+        <v>40000</v>
+      </c>
+      <c r="K52" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="L52" s="27">
+        <v>1E+36</v>
       </c>
       <c r="M52" s="11"/>
-      <c r="N52" s="11"/>
+      <c r="N52" s="11" t="s">
+        <v>193</v>
+      </c>
       <c r="O52" s="3"/>
       <c r="P52" s="3"/>
       <c r="Q52" s="3"/>
       <c r="R52" s="3"/>
       <c r="S52" s="3"/>
-      <c r="T52" s="3"/>
-    </row>
-    <row r="53" spans="1:20">
-      <c r="A53" s="13" t="s">
-        <v>160</v>
+      <c r="T52" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A53" s="14" t="s">
+        <v>209</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C53" s="3" t="s">
-        <v>161</v>
+      <c r="C53" s="34" t="s">
+        <v>210</v>
       </c>
       <c r="D53" s="22"/>
       <c r="E53" s="18">
         <v>1</v>
       </c>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
+      <c r="F53" s="34"/>
+      <c r="G53" s="34"/>
       <c r="H53" s="3"/>
-      <c r="I53" s="11">
-        <v>1</v>
-      </c>
-      <c r="J53" s="11">
-        <v>36</v>
-      </c>
-      <c r="K53" s="11" t="s">
-        <v>162</v>
+      <c r="I53" s="34">
+        <v>0</v>
+      </c>
+      <c r="J53" s="35">
+        <v>999</v>
+      </c>
+      <c r="K53" s="35" t="s">
+        <v>211</v>
       </c>
       <c r="L53" s="23">
         <v>99999</v>
@@ -4108,15 +4146,15 @@
       <c r="S53" s="3"/>
       <c r="T53" s="3"/>
     </row>
-    <row r="54" spans="1:20">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A54" s="13" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>108</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D54" s="22"/>
       <c r="E54" s="18">
@@ -4125,14 +4163,14 @@
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
-      <c r="I54" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="J54" s="11" t="s">
-        <v>165</v>
+      <c r="I54" s="11">
+        <v>1</v>
+      </c>
+      <c r="J54" s="11">
+        <v>36</v>
       </c>
       <c r="K54" s="11" t="s">
-        <v>10</v>
+        <v>162</v>
       </c>
       <c r="L54" s="23">
         <v>99999</v>
@@ -4146,45 +4184,209 @@
       <c r="S54" s="3"/>
       <c r="T54" s="3"/>
     </row>
-    <row r="55" spans="1:20">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A55" s="13" t="s">
-        <v>190</v>
+        <v>163</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>166</v>
+        <v>108</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>191</v>
+        <v>164</v>
       </c>
       <c r="D55" s="22"/>
-      <c r="E55" s="18" t="s">
-        <v>158</v>
+      <c r="E55" s="18">
+        <v>1</v>
       </c>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
-      <c r="I55" s="11">
-        <v>0</v>
-      </c>
-      <c r="J55" s="11">
-        <v>11000</v>
+      <c r="I55" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="J55" s="11" t="s">
+        <v>165</v>
       </c>
       <c r="K55" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="L55" s="27">
-        <v>1E+36</v>
+        <v>10</v>
+      </c>
+      <c r="L55" s="23">
+        <v>99999</v>
       </c>
       <c r="M55" s="11"/>
-      <c r="N55" s="11" t="s">
-        <v>193</v>
-      </c>
+      <c r="N55" s="11"/>
       <c r="O55" s="3"/>
       <c r="P55" s="3"/>
       <c r="Q55" s="3"/>
       <c r="R55" s="3"/>
       <c r="S55" s="3"/>
       <c r="T55" s="3"/>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A56" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D56" s="22"/>
+      <c r="E56" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="11">
+        <v>0</v>
+      </c>
+      <c r="J56" s="11">
+        <v>11000</v>
+      </c>
+      <c r="K56" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="L56" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M56" s="11"/>
+      <c r="N56" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="O56" s="3"/>
+      <c r="P56" s="3"/>
+      <c r="Q56" s="3"/>
+      <c r="R56" s="3"/>
+      <c r="S56" s="3"/>
+      <c r="T56" s="3"/>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A57" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="D57" s="22"/>
+      <c r="E57" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="H57" s="3"/>
+      <c r="I57" s="11">
+        <v>30</v>
+      </c>
+      <c r="J57" s="11">
+        <v>70</v>
+      </c>
+      <c r="K57" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="L57" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M57" s="11"/>
+      <c r="N57" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="O57" s="3"/>
+      <c r="P57" s="3"/>
+      <c r="Q57" s="3"/>
+      <c r="R57" s="3"/>
+      <c r="S57" s="3"/>
+      <c r="T57" s="3"/>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A58" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D58" s="22"/>
+      <c r="E58" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="H58" s="3"/>
+      <c r="I58" s="11">
+        <v>30</v>
+      </c>
+      <c r="J58" s="11">
+        <v>70</v>
+      </c>
+      <c r="K58" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="L58" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M58" s="11"/>
+      <c r="N58" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="O58" s="3"/>
+      <c r="P58" s="3"/>
+      <c r="Q58" s="3"/>
+      <c r="R58" s="3"/>
+      <c r="S58" s="3"/>
+      <c r="T58" s="3"/>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A59" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D59" s="22"/>
+      <c r="E59" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="H59" s="3"/>
+      <c r="I59" s="11">
+        <v>30</v>
+      </c>
+      <c r="J59" s="11">
+        <v>70</v>
+      </c>
+      <c r="K59" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="L59" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M59" s="11"/>
+      <c r="N59" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="O59" s="3"/>
+      <c r="P59" s="3"/>
+      <c r="Q59" s="3"/>
+      <c r="R59" s="3"/>
+      <c r="S59" s="3"/>
+      <c r="T59" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
remove lf from format
</commit_message>
<xml_diff>
--- a/roscop/code_roscop.xlsx
+++ b/roscop/code_roscop.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgrelet\go\src\github.com\jgrelet\oceano2oceansites\roscop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="90" yWindow="15" windowWidth="14505" windowHeight="8415"/>
+    <workbookView xWindow="96" yWindow="12" windowWidth="14508" windowHeight="8412"/>
   </bookViews>
   <sheets>
     <sheet name="code_roscop" sheetId="5" r:id="rId1"/>
@@ -52,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="230">
   <si>
     <t>long_name</t>
   </si>
@@ -87,9 +82,6 @@
     <t>%1d</t>
   </si>
   <si>
-    <t>%6.3lf</t>
-  </si>
-  <si>
     <t>0.001</t>
   </si>
   <si>
@@ -123,9 +115,6 @@
     <t>days since 1950-01-01T00:00:00Z</t>
   </si>
   <si>
-    <t>%7.2lf</t>
-  </si>
-  <si>
     <t>Z</t>
   </si>
   <si>
@@ -180,9 +169,6 @@
     <t>hectoPascal</t>
   </si>
   <si>
-    <t>%6.1lf</t>
-  </si>
-  <si>
     <t>RELH</t>
   </si>
   <si>
@@ -270,9 +256,6 @@
     <t>EWCT</t>
   </si>
   <si>
-    <t>%7.3lf</t>
-  </si>
-  <si>
     <t>0.01</t>
   </si>
   <si>
@@ -285,12 +268,6 @@
     <t>WMSP</t>
   </si>
   <si>
-    <t>%5.1lf</t>
-  </si>
-  <si>
-    <t>%8.3lf</t>
-  </si>
-  <si>
     <t>cm/second</t>
   </si>
   <si>
@@ -306,15 +283,9 @@
     <t>milligram/m3</t>
   </si>
   <si>
-    <t>%8.4lf</t>
-  </si>
-  <si>
     <t>TUR3</t>
   </si>
   <si>
-    <t>%6.2lf</t>
-  </si>
-  <si>
     <t>PRLF</t>
   </si>
   <si>
@@ -757,17 +728,26 @@
   </si>
   <si>
     <t xml:space="preserve">electrical conductivity </t>
+  </si>
+  <si>
+    <t>%7.2f</t>
+  </si>
+  <si>
+    <t>%8.4f</t>
+  </si>
+  <si>
+    <t>%6.2f</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0E+00"/>
     <numFmt numFmtId="165" formatCode="0.E+00"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="27">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1569,7 +1549,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1601,10 +1581,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1636,7 +1615,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1812,42 +1790,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="D17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C57" sqref="C57"/>
+      <selection pane="bottomRight" activeCell="K30" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="13"/>
+    <col min="1" max="1" width="11.5546875" style="13"/>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="34.85546875" customWidth="1"/>
-    <col min="4" max="4" width="28.85546875" style="21" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" style="17" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
-    <col min="7" max="7" width="32.85546875" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" customWidth="1"/>
-    <col min="9" max="9" width="7.5703125" style="6" customWidth="1"/>
-    <col min="10" max="10" width="8.140625" style="6" customWidth="1"/>
-    <col min="11" max="11" width="7.42578125" style="6" customWidth="1"/>
-    <col min="12" max="12" width="7.85546875" style="10" customWidth="1"/>
-    <col min="13" max="13" width="5.7109375" style="6" customWidth="1"/>
-    <col min="14" max="14" width="8.5703125" style="6" customWidth="1"/>
-    <col min="15" max="15" width="34.140625" customWidth="1"/>
-    <col min="16" max="16" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="34.88671875" customWidth="1"/>
+    <col min="4" max="4" width="28.88671875" style="21" customWidth="1"/>
+    <col min="5" max="5" width="24.109375" style="17" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" customWidth="1"/>
+    <col min="7" max="7" width="32.88671875" customWidth="1"/>
+    <col min="8" max="8" width="6.109375" customWidth="1"/>
+    <col min="9" max="9" width="7.5546875" style="6" customWidth="1"/>
+    <col min="10" max="10" width="8.109375" style="6" customWidth="1"/>
+    <col min="11" max="11" width="7.44140625" style="6" customWidth="1"/>
+    <col min="12" max="12" width="7.88671875" style="10" customWidth="1"/>
+    <col min="13" max="13" width="5.6640625" style="6" customWidth="1"/>
+    <col min="14" max="14" width="8.5546875" style="6" customWidth="1"/>
+    <col min="15" max="15" width="34.109375" customWidth="1"/>
+    <col min="16" max="16" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21">
       <c r="A1" s="15" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C1" s="19" t="s">
         <v>0</v>
@@ -1862,10 +1840,10 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>4</v>
@@ -1877,7 +1855,7 @@
         <v>6</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>7</v>
@@ -1889,94 +1867,94 @@
         <v>9</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="T1" s="7" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="U1" s="8"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21">
       <c r="A2" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U2" s="2"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21">
       <c r="A3" s="13" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="18">
@@ -1988,7 +1966,7 @@
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
       <c r="K3" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="L3" s="23">
         <v>99999</v>
@@ -1996,7 +1974,7 @@
       <c r="M3" s="11"/>
       <c r="N3" s="11"/>
       <c r="O3" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
@@ -2004,15 +1982,15 @@
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21">
       <c r="A4" s="13" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D4" s="22"/>
       <c r="E4" s="18">
@@ -2024,7 +2002,7 @@
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
       <c r="K4" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="L4" s="23">
         <v>99999</v>
@@ -2032,7 +2010,7 @@
       <c r="M4" s="11"/>
       <c r="N4" s="11"/>
       <c r="O4" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
@@ -2040,21 +2018,21 @@
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21">
       <c r="A5" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D5" s="22" t="s">
         <v>166</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>174</v>
-      </c>
       <c r="E5" s="18" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -2064,7 +2042,7 @@
       <c r="K5" s="11"/>
       <c r="L5" s="27"/>
       <c r="M5" s="11" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="N5" s="11"/>
       <c r="O5" s="3"/>
@@ -2072,27 +2050,27 @@
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
       <c r="S5" s="3" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
       <c r="A6" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -2102,7 +2080,7 @@
       <c r="K6" s="11"/>
       <c r="L6" s="27"/>
       <c r="M6" s="11" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="N6" s="11"/>
       <c r="O6" s="3"/>
@@ -2110,30 +2088,30 @@
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
       <c r="S6" s="3" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="15" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="15">
       <c r="A7" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F7" s="36" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="24"/>
@@ -2144,11 +2122,11 @@
         <v>90000</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="L7" s="27"/>
       <c r="M7" s="11" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="N7" s="11"/>
       <c r="O7" s="3"/>
@@ -2158,15 +2136,15 @@
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21">
       <c r="A8" s="13" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="D8" s="22"/>
       <c r="E8" s="18">
@@ -2182,7 +2160,7 @@
         <v>90000</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="L8" s="27"/>
       <c r="M8" s="11"/>
@@ -2194,26 +2172,26 @@
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21">
       <c r="A9" s="13" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I9" s="11">
         <v>0</v>
@@ -2222,13 +2200,13 @@
         <v>9000</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>23</v>
+        <v>227</v>
       </c>
       <c r="L9" s="27">
         <v>1E+36</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="N9" s="11"/>
       <c r="O9" s="3"/>
@@ -2237,28 +2215,28 @@
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
       <c r="T9" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
       <c r="A10" s="13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="11">
@@ -2268,7 +2246,7 @@
         <v>9000</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>23</v>
+        <v>227</v>
       </c>
       <c r="L10" s="27">
         <v>1E+36</v>
@@ -2276,7 +2254,7 @@
       <c r="M10" s="11"/>
       <c r="N10" s="11"/>
       <c r="O10" s="3" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
@@ -2284,45 +2262,45 @@
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21">
       <c r="A11" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J11" s="11">
         <v>38</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>11</v>
+        <v>104</v>
       </c>
       <c r="L11" s="27">
         <v>1E+36</v>
       </c>
       <c r="M11" s="11"/>
       <c r="N11" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
@@ -2330,45 +2308,45 @@
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21">
       <c r="A12" s="13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E12" s="18">
         <v>1</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J12" s="11">
         <v>38</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>11</v>
+        <v>104</v>
       </c>
       <c r="L12" s="27">
         <v>1E+36</v>
       </c>
       <c r="M12" s="11"/>
       <c r="N12" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
@@ -2376,23 +2354,23 @@
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21">
       <c r="A13" s="13" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="D13" s="22"/>
       <c r="E13" s="18" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="11">
@@ -2402,14 +2380,14 @@
         <v>70</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>11</v>
+        <v>104</v>
       </c>
       <c r="L13" s="27">
         <v>1E+36</v>
       </c>
       <c r="M13" s="11"/>
       <c r="N13" s="11" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
@@ -2418,45 +2396,45 @@
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21">
       <c r="A14" s="13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J14" s="11">
         <v>38</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>11</v>
+        <v>104</v>
       </c>
       <c r="L14" s="27">
         <v>1E+36</v>
       </c>
       <c r="M14" s="11"/>
       <c r="N14" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
@@ -2464,45 +2442,45 @@
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21">
       <c r="A15" s="13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J15" s="11">
         <v>38</v>
       </c>
       <c r="K15" s="11" t="s">
-        <v>11</v>
+        <v>104</v>
       </c>
       <c r="L15" s="27">
         <v>1E+36</v>
       </c>
       <c r="M15" s="11"/>
       <c r="N15" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
@@ -2510,25 +2488,25 @@
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21">
       <c r="A16" s="13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="11">
@@ -2538,17 +2516,17 @@
         <v>1600</v>
       </c>
       <c r="K16" s="11" t="s">
-        <v>23</v>
+        <v>227</v>
       </c>
       <c r="L16" s="27">
         <v>1E+36</v>
       </c>
       <c r="M16" s="11"/>
       <c r="N16" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
@@ -2556,45 +2534,45 @@
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20">
       <c r="A17" s="13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J17" s="11">
         <v>38</v>
       </c>
       <c r="K17" s="11" t="s">
-        <v>11</v>
+        <v>104</v>
       </c>
       <c r="L17" s="27">
         <v>1E+36</v>
       </c>
       <c r="M17" s="11"/>
       <c r="N17" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
@@ -2602,25 +2580,25 @@
       <c r="S17" s="3"/>
       <c r="T17" s="3"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20">
       <c r="A18" s="13" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="11">
@@ -2630,17 +2608,17 @@
         <v>200</v>
       </c>
       <c r="K18" s="11" t="s">
-        <v>11</v>
+        <v>104</v>
       </c>
       <c r="L18" s="27">
         <v>1E+36</v>
       </c>
       <c r="M18" s="11"/>
       <c r="N18" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
@@ -2648,25 +2626,25 @@
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20">
       <c r="A19" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="18" t="s">
         <v>36</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D19" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>38</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="11">
@@ -2676,17 +2654,17 @@
         <v>360</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>77</v>
+        <v>147</v>
       </c>
       <c r="L19" s="27">
         <v>1E+36</v>
       </c>
       <c r="M19" s="11"/>
       <c r="N19" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
@@ -2694,25 +2672,25 @@
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20">
       <c r="A20" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="18" t="s">
         <v>39</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D20" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>41</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="11">
@@ -2722,17 +2700,17 @@
         <v>1030</v>
       </c>
       <c r="K20" s="11" t="s">
-        <v>78</v>
+        <v>189</v>
       </c>
       <c r="L20" s="27">
         <v>1E+36</v>
       </c>
       <c r="M20" s="11"/>
       <c r="N20" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
@@ -2740,25 +2718,25 @@
       <c r="S20" s="3"/>
       <c r="T20" s="3"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20">
       <c r="A21" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="18" t="s">
         <v>43</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D21" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="E21" s="18" t="s">
-        <v>46</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="11">
@@ -2768,17 +2746,17 @@
         <v>100</v>
       </c>
       <c r="K21" s="11" t="s">
-        <v>42</v>
+        <v>184</v>
       </c>
       <c r="L21" s="27">
         <v>1E+36</v>
       </c>
       <c r="M21" s="11"/>
       <c r="N21" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O21" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
@@ -2786,23 +2764,23 @@
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20">
       <c r="A22" s="13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D22" s="22"/>
       <c r="E22" s="18" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="11">
@@ -2812,17 +2790,17 @@
         <v>100</v>
       </c>
       <c r="K22" s="11" t="s">
-        <v>72</v>
+        <v>131</v>
       </c>
       <c r="L22" s="27">
         <v>1E+36</v>
       </c>
       <c r="M22" s="11"/>
       <c r="N22" s="11" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="P22" s="3"/>
       <c r="Q22" s="3"/>
@@ -2830,23 +2808,23 @@
       <c r="S22" s="3"/>
       <c r="T22" s="3"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20">
       <c r="A23" s="13" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D23" s="22"/>
       <c r="E23" s="18" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="11">
@@ -2856,17 +2834,17 @@
         <v>100</v>
       </c>
       <c r="K23" s="11" t="s">
-        <v>72</v>
+        <v>131</v>
       </c>
       <c r="L23" s="27">
         <v>1E+36</v>
       </c>
       <c r="M23" s="11"/>
       <c r="N23" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O23" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
@@ -2874,45 +2852,45 @@
       <c r="S23" s="3"/>
       <c r="T23" s="3"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20">
       <c r="A24" s="13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J24" s="11">
         <v>38</v>
       </c>
       <c r="K24" s="11" t="s">
-        <v>11</v>
+        <v>104</v>
       </c>
       <c r="L24" s="27">
         <v>1E+36</v>
       </c>
       <c r="M24" s="11"/>
       <c r="N24" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O24" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
@@ -2920,45 +2898,45 @@
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20">
       <c r="A25" s="13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H25" s="3"/>
       <c r="I25" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J25" s="11">
         <v>38</v>
       </c>
       <c r="K25" s="11" t="s">
-        <v>11</v>
+        <v>104</v>
       </c>
       <c r="L25" s="27">
         <v>1E+36</v>
       </c>
       <c r="M25" s="11"/>
       <c r="N25" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O25" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
@@ -2966,45 +2944,45 @@
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20">
       <c r="A26" s="13" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H26" s="3"/>
       <c r="I26" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J26" s="11">
         <v>38</v>
       </c>
       <c r="K26" s="11" t="s">
-        <v>11</v>
+        <v>104</v>
       </c>
       <c r="L26" s="27">
         <v>1E+36</v>
       </c>
       <c r="M26" s="11"/>
       <c r="N26" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O26" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
@@ -3012,23 +2990,23 @@
       <c r="S26" s="3"/>
       <c r="T26" s="3"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20">
       <c r="A27" s="13" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D27" s="22"/>
       <c r="E27" s="18" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H27" s="3"/>
       <c r="I27" s="11">
@@ -3038,14 +3016,14 @@
         <v>700</v>
       </c>
       <c r="K27" s="11" t="s">
-        <v>72</v>
+        <v>131</v>
       </c>
       <c r="L27" s="27">
         <v>1E+36</v>
       </c>
       <c r="M27" s="11"/>
       <c r="N27" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
@@ -3054,23 +3032,23 @@
       <c r="S27" s="3"/>
       <c r="T27" s="3"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20">
       <c r="A28" s="13" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="18" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H28" s="3"/>
       <c r="I28" s="11">
@@ -3080,14 +3058,14 @@
         <v>1</v>
       </c>
       <c r="K28" s="11" t="s">
-        <v>84</v>
+        <v>228</v>
       </c>
       <c r="L28" s="27">
         <v>1E+36</v>
       </c>
       <c r="M28" s="11"/>
       <c r="N28" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O28" s="3"/>
       <c r="P28" s="3"/>
@@ -3096,23 +3074,23 @@
       <c r="S28" s="3"/>
       <c r="T28" s="3"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20">
       <c r="A29" s="25" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="D29" s="22"/>
       <c r="E29" s="29" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H29" s="3"/>
       <c r="I29" s="30">
@@ -3122,14 +3100,14 @@
         <v>10</v>
       </c>
       <c r="K29" s="30" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="L29" s="27">
         <v>1E+36</v>
       </c>
       <c r="M29" s="11"/>
       <c r="N29" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
@@ -3138,23 +3116,23 @@
       <c r="S29" s="3"/>
       <c r="T29" s="3"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20">
       <c r="A30" s="13" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="18" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H30" s="3"/>
       <c r="I30" s="11">
@@ -3164,14 +3142,14 @@
         <v>100</v>
       </c>
       <c r="K30" s="11" t="s">
-        <v>86</v>
+        <v>229</v>
       </c>
       <c r="L30" s="27">
         <v>1E+36</v>
       </c>
       <c r="M30" s="11"/>
       <c r="N30" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O30" s="3"/>
       <c r="P30" s="3"/>
@@ -3180,23 +3158,23 @@
       <c r="S30" s="3"/>
       <c r="T30" s="3"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20">
       <c r="A31" s="25" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="18" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H31" s="3"/>
       <c r="I31" s="30">
@@ -3206,14 +3184,14 @@
         <v>3000</v>
       </c>
       <c r="K31" s="30" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="L31" s="27">
         <v>1E+36</v>
       </c>
       <c r="M31" s="11"/>
       <c r="N31" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O31" s="3"/>
       <c r="P31" s="3"/>
@@ -3222,23 +3200,23 @@
       <c r="S31" s="3"/>
       <c r="T31" s="3"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20">
       <c r="A32" s="25" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="D32" s="22"/>
       <c r="E32" s="18" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H32" s="3"/>
       <c r="I32" s="30">
@@ -3248,14 +3226,14 @@
         <v>4000</v>
       </c>
       <c r="K32" s="30" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="L32" s="27">
         <v>1E+36</v>
       </c>
       <c r="M32" s="11"/>
       <c r="N32" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O32" s="3"/>
       <c r="P32" s="3"/>
@@ -3264,23 +3242,23 @@
       <c r="S32" s="3"/>
       <c r="T32" s="3"/>
     </row>
-    <row r="33" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:20" ht="12.6" customHeight="1">
       <c r="A33" s="25" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="D33" s="22"/>
       <c r="E33" s="18" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="30">
@@ -3290,14 +3268,14 @@
         <v>3000</v>
       </c>
       <c r="K33" s="30" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="L33" s="27">
         <v>1E+36</v>
       </c>
       <c r="M33" s="11"/>
       <c r="N33" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
@@ -3306,23 +3284,23 @@
       <c r="S33" s="3"/>
       <c r="T33" s="3"/>
     </row>
-    <row r="34" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:20" ht="12.6" customHeight="1">
       <c r="A34" s="26" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="D34" s="22"/>
       <c r="E34" s="32" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H34" s="3"/>
       <c r="I34" s="31">
@@ -3332,14 +3310,14 @@
         <v>999999</v>
       </c>
       <c r="K34" s="33" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="L34" s="27">
         <v>1E+36</v>
       </c>
       <c r="M34" s="11"/>
       <c r="N34" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O34" s="3"/>
       <c r="P34" s="3"/>
@@ -3348,40 +3326,40 @@
       <c r="S34" s="3"/>
       <c r="T34" s="3"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:20">
       <c r="A35" s="13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D35" s="22"/>
       <c r="E35" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H35" s="3"/>
       <c r="I35" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J35" s="11">
         <v>38</v>
       </c>
       <c r="K35" s="11" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="L35" s="27">
         <v>1E+36</v>
       </c>
       <c r="M35" s="11"/>
       <c r="N35" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O35" s="3"/>
       <c r="P35" s="3"/>
@@ -3390,15 +3368,15 @@
       <c r="S35" s="3"/>
       <c r="T35" s="3"/>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:20">
       <c r="A36" s="13" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D36" s="22"/>
       <c r="E36" s="18">
@@ -3406,24 +3384,24 @@
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H36" s="3"/>
       <c r="I36" s="11" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="J36" s="11" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="K36" s="11" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="L36" s="27">
         <v>1E+36</v>
       </c>
       <c r="M36" s="11"/>
       <c r="N36" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O36" s="3"/>
       <c r="P36" s="3"/>
@@ -3432,23 +3410,23 @@
       <c r="S36" s="3"/>
       <c r="T36" s="3"/>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:20">
       <c r="A37" s="13" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D37" s="22"/>
       <c r="E37" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F37" s="3"/>
       <c r="G37" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H37" s="3"/>
       <c r="I37" s="11">
@@ -3458,14 +3436,14 @@
         <v>32</v>
       </c>
       <c r="K37" s="11" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="L37" s="27">
         <v>1E+36</v>
       </c>
       <c r="M37" s="11"/>
       <c r="N37" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O37" s="3"/>
       <c r="P37" s="3"/>
@@ -3474,23 +3452,23 @@
       <c r="S37" s="3"/>
       <c r="T37" s="3"/>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:20">
       <c r="A38" s="13" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D38" s="22"/>
       <c r="E38" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H38" s="3"/>
       <c r="I38" s="11">
@@ -3500,14 +3478,14 @@
         <v>32</v>
       </c>
       <c r="K38" s="11" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="L38" s="27">
         <v>1E+36</v>
       </c>
       <c r="M38" s="11"/>
       <c r="N38" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O38" s="3"/>
       <c r="P38" s="3"/>
@@ -3516,23 +3494,23 @@
       <c r="S38" s="3"/>
       <c r="T38" s="3"/>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:20">
       <c r="A39" s="13" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D39" s="22"/>
       <c r="E39" s="18" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H39" s="3"/>
       <c r="I39" s="11">
@@ -3542,14 +3520,14 @@
         <v>37</v>
       </c>
       <c r="K39" s="11" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="L39" s="27">
         <v>1E+36</v>
       </c>
       <c r="M39" s="11"/>
       <c r="N39" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O39" s="3"/>
       <c r="P39" s="3"/>
@@ -3558,23 +3536,23 @@
       <c r="S39" s="3"/>
       <c r="T39" s="3"/>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:20">
       <c r="A40" s="13" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="D40" s="22"/>
       <c r="E40" s="18" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="F40" s="3"/>
       <c r="G40" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H40" s="3"/>
       <c r="I40" s="11">
@@ -3584,14 +3562,14 @@
         <v>37</v>
       </c>
       <c r="K40" s="11" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="L40" s="27">
         <v>1E+36</v>
       </c>
       <c r="M40" s="11"/>
       <c r="N40" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O40" s="3"/>
       <c r="P40" s="3"/>
@@ -3600,23 +3578,23 @@
       <c r="S40" s="3"/>
       <c r="T40" s="3"/>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:20">
       <c r="A41" s="13" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="D41" s="22"/>
       <c r="E41" s="18" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H41" s="3"/>
       <c r="I41" s="11">
@@ -3626,14 +3604,14 @@
         <v>7</v>
       </c>
       <c r="K41" s="11" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="L41" s="27">
         <v>1E+36</v>
       </c>
       <c r="M41" s="11"/>
       <c r="N41" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O41" s="3"/>
       <c r="P41" s="3"/>
@@ -3642,23 +3620,23 @@
       <c r="S41" s="3"/>
       <c r="T41" s="3"/>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:20">
       <c r="A42" s="13" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="D42" s="22"/>
       <c r="E42" s="18" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H42" s="3"/>
       <c r="I42" s="11">
@@ -3668,14 +3646,14 @@
         <v>7</v>
       </c>
       <c r="K42" s="11" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="L42" s="27">
         <v>1E+36</v>
       </c>
       <c r="M42" s="11"/>
       <c r="N42" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O42" s="3"/>
       <c r="P42" s="3"/>
@@ -3684,23 +3662,23 @@
       <c r="S42" s="3"/>
       <c r="T42" s="3"/>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:20">
       <c r="A43" s="13" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="D43" s="22"/>
       <c r="E43" s="18" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="F43" s="3"/>
       <c r="G43" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H43" s="3"/>
       <c r="I43" s="11">
@@ -3710,14 +3688,14 @@
         <v>10</v>
       </c>
       <c r="K43" s="11" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="L43" s="27">
         <v>1E+36</v>
       </c>
       <c r="M43" s="11"/>
       <c r="N43" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O43" s="3"/>
       <c r="P43" s="3"/>
@@ -3726,23 +3704,23 @@
       <c r="S43" s="3"/>
       <c r="T43" s="3"/>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:20">
       <c r="A44" s="13" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="D44" s="22"/>
       <c r="E44" s="18" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H44" s="3"/>
       <c r="I44" s="11">
@@ -3752,14 +3730,14 @@
         <v>10</v>
       </c>
       <c r="K44" s="11" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="L44" s="27">
         <v>1E+36</v>
       </c>
       <c r="M44" s="11"/>
       <c r="N44" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O44" s="3"/>
       <c r="P44" s="3"/>
@@ -3768,23 +3746,23 @@
       <c r="S44" s="3"/>
       <c r="T44" s="3"/>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:20">
       <c r="A45" s="13" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="D45" s="22"/>
       <c r="E45" s="18" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F45" s="3"/>
       <c r="G45" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H45" s="3"/>
       <c r="I45" s="11">
@@ -3794,14 +3772,14 @@
         <v>450</v>
       </c>
       <c r="K45" s="11" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="L45" s="27">
         <v>1E+36</v>
       </c>
       <c r="M45" s="11"/>
       <c r="N45" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O45" s="3"/>
       <c r="P45" s="3"/>
@@ -3810,23 +3788,23 @@
       <c r="S45" s="3"/>
       <c r="T45" s="3"/>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:20">
       <c r="A46" s="13" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="D46" s="22"/>
       <c r="E46" s="18" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F46" s="3"/>
       <c r="G46" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H46" s="3"/>
       <c r="I46" s="11">
@@ -3836,14 +3814,14 @@
         <v>450</v>
       </c>
       <c r="K46" s="11" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="L46" s="27">
         <v>1E+36</v>
       </c>
       <c r="M46" s="11"/>
       <c r="N46" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O46" s="3"/>
       <c r="P46" s="3"/>
@@ -3852,23 +3830,23 @@
       <c r="S46" s="3"/>
       <c r="T46" s="3"/>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:20">
       <c r="A47" s="13" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="D47" s="22"/>
       <c r="E47" s="18" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H47" s="3"/>
       <c r="I47" s="11">
@@ -3878,14 +3856,14 @@
         <v>10</v>
       </c>
       <c r="K47" s="11" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="L47" s="27">
         <v>1E+36</v>
       </c>
       <c r="M47" s="11"/>
       <c r="N47" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O47" s="3"/>
       <c r="P47" s="3"/>
@@ -3894,23 +3872,23 @@
       <c r="S47" s="3"/>
       <c r="T47" s="3"/>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:20">
       <c r="A48" s="13" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="D48" s="22"/>
       <c r="E48" s="18" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="F48" s="3"/>
       <c r="G48" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H48" s="3"/>
       <c r="I48" s="11">
@@ -3920,14 +3898,14 @@
         <v>10</v>
       </c>
       <c r="K48" s="11" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="L48" s="27">
         <v>1E+36</v>
       </c>
       <c r="M48" s="11"/>
       <c r="N48" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O48" s="3"/>
       <c r="P48" s="3"/>
@@ -3936,23 +3914,23 @@
       <c r="S48" s="3"/>
       <c r="T48" s="3"/>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:20">
       <c r="A49" s="13" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="D49" s="22"/>
       <c r="E49" s="18" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="F49" s="3"/>
       <c r="G49" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H49" s="3"/>
       <c r="I49" s="11">
@@ -3962,14 +3940,14 @@
         <v>1</v>
       </c>
       <c r="K49" s="11" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="L49" s="27">
         <v>1E+36</v>
       </c>
       <c r="M49" s="11"/>
       <c r="N49" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O49" s="3"/>
       <c r="P49" s="3"/>
@@ -3978,23 +3956,23 @@
       <c r="S49" s="3"/>
       <c r="T49" s="3"/>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:20">
       <c r="A50" s="13" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="D50" s="22"/>
       <c r="E50" s="18" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="F50" s="3"/>
       <c r="G50" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H50" s="3"/>
       <c r="I50" s="11">
@@ -4004,14 +3982,14 @@
         <v>1</v>
       </c>
       <c r="K50" s="11" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="L50" s="27">
         <v>1E+36</v>
       </c>
       <c r="M50" s="11"/>
       <c r="N50" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O50" s="3"/>
       <c r="P50" s="3"/>
@@ -4020,23 +3998,23 @@
       <c r="S50" s="3"/>
       <c r="T50" s="3"/>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:20">
       <c r="A51" s="13" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D51" s="22"/>
       <c r="E51" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F51" s="3"/>
       <c r="G51" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H51" s="3"/>
       <c r="I51" s="11">
@@ -4046,14 +4024,14 @@
         <v>90</v>
       </c>
       <c r="K51" s="11" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="L51" s="27">
         <v>1E+36</v>
       </c>
       <c r="M51" s="11"/>
       <c r="N51" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O51" s="3"/>
       <c r="P51" s="3"/>
@@ -4062,26 +4040,26 @@
       <c r="S51" s="3"/>
       <c r="T51" s="3"/>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:20">
       <c r="A52" s="13" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D52" s="22"/>
       <c r="E52" s="18" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="F52" s="3"/>
       <c r="G52" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I52" s="11">
         <v>0</v>
@@ -4090,14 +4068,14 @@
         <v>40000</v>
       </c>
       <c r="K52" s="11" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="L52" s="27">
         <v>1E+36</v>
       </c>
       <c r="M52" s="11"/>
       <c r="N52" s="11" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="O52" s="3"/>
       <c r="P52" s="3"/>
@@ -4105,18 +4083,18 @@
       <c r="R52" s="3"/>
       <c r="S52" s="3"/>
       <c r="T52" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20">
       <c r="A53" s="14" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C53" s="34" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D53" s="22"/>
       <c r="E53" s="18">
@@ -4132,7 +4110,7 @@
         <v>999</v>
       </c>
       <c r="K53" s="35" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="L53" s="23">
         <v>99999</v>
@@ -4146,15 +4124,15 @@
       <c r="S53" s="3"/>
       <c r="T53" s="3"/>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:20">
       <c r="A54" s="13" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="D54" s="22"/>
       <c r="E54" s="18">
@@ -4170,7 +4148,7 @@
         <v>36</v>
       </c>
       <c r="K54" s="11" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="L54" s="23">
         <v>99999</v>
@@ -4184,15 +4162,15 @@
       <c r="S54" s="3"/>
       <c r="T54" s="3"/>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:20">
       <c r="A55" s="13" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="D55" s="22"/>
       <c r="E55" s="18">
@@ -4202,10 +4180,10 @@
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
       <c r="I55" s="11" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="J55" s="11" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="K55" s="11" t="s">
         <v>10</v>
@@ -4222,19 +4200,19 @@
       <c r="S55" s="3"/>
       <c r="T55" s="3"/>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:20">
       <c r="A56" s="13" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="D56" s="22"/>
       <c r="E56" s="18" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
@@ -4246,14 +4224,14 @@
         <v>11000</v>
       </c>
       <c r="K56" s="11" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="L56" s="27">
         <v>1E+36</v>
       </c>
       <c r="M56" s="11"/>
       <c r="N56" s="11" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="O56" s="3"/>
       <c r="P56" s="3"/>
@@ -4262,23 +4240,23 @@
       <c r="S56" s="3"/>
       <c r="T56" s="3"/>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:20">
       <c r="A57" s="13" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="D57" s="22"/>
       <c r="E57" s="18" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="F57" s="3"/>
       <c r="G57" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H57" s="3"/>
       <c r="I57" s="11">
@@ -4288,14 +4266,14 @@
         <v>70</v>
       </c>
       <c r="K57" s="11" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="L57" s="27">
         <v>1E+36</v>
       </c>
       <c r="M57" s="11"/>
       <c r="N57" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O57" s="3"/>
       <c r="P57" s="3"/>
@@ -4304,23 +4282,23 @@
       <c r="S57" s="3"/>
       <c r="T57" s="3"/>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:20">
       <c r="A58" s="13" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="D58" s="22"/>
       <c r="E58" s="18" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="F58" s="3"/>
       <c r="G58" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H58" s="3"/>
       <c r="I58" s="11">
@@ -4330,14 +4308,14 @@
         <v>70</v>
       </c>
       <c r="K58" s="11" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="L58" s="27">
         <v>1E+36</v>
       </c>
       <c r="M58" s="11"/>
       <c r="N58" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O58" s="3"/>
       <c r="P58" s="3"/>
@@ -4346,23 +4324,23 @@
       <c r="S58" s="3"/>
       <c r="T58" s="3"/>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:20">
       <c r="A59" s="13" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="D59" s="22"/>
       <c r="E59" s="18" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="F59" s="3"/>
       <c r="G59" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H59" s="3"/>
       <c r="I59" s="11">
@@ -4372,14 +4350,14 @@
         <v>70</v>
       </c>
       <c r="K59" s="11" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="L59" s="27">
         <v>1E+36</v>
       </c>
       <c r="M59" s="11"/>
       <c r="N59" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O59" s="3"/>
       <c r="P59" s="3"/>

</xml_diff>

<commit_message>
update file with new physical parameters
</commit_message>
<xml_diff>
--- a/roscop/code_roscop.xlsx
+++ b/roscop/code_roscop.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="261">
   <si>
     <t>long_name</t>
   </si>
@@ -703,12 +703,6 @@
     <t>_FillValue</t>
   </si>
   <si>
-    <t>COND1</t>
-  </si>
-  <si>
-    <t>COND2</t>
-  </si>
-  <si>
     <t>mS/cm</t>
   </si>
   <si>
@@ -724,12 +718,6 @@
     <t>0.002</t>
   </si>
   <si>
-    <t>COND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">electrical conductivity </t>
-  </si>
-  <si>
     <t>%7.2f</t>
   </si>
   <si>
@@ -737,6 +725,111 @@
   </si>
   <si>
     <t>%6.2f</t>
+  </si>
+  <si>
+    <t>LGH5</t>
+  </si>
+  <si>
+    <t>immerged/surf irradiance ratio</t>
+  </si>
+  <si>
+    <t>DOX1</t>
+  </si>
+  <si>
+    <t>volume_fraction_of_oxygen_in_sea_water</t>
+  </si>
+  <si>
+    <t>Ocean oxygen in ml per liter</t>
+  </si>
+  <si>
+    <t>DEPH</t>
+  </si>
+  <si>
+    <t>TUR2</t>
+  </si>
+  <si>
+    <t>LINC</t>
+  </si>
+  <si>
+    <t>long wave incoming radiation</t>
+  </si>
+  <si>
+    <t>%+5.1f</t>
+  </si>
+  <si>
+    <t>light attenuation coefficient</t>
+  </si>
+  <si>
+    <t>NTRI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nitrite (no2-n) </t>
+  </si>
+  <si>
+    <t>millimole/m3</t>
+  </si>
+  <si>
+    <t>NTIW</t>
+  </si>
+  <si>
+    <t>moles_of_nitrite_per_unit_mass_in_sea_water</t>
+  </si>
+  <si>
+    <t>moles_concentration_of_nitrite_in_sea_water</t>
+  </si>
+  <si>
+    <t>NTZW</t>
+  </si>
+  <si>
+    <t>NTRZ</t>
+  </si>
+  <si>
+    <t>nitrate + nitrite</t>
+  </si>
+  <si>
+    <t>moles_concentration_of_nitrate_and_nitrite_in_sea_water</t>
+  </si>
+  <si>
+    <t>moles_of_nitrate_and_nitrite_per_unit_mass_in_sea_water</t>
+  </si>
+  <si>
+    <t>NTAW</t>
+  </si>
+  <si>
+    <t>NTRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nitrate (no3-n) </t>
+  </si>
+  <si>
+    <t>moles_of_nitrate_per_unit_mass_in_sea_water</t>
+  </si>
+  <si>
+    <t>moles_concentration_of_nitrate_in_sea_water</t>
+  </si>
+  <si>
+    <t>PHOW</t>
+  </si>
+  <si>
+    <t>PHOS</t>
+  </si>
+  <si>
+    <t>phosphate (po4-p)</t>
+  </si>
+  <si>
+    <t>moles_of_phosphate_per_unit_mass_in_sea_water</t>
+  </si>
+  <si>
+    <t>moles_phosphate_of_nitrate_in_sea_water</t>
+  </si>
+  <si>
+    <t>PHPT</t>
+  </si>
+  <si>
+    <t>total pheophytin</t>
+  </si>
+  <si>
+    <t>milligramm/m3</t>
   </si>
 </sst>
 </file>
@@ -1791,13 +1884,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U59"/>
+  <dimension ref="A1:U71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="D17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="H34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K30" sqref="K1:K1048576"/>
+      <selection pane="bottomRight" activeCell="K58" sqref="K58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
@@ -2174,7 +2267,7 @@
     </row>
     <row r="9" spans="1:21">
       <c r="A9" s="13" t="s">
-        <v>103</v>
+        <v>231</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>158</v>
@@ -2200,7 +2293,7 @@
         <v>9000</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="L9" s="27">
         <v>1E+36</v>
@@ -2220,25 +2313,25 @@
     </row>
     <row r="10" spans="1:21">
       <c r="A10" s="13" t="s">
-        <v>45</v>
+        <v>103</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>46</v>
+        <v>181</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>211</v>
+        <v>150</v>
       </c>
       <c r="F10" s="3"/>
-      <c r="G10" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="I10" s="11">
         <v>0</v>
       </c>
@@ -2246,61 +2339,61 @@
         <v>9000</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="L10" s="27">
         <v>1E+36</v>
       </c>
-      <c r="M10" s="11"/>
+      <c r="M10" s="11" t="s">
+        <v>22</v>
+      </c>
       <c r="N10" s="11"/>
-      <c r="O10" s="3" t="s">
-        <v>212</v>
-      </c>
+      <c r="O10" s="3"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
       <c r="S10" s="3"/>
-      <c r="T10" s="3"/>
+      <c r="T10" s="3" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="11" spans="1:21">
       <c r="A11" s="13" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>23</v>
+        <v>204</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>16</v>
+        <v>211</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
         <v>210</v>
       </c>
       <c r="H11" s="3"/>
-      <c r="I11" s="11" t="s">
-        <v>12</v>
+      <c r="I11" s="11">
+        <v>0</v>
       </c>
       <c r="J11" s="11">
-        <v>38</v>
+        <v>9000</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>104</v>
+        <v>223</v>
       </c>
       <c r="L11" s="27">
         <v>1E+36</v>
       </c>
       <c r="M11" s="11"/>
-      <c r="N11" s="11" t="s">
-        <v>11</v>
-      </c>
+      <c r="N11" s="11"/>
       <c r="O11" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
@@ -2310,19 +2403,19 @@
     </row>
     <row r="12" spans="1:21">
       <c r="A12" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" s="18">
-        <v>1</v>
+        <v>23</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>16</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3" t="s">
@@ -2346,7 +2439,7 @@
         <v>11</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
@@ -2356,28 +2449,30 @@
     </row>
     <row r="13" spans="1:21">
       <c r="A13" s="13" t="s">
-        <v>221</v>
+        <v>53</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>222</v>
+        <v>158</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="D13" s="22"/>
-      <c r="E13" s="18" t="s">
-        <v>220</v>
+        <v>83</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="18">
+        <v>1</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3" t="s">
         <v>210</v>
       </c>
       <c r="H13" s="3"/>
-      <c r="I13" s="11">
-        <v>30</v>
+      <c r="I13" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="J13" s="11">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="K13" s="11" t="s">
         <v>104</v>
@@ -2387,9 +2482,11 @@
       </c>
       <c r="M13" s="11"/>
       <c r="N13" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="O13" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>214</v>
+      </c>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
@@ -2398,30 +2495,28 @@
     </row>
     <row r="14" spans="1:21">
       <c r="A14" s="13" t="s">
-        <v>56</v>
+        <v>219</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>158</v>
+        <v>220</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>208</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="D14" s="22"/>
       <c r="E14" s="18" t="s">
-        <v>57</v>
+        <v>218</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3" t="s">
         <v>210</v>
       </c>
       <c r="H14" s="3"/>
-      <c r="I14" s="11" t="s">
-        <v>12</v>
+      <c r="I14" s="11">
+        <v>30</v>
       </c>
       <c r="J14" s="11">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="K14" s="11" t="s">
         <v>104</v>
@@ -2431,11 +2526,9 @@
       </c>
       <c r="M14" s="11"/>
       <c r="N14" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="O14" s="3" t="s">
-        <v>58</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="O14" s="3"/>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
       <c r="R14" s="3"/>
@@ -2444,33 +2537,33 @@
     </row>
     <row r="15" spans="1:21">
       <c r="A15" s="13" t="s">
-        <v>59</v>
+        <v>228</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>60</v>
+        <v>229</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>61</v>
+        <v>126</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3" t="s">
         <v>210</v>
       </c>
       <c r="H15" s="3"/>
-      <c r="I15" s="11" t="s">
-        <v>12</v>
+      <c r="I15" s="11">
+        <v>0</v>
       </c>
       <c r="J15" s="11">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="K15" s="11" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="L15" s="27">
         <v>1E+36</v>
@@ -2480,7 +2573,7 @@
         <v>11</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>62</v>
+        <v>230</v>
       </c>
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
@@ -2490,19 +2583,19 @@
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="13" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
@@ -2510,13 +2603,13 @@
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="11">
-        <v>1350</v>
+        <v>0</v>
       </c>
       <c r="J16" s="11">
-        <v>1600</v>
+        <v>450</v>
       </c>
       <c r="K16" s="11" t="s">
-        <v>227</v>
+        <v>131</v>
       </c>
       <c r="L16" s="27">
         <v>1E+36</v>
@@ -2526,7 +2619,7 @@
         <v>11</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
@@ -2536,19 +2629,19 @@
     </row>
     <row r="17" spans="1:20">
       <c r="A17" s="13" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3" t="s">
@@ -2572,7 +2665,7 @@
         <v>11</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
@@ -2582,16 +2675,16 @@
     </row>
     <row r="18" spans="1:20">
       <c r="A18" s="13" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>32</v>
+        <v>207</v>
       </c>
       <c r="E18" s="18" t="s">
         <v>33</v>
@@ -2602,13 +2695,13 @@
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="11">
-        <v>0</v>
+        <v>1350</v>
       </c>
       <c r="J18" s="11">
-        <v>200</v>
+        <v>1600</v>
       </c>
       <c r="K18" s="11" t="s">
-        <v>104</v>
+        <v>223</v>
       </c>
       <c r="L18" s="27">
         <v>1E+36</v>
@@ -2618,7 +2711,7 @@
         <v>11</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
@@ -2628,33 +2721,33 @@
     </row>
     <row r="19" spans="1:20">
       <c r="A19" s="13" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3" t="s">
         <v>210</v>
       </c>
       <c r="H19" s="3"/>
-      <c r="I19" s="11">
-        <v>0</v>
+      <c r="I19" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="J19" s="11">
-        <v>360</v>
+        <v>38</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>147</v>
+        <v>104</v>
       </c>
       <c r="L19" s="27">
         <v>1E+36</v>
@@ -2664,7 +2757,7 @@
         <v>11</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
@@ -2674,19 +2767,19 @@
     </row>
     <row r="20" spans="1:20">
       <c r="A20" s="13" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3" t="s">
@@ -2694,13 +2787,13 @@
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="11">
-        <v>940</v>
+        <v>0</v>
       </c>
       <c r="J20" s="11">
-        <v>1030</v>
+        <v>200</v>
       </c>
       <c r="K20" s="11" t="s">
-        <v>189</v>
+        <v>104</v>
       </c>
       <c r="L20" s="27">
         <v>1E+36</v>
@@ -2710,7 +2803,7 @@
         <v>11</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
@@ -2720,19 +2813,19 @@
     </row>
     <row r="21" spans="1:20">
       <c r="A21" s="13" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3" t="s">
@@ -2743,10 +2836,10 @@
         <v>0</v>
       </c>
       <c r="J21" s="11">
-        <v>100</v>
+        <v>360</v>
       </c>
       <c r="K21" s="11" t="s">
-        <v>184</v>
+        <v>147</v>
       </c>
       <c r="L21" s="27">
         <v>1E+36</v>
@@ -2756,7 +2849,7 @@
         <v>11</v>
       </c>
       <c r="O21" s="3" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
@@ -2766,17 +2859,19 @@
     </row>
     <row r="22" spans="1:20">
       <c r="A22" s="13" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D22" s="22"/>
+        <v>90</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>38</v>
+      </c>
       <c r="E22" s="18" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3" t="s">
@@ -2784,23 +2879,23 @@
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="11">
-        <v>-100</v>
+        <v>940</v>
       </c>
       <c r="J22" s="11">
-        <v>100</v>
+        <v>1030</v>
       </c>
       <c r="K22" s="11" t="s">
-        <v>131</v>
+        <v>189</v>
       </c>
       <c r="L22" s="27">
         <v>1E+36</v>
       </c>
       <c r="M22" s="11"/>
       <c r="N22" s="11" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="P22" s="3"/>
       <c r="Q22" s="3"/>
@@ -2810,17 +2905,19 @@
     </row>
     <row r="23" spans="1:20">
       <c r="A23" s="13" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D23" s="22"/>
+        <v>91</v>
+      </c>
+      <c r="D23" s="22" t="s">
+        <v>42</v>
+      </c>
       <c r="E23" s="18" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3" t="s">
@@ -2828,23 +2925,23 @@
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="11">
-        <v>-100</v>
+        <v>0</v>
       </c>
       <c r="J23" s="11">
         <v>100</v>
       </c>
       <c r="K23" s="11" t="s">
-        <v>131</v>
+        <v>184</v>
       </c>
       <c r="L23" s="27">
         <v>1E+36</v>
       </c>
       <c r="M23" s="11"/>
       <c r="N23" s="11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="O23" s="3" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
@@ -2854,43 +2951,41 @@
     </row>
     <row r="24" spans="1:20">
       <c r="A24" s="13" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D24" s="22" t="s">
-        <v>23</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="D24" s="22"/>
       <c r="E24" s="18" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3" t="s">
         <v>210</v>
       </c>
       <c r="H24" s="3"/>
-      <c r="I24" s="11" t="s">
-        <v>12</v>
+      <c r="I24" s="11">
+        <v>-100</v>
       </c>
       <c r="J24" s="11">
-        <v>38</v>
+        <v>100</v>
       </c>
       <c r="K24" s="11" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="L24" s="27">
         <v>1E+36</v>
       </c>
       <c r="M24" s="11"/>
       <c r="N24" s="11" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="O24" s="3" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
@@ -2900,43 +2995,41 @@
     </row>
     <row r="25" spans="1:20">
       <c r="A25" s="13" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D25" s="22" t="s">
-        <v>23</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="D25" s="22"/>
       <c r="E25" s="18" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3" t="s">
         <v>210</v>
       </c>
       <c r="H25" s="3"/>
-      <c r="I25" s="11" t="s">
-        <v>12</v>
+      <c r="I25" s="11">
+        <v>-100</v>
       </c>
       <c r="J25" s="11">
-        <v>38</v>
+        <v>100</v>
       </c>
       <c r="K25" s="11" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="L25" s="27">
         <v>1E+36</v>
       </c>
       <c r="M25" s="11"/>
       <c r="N25" s="11" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="O25" s="3" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
@@ -2946,19 +3039,19 @@
     </row>
     <row r="26" spans="1:20">
       <c r="A26" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>54</v>
+        <v>23</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>206</v>
+        <v>16</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3" t="s">
@@ -2982,7 +3075,7 @@
         <v>11</v>
       </c>
       <c r="O26" s="3" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
@@ -2992,31 +3085,33 @@
     </row>
     <row r="27" spans="1:20">
       <c r="A27" s="13" t="s">
-        <v>74</v>
+        <v>27</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D27" s="22"/>
+        <v>95</v>
+      </c>
+      <c r="D27" s="22" t="s">
+        <v>23</v>
+      </c>
       <c r="E27" s="18" t="s">
-        <v>75</v>
+        <v>16</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3" t="s">
         <v>210</v>
       </c>
       <c r="H27" s="3"/>
-      <c r="I27" s="11">
-        <v>100</v>
+      <c r="I27" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="J27" s="11">
-        <v>700</v>
+        <v>38</v>
       </c>
       <c r="K27" s="11" t="s">
-        <v>131</v>
+        <v>104</v>
       </c>
       <c r="L27" s="27">
         <v>1E+36</v>
@@ -3025,7 +3120,9 @@
       <c r="N27" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="O27" s="3"/>
+      <c r="O27" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="P27" s="3"/>
       <c r="Q27" s="3"/>
       <c r="R27" s="3"/>
@@ -3034,31 +3131,33 @@
     </row>
     <row r="28" spans="1:20">
       <c r="A28" s="13" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D28" s="22"/>
+        <v>96</v>
+      </c>
+      <c r="D28" s="22" t="s">
+        <v>54</v>
+      </c>
       <c r="E28" s="18" t="s">
-        <v>77</v>
+        <v>206</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3" t="s">
         <v>210</v>
       </c>
       <c r="H28" s="3"/>
-      <c r="I28" s="11">
-        <v>0</v>
+      <c r="I28" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="J28" s="11">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="K28" s="11" t="s">
-        <v>228</v>
+        <v>104</v>
       </c>
       <c r="L28" s="27">
         <v>1E+36</v>
@@ -3067,7 +3166,9 @@
       <c r="N28" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="O28" s="3"/>
+      <c r="O28" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="P28" s="3"/>
       <c r="Q28" s="3"/>
       <c r="R28" s="3"/>
@@ -3075,32 +3176,32 @@
       <c r="T28" s="3"/>
     </row>
     <row r="29" spans="1:20">
-      <c r="A29" s="25" t="s">
-        <v>194</v>
+      <c r="A29" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C29" s="28" t="s">
-        <v>195</v>
+      <c r="C29" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="D29" s="22"/>
-      <c r="E29" s="29" t="s">
-        <v>196</v>
+      <c r="E29" s="18" t="s">
+        <v>75</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3" t="s">
         <v>210</v>
       </c>
       <c r="H29" s="3"/>
-      <c r="I29" s="30">
-        <v>0</v>
-      </c>
-      <c r="J29" s="30">
-        <v>10</v>
-      </c>
-      <c r="K29" s="30" t="s">
-        <v>104</v>
+      <c r="I29" s="11">
+        <v>100</v>
+      </c>
+      <c r="J29" s="11">
+        <v>700</v>
+      </c>
+      <c r="K29" s="11" t="s">
+        <v>131</v>
       </c>
       <c r="L29" s="27">
         <v>1E+36</v>
@@ -3118,17 +3219,17 @@
     </row>
     <row r="30" spans="1:20">
       <c r="A30" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="18" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3" t="s">
@@ -3139,10 +3240,10 @@
         <v>0</v>
       </c>
       <c r="J30" s="11">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="K30" s="11" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="L30" s="27">
         <v>1E+36</v>
@@ -3160,17 +3261,17 @@
     </row>
     <row r="31" spans="1:20">
       <c r="A31" s="25" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="D31" s="22"/>
-      <c r="E31" s="18" t="s">
-        <v>188</v>
+      <c r="E31" s="29" t="s">
+        <v>196</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3" t="s">
@@ -3181,10 +3282,10 @@
         <v>0</v>
       </c>
       <c r="J31" s="30">
-        <v>3000</v>
+        <v>10</v>
       </c>
       <c r="K31" s="30" t="s">
-        <v>189</v>
+        <v>104</v>
       </c>
       <c r="L31" s="27">
         <v>1E+36</v>
@@ -3202,17 +3303,17 @@
     </row>
     <row r="32" spans="1:20">
       <c r="A32" s="25" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>191</v>
+        <v>236</v>
       </c>
       <c r="D32" s="22"/>
-      <c r="E32" s="18" t="s">
-        <v>188</v>
+      <c r="E32" s="29" t="s">
+        <v>196</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3" t="s">
@@ -3223,10 +3324,10 @@
         <v>0</v>
       </c>
       <c r="J32" s="30">
-        <v>4000</v>
+        <v>10</v>
       </c>
       <c r="K32" s="30" t="s">
-        <v>189</v>
+        <v>104</v>
       </c>
       <c r="L32" s="27">
         <v>1E+36</v>
@@ -3242,33 +3343,33 @@
       <c r="S32" s="3"/>
       <c r="T32" s="3"/>
     </row>
-    <row r="33" spans="1:20" ht="12.6" customHeight="1">
-      <c r="A33" s="25" t="s">
-        <v>192</v>
+    <row r="33" spans="1:20">
+      <c r="A33" s="13" t="s">
+        <v>78</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C33" s="28" t="s">
-        <v>193</v>
+      <c r="C33" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="D33" s="22"/>
       <c r="E33" s="18" t="s">
-        <v>188</v>
+        <v>43</v>
       </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3" t="s">
         <v>210</v>
       </c>
       <c r="H33" s="3"/>
-      <c r="I33" s="30">
+      <c r="I33" s="11">
         <v>0</v>
       </c>
-      <c r="J33" s="30">
-        <v>3000</v>
-      </c>
-      <c r="K33" s="30" t="s">
-        <v>189</v>
+      <c r="J33" s="11">
+        <v>100</v>
+      </c>
+      <c r="K33" s="11" t="s">
+        <v>225</v>
       </c>
       <c r="L33" s="27">
         <v>1E+36</v>
@@ -3284,33 +3385,33 @@
       <c r="S33" s="3"/>
       <c r="T33" s="3"/>
     </row>
-    <row r="34" spans="1:20" ht="12.6" customHeight="1">
-      <c r="A34" s="26" t="s">
-        <v>197</v>
+    <row r="34" spans="1:20">
+      <c r="A34" s="25" t="s">
+        <v>186</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C34" s="31" t="s">
-        <v>198</v>
+      <c r="C34" s="28" t="s">
+        <v>187</v>
       </c>
       <c r="D34" s="22"/>
-      <c r="E34" s="32" t="s">
-        <v>199</v>
+      <c r="E34" s="18" t="s">
+        <v>188</v>
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="3" t="s">
         <v>210</v>
       </c>
       <c r="H34" s="3"/>
-      <c r="I34" s="31">
+      <c r="I34" s="30">
         <v>0</v>
       </c>
-      <c r="J34" s="33">
-        <v>999999</v>
-      </c>
-      <c r="K34" s="33" t="s">
-        <v>200</v>
+      <c r="J34" s="30">
+        <v>3000</v>
+      </c>
+      <c r="K34" s="30" t="s">
+        <v>189</v>
       </c>
       <c r="L34" s="27">
         <v>1E+36</v>
@@ -3327,32 +3428,32 @@
       <c r="T34" s="3"/>
     </row>
     <row r="35" spans="1:20">
-      <c r="A35" s="13" t="s">
-        <v>63</v>
+      <c r="A35" s="25" t="s">
+        <v>190</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>94</v>
+      <c r="C35" s="28" t="s">
+        <v>191</v>
       </c>
       <c r="D35" s="22"/>
       <c r="E35" s="18" t="s">
-        <v>16</v>
+        <v>188</v>
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3" t="s">
         <v>210</v>
       </c>
       <c r="H35" s="3"/>
-      <c r="I35" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="J35" s="11">
-        <v>38</v>
-      </c>
-      <c r="K35" s="11" t="s">
-        <v>104</v>
+      <c r="I35" s="30">
+        <v>0</v>
+      </c>
+      <c r="J35" s="30">
+        <v>4000</v>
+      </c>
+      <c r="K35" s="30" t="s">
+        <v>189</v>
       </c>
       <c r="L35" s="27">
         <v>1E+36</v>
@@ -3368,33 +3469,33 @@
       <c r="S35" s="3"/>
       <c r="T35" s="3"/>
     </row>
-    <row r="36" spans="1:20">
-      <c r="A36" s="13" t="s">
-        <v>105</v>
+    <row r="36" spans="1:20" ht="12.6" customHeight="1">
+      <c r="A36" s="25" t="s">
+        <v>186</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>106</v>
+      <c r="C36" s="28" t="s">
+        <v>187</v>
       </c>
       <c r="D36" s="22"/>
-      <c r="E36" s="18">
-        <v>1</v>
+      <c r="E36" s="18" t="s">
+        <v>188</v>
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3" t="s">
         <v>210</v>
       </c>
       <c r="H36" s="3"/>
-      <c r="I36" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="J36" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="K36" s="11" t="s">
-        <v>109</v>
+      <c r="I36" s="30">
+        <v>0</v>
+      </c>
+      <c r="J36" s="30">
+        <v>3000</v>
+      </c>
+      <c r="K36" s="30" t="s">
+        <v>189</v>
       </c>
       <c r="L36" s="27">
         <v>1E+36</v>
@@ -3410,33 +3511,33 @@
       <c r="S36" s="3"/>
       <c r="T36" s="3"/>
     </row>
-    <row r="37" spans="1:20">
-      <c r="A37" s="13" t="s">
-        <v>110</v>
+    <row r="37" spans="1:20" ht="12.6" customHeight="1">
+      <c r="A37" s="25" t="s">
+        <v>192</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>111</v>
+      <c r="C37" s="28" t="s">
+        <v>193</v>
       </c>
       <c r="D37" s="22"/>
       <c r="E37" s="18" t="s">
-        <v>16</v>
+        <v>188</v>
       </c>
       <c r="F37" s="3"/>
       <c r="G37" s="3" t="s">
         <v>210</v>
       </c>
       <c r="H37" s="3"/>
-      <c r="I37" s="11">
-        <v>-2</v>
-      </c>
-      <c r="J37" s="11">
-        <v>32</v>
-      </c>
-      <c r="K37" s="11" t="s">
-        <v>104</v>
+      <c r="I37" s="30">
+        <v>0</v>
+      </c>
+      <c r="J37" s="30">
+        <v>3000</v>
+      </c>
+      <c r="K37" s="30" t="s">
+        <v>189</v>
       </c>
       <c r="L37" s="27">
         <v>1E+36</v>
@@ -3452,40 +3553,40 @@
       <c r="S37" s="3"/>
       <c r="T37" s="3"/>
     </row>
-    <row r="38" spans="1:20">
-      <c r="A38" s="13" t="s">
-        <v>112</v>
+    <row r="38" spans="1:20" ht="12.6" customHeight="1">
+      <c r="A38" s="25" t="s">
+        <v>226</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>113</v>
+      <c r="C38" s="28" t="s">
+        <v>227</v>
       </c>
       <c r="D38" s="22"/>
       <c r="E38" s="18" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3" t="s">
         <v>210</v>
       </c>
       <c r="H38" s="3"/>
-      <c r="I38" s="11">
-        <v>-2</v>
-      </c>
-      <c r="J38" s="11">
-        <v>32</v>
-      </c>
-      <c r="K38" s="11" t="s">
-        <v>104</v>
+      <c r="I38" s="30">
+        <v>0</v>
+      </c>
+      <c r="J38" s="30">
+        <v>100</v>
+      </c>
+      <c r="K38" s="30" t="s">
+        <v>225</v>
       </c>
       <c r="L38" s="27">
         <v>1E+36</v>
       </c>
       <c r="M38" s="11"/>
       <c r="N38" s="11" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="O38" s="3"/>
       <c r="P38" s="3"/>
@@ -3494,33 +3595,33 @@
       <c r="S38" s="3"/>
       <c r="T38" s="3"/>
     </row>
-    <row r="39" spans="1:20">
-      <c r="A39" s="13" t="s">
-        <v>114</v>
+    <row r="39" spans="1:20" ht="12.6" customHeight="1">
+      <c r="A39" s="26" t="s">
+        <v>197</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>115</v>
+      <c r="C39" s="31" t="s">
+        <v>198</v>
       </c>
       <c r="D39" s="22"/>
-      <c r="E39" s="18" t="s">
-        <v>206</v>
+      <c r="E39" s="32" t="s">
+        <v>199</v>
       </c>
       <c r="F39" s="3"/>
       <c r="G39" s="3" t="s">
         <v>210</v>
       </c>
       <c r="H39" s="3"/>
-      <c r="I39" s="11">
-        <v>33</v>
-      </c>
-      <c r="J39" s="11">
-        <v>37</v>
-      </c>
-      <c r="K39" s="11" t="s">
-        <v>104</v>
+      <c r="I39" s="31">
+        <v>0</v>
+      </c>
+      <c r="J39" s="33">
+        <v>999999</v>
+      </c>
+      <c r="K39" s="33" t="s">
+        <v>200</v>
       </c>
       <c r="L39" s="27">
         <v>1E+36</v>
@@ -3536,40 +3637,40 @@
       <c r="S39" s="3"/>
       <c r="T39" s="3"/>
     </row>
-    <row r="40" spans="1:20">
-      <c r="A40" s="13" t="s">
-        <v>116</v>
+    <row r="40" spans="1:20" ht="12.6" customHeight="1">
+      <c r="A40" s="26" t="s">
+        <v>233</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>117</v>
+      <c r="C40" s="31" t="s">
+        <v>234</v>
       </c>
       <c r="D40" s="22"/>
-      <c r="E40" s="18" t="s">
-        <v>206</v>
+      <c r="E40" s="32" t="s">
+        <v>77</v>
       </c>
       <c r="F40" s="3"/>
       <c r="G40" s="3" t="s">
         <v>210</v>
       </c>
       <c r="H40" s="3"/>
-      <c r="I40" s="11">
-        <v>33</v>
-      </c>
-      <c r="J40" s="11">
-        <v>37</v>
-      </c>
-      <c r="K40" s="11" t="s">
-        <v>104</v>
+      <c r="I40" s="31">
+        <v>-500</v>
+      </c>
+      <c r="J40" s="33">
+        <v>500</v>
+      </c>
+      <c r="K40" s="33" t="s">
+        <v>235</v>
       </c>
       <c r="L40" s="27">
         <v>1E+36</v>
       </c>
       <c r="M40" s="11"/>
       <c r="N40" s="11" t="s">
-        <v>11</v>
+        <v>185</v>
       </c>
       <c r="O40" s="3"/>
       <c r="P40" s="3"/>
@@ -3580,31 +3681,31 @@
     </row>
     <row r="41" spans="1:20">
       <c r="A41" s="13" t="s">
-        <v>118</v>
+        <v>63</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
       <c r="D41" s="22"/>
       <c r="E41" s="18" t="s">
-        <v>120</v>
+        <v>16</v>
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3" t="s">
         <v>210</v>
       </c>
       <c r="H41" s="3"/>
-      <c r="I41" s="11">
-        <v>3</v>
+      <c r="I41" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="J41" s="11">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="K41" s="11" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="L41" s="27">
         <v>1E+36</v>
@@ -3622,31 +3723,31 @@
     </row>
     <row r="42" spans="1:20">
       <c r="A42" s="13" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="D42" s="22"/>
-      <c r="E42" s="18" t="s">
-        <v>120</v>
+      <c r="E42" s="18">
+        <v>1</v>
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3" t="s">
         <v>210</v>
       </c>
       <c r="H42" s="3"/>
-      <c r="I42" s="11">
-        <v>3</v>
-      </c>
-      <c r="J42" s="11">
-        <v>7</v>
+      <c r="I42" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="J42" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="K42" s="11" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="L42" s="27">
         <v>1E+36</v>
@@ -3664,17 +3765,17 @@
     </row>
     <row r="43" spans="1:20">
       <c r="A43" s="13" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="D43" s="22"/>
       <c r="E43" s="18" t="s">
-        <v>126</v>
+        <v>16</v>
       </c>
       <c r="F43" s="3"/>
       <c r="G43" s="3" t="s">
@@ -3682,13 +3783,13 @@
       </c>
       <c r="H43" s="3"/>
       <c r="I43" s="11">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="J43" s="11">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="K43" s="11" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="L43" s="27">
         <v>1E+36</v>
@@ -3706,17 +3807,17 @@
     </row>
     <row r="44" spans="1:20">
       <c r="A44" s="13" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="D44" s="22"/>
       <c r="E44" s="18" t="s">
-        <v>126</v>
+        <v>16</v>
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3" t="s">
@@ -3724,13 +3825,13 @@
       </c>
       <c r="H44" s="3"/>
       <c r="I44" s="11">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="J44" s="11">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="K44" s="11" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="L44" s="27">
         <v>1E+36</v>
@@ -3748,17 +3849,17 @@
     </row>
     <row r="45" spans="1:20">
       <c r="A45" s="13" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="D45" s="22"/>
       <c r="E45" s="18" t="s">
-        <v>57</v>
+        <v>206</v>
       </c>
       <c r="F45" s="3"/>
       <c r="G45" s="3" t="s">
@@ -3766,13 +3867,13 @@
       </c>
       <c r="H45" s="3"/>
       <c r="I45" s="11">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="J45" s="11">
-        <v>450</v>
+        <v>37</v>
       </c>
       <c r="K45" s="11" t="s">
-        <v>131</v>
+        <v>104</v>
       </c>
       <c r="L45" s="27">
         <v>1E+36</v>
@@ -3790,17 +3891,17 @@
     </row>
     <row r="46" spans="1:20">
       <c r="A46" s="13" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="D46" s="22"/>
       <c r="E46" s="18" t="s">
-        <v>57</v>
+        <v>206</v>
       </c>
       <c r="F46" s="3"/>
       <c r="G46" s="3" t="s">
@@ -3808,13 +3909,13 @@
       </c>
       <c r="H46" s="3"/>
       <c r="I46" s="11">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="J46" s="11">
-        <v>450</v>
+        <v>37</v>
       </c>
       <c r="K46" s="11" t="s">
-        <v>131</v>
+        <v>104</v>
       </c>
       <c r="L46" s="27">
         <v>1E+36</v>
@@ -3832,17 +3933,17 @@
     </row>
     <row r="47" spans="1:20">
       <c r="A47" s="13" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="D47" s="22"/>
       <c r="E47" s="18" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3" t="s">
@@ -3850,13 +3951,13 @@
       </c>
       <c r="H47" s="3"/>
       <c r="I47" s="11">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J47" s="11">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="K47" s="11" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="L47" s="27">
         <v>1E+36</v>
@@ -3874,17 +3975,17 @@
     </row>
     <row r="48" spans="1:20">
       <c r="A48" s="13" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="D48" s="22"/>
       <c r="E48" s="18" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="F48" s="3"/>
       <c r="G48" s="3" t="s">
@@ -3892,13 +3993,13 @@
       </c>
       <c r="H48" s="3"/>
       <c r="I48" s="11">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J48" s="11">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="K48" s="11" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="L48" s="27">
         <v>1E+36</v>
@@ -3916,17 +4017,17 @@
     </row>
     <row r="49" spans="1:20">
       <c r="A49" s="13" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="D49" s="22"/>
       <c r="E49" s="18" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="F49" s="3"/>
       <c r="G49" s="3" t="s">
@@ -3934,13 +4035,13 @@
       </c>
       <c r="H49" s="3"/>
       <c r="I49" s="11">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J49" s="11">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K49" s="11" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="L49" s="27">
         <v>1E+36</v>
@@ -3958,17 +4059,17 @@
     </row>
     <row r="50" spans="1:20">
       <c r="A50" s="13" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="D50" s="22"/>
       <c r="E50" s="18" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="F50" s="3"/>
       <c r="G50" s="3" t="s">
@@ -3976,13 +4077,13 @@
       </c>
       <c r="H50" s="3"/>
       <c r="I50" s="11">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J50" s="11">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K50" s="11" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="L50" s="27">
         <v>1E+36</v>
@@ -4000,17 +4101,17 @@
     </row>
     <row r="51" spans="1:20">
       <c r="A51" s="13" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="D51" s="22"/>
       <c r="E51" s="18" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="F51" s="3"/>
       <c r="G51" s="3" t="s">
@@ -4021,10 +4122,10 @@
         <v>0</v>
       </c>
       <c r="J51" s="11">
-        <v>90</v>
+        <v>450</v>
       </c>
       <c r="K51" s="11" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="L51" s="27">
         <v>1E+36</v>
@@ -4042,81 +4143,81 @@
     </row>
     <row r="52" spans="1:20">
       <c r="A52" s="13" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="D52" s="22"/>
       <c r="E52" s="18" t="s">
-        <v>150</v>
+        <v>57</v>
       </c>
       <c r="F52" s="3"/>
       <c r="G52" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="H52" s="3" t="s">
-        <v>44</v>
-      </c>
+      <c r="H52" s="3"/>
       <c r="I52" s="11">
         <v>0</v>
       </c>
       <c r="J52" s="11">
-        <v>40000</v>
+        <v>450</v>
       </c>
       <c r="K52" s="11" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
       <c r="L52" s="27">
         <v>1E+36</v>
       </c>
       <c r="M52" s="11"/>
       <c r="N52" s="11" t="s">
-        <v>185</v>
+        <v>11</v>
       </c>
       <c r="O52" s="3"/>
       <c r="P52" s="3"/>
       <c r="Q52" s="3"/>
       <c r="R52" s="3"/>
       <c r="S52" s="3"/>
-      <c r="T52" s="3" t="s">
-        <v>180</v>
-      </c>
+      <c r="T52" s="3"/>
     </row>
     <row r="53" spans="1:20">
-      <c r="A53" s="14" t="s">
-        <v>201</v>
+      <c r="A53" s="13" t="s">
+        <v>133</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C53" s="34" t="s">
-        <v>202</v>
+        <v>158</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="D53" s="22"/>
-      <c r="E53" s="18">
-        <v>1</v>
-      </c>
-      <c r="F53" s="34"/>
-      <c r="G53" s="34"/>
+      <c r="E53" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3" t="s">
+        <v>210</v>
+      </c>
       <c r="H53" s="3"/>
-      <c r="I53" s="34">
+      <c r="I53" s="11">
         <v>0</v>
       </c>
-      <c r="J53" s="35">
-        <v>999</v>
-      </c>
-      <c r="K53" s="35" t="s">
-        <v>203</v>
-      </c>
-      <c r="L53" s="23">
-        <v>99999</v>
+      <c r="J53" s="11">
+        <v>10</v>
+      </c>
+      <c r="K53" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="L53" s="27">
+        <v>1E+36</v>
       </c>
       <c r="M53" s="11"/>
-      <c r="N53" s="11"/>
+      <c r="N53" s="11" t="s">
+        <v>11</v>
+      </c>
       <c r="O53" s="3"/>
       <c r="P53" s="3"/>
       <c r="Q53" s="3"/>
@@ -4126,35 +4227,39 @@
     </row>
     <row r="54" spans="1:20">
       <c r="A54" s="13" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>100</v>
+        <v>158</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="D54" s="22"/>
-      <c r="E54" s="18">
-        <v>1</v>
+      <c r="E54" s="18" t="s">
+        <v>135</v>
       </c>
       <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
+      <c r="G54" s="3" t="s">
+        <v>210</v>
+      </c>
       <c r="H54" s="3"/>
       <c r="I54" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J54" s="11">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="K54" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="L54" s="23">
-        <v>99999</v>
+        <v>136</v>
+      </c>
+      <c r="L54" s="27">
+        <v>1E+36</v>
       </c>
       <c r="M54" s="11"/>
-      <c r="N54" s="11"/>
+      <c r="N54" s="11" t="s">
+        <v>11</v>
+      </c>
       <c r="O54" s="3"/>
       <c r="P54" s="3"/>
       <c r="Q54" s="3"/>
@@ -4164,35 +4269,39 @@
     </row>
     <row r="55" spans="1:20">
       <c r="A55" s="13" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>100</v>
+        <v>158</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="D55" s="22"/>
-      <c r="E55" s="18">
+      <c r="E55" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="H55" s="3"/>
+      <c r="I55" s="11">
+        <v>-1</v>
+      </c>
+      <c r="J55" s="11">
         <v>1</v>
       </c>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
-      <c r="H55" s="3"/>
-      <c r="I55" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="J55" s="11" t="s">
-        <v>157</v>
-      </c>
       <c r="K55" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="L55" s="23">
-        <v>99999</v>
+        <v>142</v>
+      </c>
+      <c r="L55" s="27">
+        <v>1E+36</v>
       </c>
       <c r="M55" s="11"/>
-      <c r="N55" s="11"/>
+      <c r="N55" s="11" t="s">
+        <v>11</v>
+      </c>
       <c r="O55" s="3"/>
       <c r="P55" s="3"/>
       <c r="Q55" s="3"/>
@@ -4202,36 +4311,38 @@
     </row>
     <row r="56" spans="1:20">
       <c r="A56" s="13" t="s">
-        <v>182</v>
+        <v>143</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>183</v>
+        <v>144</v>
       </c>
       <c r="D56" s="22"/>
       <c r="E56" s="18" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="F56" s="3"/>
-      <c r="G56" s="3"/>
+      <c r="G56" s="3" t="s">
+        <v>210</v>
+      </c>
       <c r="H56" s="3"/>
       <c r="I56" s="11">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J56" s="11">
-        <v>11000</v>
+        <v>1</v>
       </c>
       <c r="K56" s="11" t="s">
-        <v>184</v>
+        <v>142</v>
       </c>
       <c r="L56" s="27">
         <v>1E+36</v>
       </c>
       <c r="M56" s="11"/>
       <c r="N56" s="11" t="s">
-        <v>185</v>
+        <v>222</v>
       </c>
       <c r="O56" s="3"/>
       <c r="P56" s="3"/>
@@ -4242,17 +4353,19 @@
     </row>
     <row r="57" spans="1:20">
       <c r="A57" s="13" t="s">
-        <v>225</v>
+        <v>240</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>158</v>
+        <v>220</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="D57" s="22"/>
+        <v>238</v>
+      </c>
+      <c r="D57" s="22" t="s">
+        <v>241</v>
+      </c>
       <c r="E57" s="18" t="s">
-        <v>220</v>
+        <v>57</v>
       </c>
       <c r="F57" s="3"/>
       <c r="G57" s="3" t="s">
@@ -4260,13 +4373,13 @@
       </c>
       <c r="H57" s="3"/>
       <c r="I57" s="11">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="J57" s="11">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="K57" s="11" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="L57" s="27">
         <v>1E+36</v>
@@ -4284,17 +4397,19 @@
     </row>
     <row r="58" spans="1:20">
       <c r="A58" s="13" t="s">
-        <v>218</v>
+        <v>237</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>158</v>
+        <v>220</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="D58" s="22"/>
+        <v>238</v>
+      </c>
+      <c r="D58" s="22" t="s">
+        <v>242</v>
+      </c>
       <c r="E58" s="18" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="F58" s="3"/>
       <c r="G58" s="3" t="s">
@@ -4302,10 +4417,10 @@
       </c>
       <c r="H58" s="3"/>
       <c r="I58" s="11">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="J58" s="11">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="K58" s="11" t="s">
         <v>104</v>
@@ -4326,17 +4441,19 @@
     </row>
     <row r="59" spans="1:20">
       <c r="A59" s="13" t="s">
-        <v>219</v>
+        <v>248</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>158</v>
+        <v>220</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D59" s="22"/>
+        <v>250</v>
+      </c>
+      <c r="D59" s="22" t="s">
+        <v>251</v>
+      </c>
       <c r="E59" s="18" t="s">
-        <v>220</v>
+        <v>57</v>
       </c>
       <c r="F59" s="3"/>
       <c r="G59" s="3" t="s">
@@ -4344,13 +4461,13 @@
       </c>
       <c r="H59" s="3"/>
       <c r="I59" s="11">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="J59" s="11">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="K59" s="11" t="s">
-        <v>104</v>
+        <v>127</v>
       </c>
       <c r="L59" s="27">
         <v>1E+36</v>
@@ -4365,6 +4482,510 @@
       <c r="R59" s="3"/>
       <c r="S59" s="3"/>
       <c r="T59" s="3"/>
+    </row>
+    <row r="60" spans="1:20">
+      <c r="A60" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="D60" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="E60" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="H60" s="3"/>
+      <c r="I60" s="11">
+        <v>0</v>
+      </c>
+      <c r="J60" s="11">
+        <v>56</v>
+      </c>
+      <c r="K60" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="L60" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M60" s="11"/>
+      <c r="N60" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="O60" s="3"/>
+      <c r="P60" s="3"/>
+      <c r="Q60" s="3"/>
+      <c r="R60" s="3"/>
+      <c r="S60" s="3"/>
+      <c r="T60" s="3"/>
+    </row>
+    <row r="61" spans="1:20">
+      <c r="A61" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D61" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="E61" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="H61" s="3"/>
+      <c r="I61" s="11">
+        <v>0</v>
+      </c>
+      <c r="J61" s="11">
+        <v>10</v>
+      </c>
+      <c r="K61" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="L61" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M61" s="11"/>
+      <c r="N61" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="O61" s="3"/>
+      <c r="P61" s="3"/>
+      <c r="Q61" s="3"/>
+      <c r="R61" s="3"/>
+      <c r="S61" s="3"/>
+      <c r="T61" s="3"/>
+    </row>
+    <row r="62" spans="1:20">
+      <c r="A62" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D62" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="E62" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="F62" s="3"/>
+      <c r="G62" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="H62" s="3"/>
+      <c r="I62" s="11">
+        <v>0</v>
+      </c>
+      <c r="J62" s="11">
+        <v>100</v>
+      </c>
+      <c r="K62" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="L62" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M62" s="11"/>
+      <c r="N62" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="O62" s="3"/>
+      <c r="P62" s="3"/>
+      <c r="Q62" s="3"/>
+      <c r="R62" s="3"/>
+      <c r="S62" s="3"/>
+      <c r="T62" s="3"/>
+    </row>
+    <row r="63" spans="1:20">
+      <c r="A63" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="D63" s="22" t="s">
+        <v>256</v>
+      </c>
+      <c r="E63" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="H63" s="3"/>
+      <c r="I63" s="11">
+        <v>0</v>
+      </c>
+      <c r="J63" s="11">
+        <v>10</v>
+      </c>
+      <c r="K63" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L63" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M63" s="11"/>
+      <c r="N63" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="O63" s="3"/>
+      <c r="P63" s="3"/>
+      <c r="Q63" s="3"/>
+      <c r="R63" s="3"/>
+      <c r="S63" s="3"/>
+      <c r="T63" s="3"/>
+    </row>
+    <row r="64" spans="1:20">
+      <c r="A64" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="D64" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="E64" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="H64" s="3"/>
+      <c r="I64" s="11">
+        <v>0</v>
+      </c>
+      <c r="J64" s="11">
+        <v>4</v>
+      </c>
+      <c r="K64" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="L64" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M64" s="11"/>
+      <c r="N64" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="O64" s="3"/>
+      <c r="P64" s="3"/>
+      <c r="Q64" s="3"/>
+      <c r="R64" s="3"/>
+      <c r="S64" s="3"/>
+      <c r="T64" s="3"/>
+    </row>
+    <row r="65" spans="1:20">
+      <c r="A65" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="D65" s="22"/>
+      <c r="E65" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="F65" s="3"/>
+      <c r="G65" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="H65" s="3"/>
+      <c r="I65" s="11">
+        <v>0</v>
+      </c>
+      <c r="J65" s="11">
+        <v>99</v>
+      </c>
+      <c r="K65" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="L65" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M65" s="11"/>
+      <c r="N65" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="O65" s="3"/>
+      <c r="P65" s="3"/>
+      <c r="Q65" s="3"/>
+      <c r="R65" s="3"/>
+      <c r="S65" s="3"/>
+      <c r="T65" s="3"/>
+    </row>
+    <row r="66" spans="1:20">
+      <c r="A66" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D66" s="22"/>
+      <c r="E66" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="H66" s="3"/>
+      <c r="I66" s="11">
+        <v>0</v>
+      </c>
+      <c r="J66" s="11">
+        <v>90</v>
+      </c>
+      <c r="K66" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="L66" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M66" s="11"/>
+      <c r="N66" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="O66" s="3"/>
+      <c r="P66" s="3"/>
+      <c r="Q66" s="3"/>
+      <c r="R66" s="3"/>
+      <c r="S66" s="3"/>
+      <c r="T66" s="3"/>
+    </row>
+    <row r="67" spans="1:20">
+      <c r="A67" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D67" s="22"/>
+      <c r="E67" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="H67" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I67" s="11">
+        <v>0</v>
+      </c>
+      <c r="J67" s="11">
+        <v>40000</v>
+      </c>
+      <c r="K67" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="L67" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M67" s="11"/>
+      <c r="N67" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="O67" s="3"/>
+      <c r="P67" s="3"/>
+      <c r="Q67" s="3"/>
+      <c r="R67" s="3"/>
+      <c r="S67" s="3"/>
+      <c r="T67" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20">
+      <c r="A68" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C68" s="34" t="s">
+        <v>202</v>
+      </c>
+      <c r="D68" s="22"/>
+      <c r="E68" s="18">
+        <v>1</v>
+      </c>
+      <c r="F68" s="34"/>
+      <c r="G68" s="34"/>
+      <c r="H68" s="3"/>
+      <c r="I68" s="34">
+        <v>0</v>
+      </c>
+      <c r="J68" s="35">
+        <v>999</v>
+      </c>
+      <c r="K68" s="35" t="s">
+        <v>203</v>
+      </c>
+      <c r="L68" s="23">
+        <v>99999</v>
+      </c>
+      <c r="M68" s="11"/>
+      <c r="N68" s="11"/>
+      <c r="O68" s="3"/>
+      <c r="P68" s="3"/>
+      <c r="Q68" s="3"/>
+      <c r="R68" s="3"/>
+      <c r="S68" s="3"/>
+      <c r="T68" s="3"/>
+    </row>
+    <row r="69" spans="1:20">
+      <c r="A69" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D69" s="22"/>
+      <c r="E69" s="18">
+        <v>1</v>
+      </c>
+      <c r="F69" s="3"/>
+      <c r="G69" s="3"/>
+      <c r="H69" s="3"/>
+      <c r="I69" s="11">
+        <v>1</v>
+      </c>
+      <c r="J69" s="11">
+        <v>36</v>
+      </c>
+      <c r="K69" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="L69" s="23">
+        <v>99999</v>
+      </c>
+      <c r="M69" s="11"/>
+      <c r="N69" s="11"/>
+      <c r="O69" s="3"/>
+      <c r="P69" s="3"/>
+      <c r="Q69" s="3"/>
+      <c r="R69" s="3"/>
+      <c r="S69" s="3"/>
+      <c r="T69" s="3"/>
+    </row>
+    <row r="70" spans="1:20">
+      <c r="A70" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D70" s="22"/>
+      <c r="E70" s="18">
+        <v>1</v>
+      </c>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3"/>
+      <c r="H70" s="3"/>
+      <c r="I70" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="J70" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="K70" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="L70" s="23">
+        <v>99999</v>
+      </c>
+      <c r="M70" s="11"/>
+      <c r="N70" s="11"/>
+      <c r="O70" s="3"/>
+      <c r="P70" s="3"/>
+      <c r="Q70" s="3"/>
+      <c r="R70" s="3"/>
+      <c r="S70" s="3"/>
+      <c r="T70" s="3"/>
+    </row>
+    <row r="71" spans="1:20">
+      <c r="A71" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D71" s="22"/>
+      <c r="E71" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="F71" s="3"/>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3"/>
+      <c r="I71" s="11">
+        <v>0</v>
+      </c>
+      <c r="J71" s="11">
+        <v>11000</v>
+      </c>
+      <c r="K71" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="L71" s="27">
+        <v>1E+36</v>
+      </c>
+      <c r="M71" s="11"/>
+      <c r="N71" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="O71" s="3"/>
+      <c r="P71" s="3"/>
+      <c r="Q71" s="3"/>
+      <c r="R71" s="3"/>
+      <c r="S71" s="3"/>
+      <c r="T71" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
change bad float33 type to float32
</commit_message>
<xml_diff>
--- a/roscop/code_roscop.xlsx
+++ b/roscop/code_roscop.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgrelet\go\src\github.com\jgrelet\oceano2oceansites\roscop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="96" yWindow="12" windowWidth="14508" windowHeight="8412"/>
+    <workbookView xWindow="90" yWindow="15" windowWidth="14505" windowHeight="8415"/>
   </bookViews>
   <sheets>
     <sheet name="code_roscop" sheetId="5" r:id="rId1"/>
@@ -47,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="260">
   <si>
     <t>long_name</t>
   </si>
@@ -707,9 +712,6 @@
   </si>
   <si>
     <t>CNDC</t>
-  </si>
-  <si>
-    <t>float33</t>
   </si>
   <si>
     <t>electrical conductivity</t>
@@ -835,12 +837,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0E+00"/>
     <numFmt numFmtId="165" formatCode="0.E+00"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1642,7 +1644,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1674,9 +1676,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1708,6 +1711,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1883,37 +1887,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="H34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K58" sqref="K58"/>
+      <selection pane="bottomRight" activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="13"/>
+    <col min="1" max="1" width="11.5703125" style="13"/>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="34.88671875" customWidth="1"/>
-    <col min="4" max="4" width="28.88671875" style="21" customWidth="1"/>
-    <col min="5" max="5" width="24.109375" style="17" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" customWidth="1"/>
-    <col min="7" max="7" width="32.88671875" customWidth="1"/>
-    <col min="8" max="8" width="6.109375" customWidth="1"/>
-    <col min="9" max="9" width="7.5546875" style="6" customWidth="1"/>
-    <col min="10" max="10" width="8.109375" style="6" customWidth="1"/>
-    <col min="11" max="11" width="7.44140625" style="6" customWidth="1"/>
-    <col min="12" max="12" width="7.88671875" style="10" customWidth="1"/>
-    <col min="13" max="13" width="5.6640625" style="6" customWidth="1"/>
-    <col min="14" max="14" width="8.5546875" style="6" customWidth="1"/>
-    <col min="15" max="15" width="34.109375" customWidth="1"/>
-    <col min="16" max="16" width="11.44140625" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" style="21" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" style="17" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="32.85546875" customWidth="1"/>
+    <col min="8" max="8" width="6.140625" customWidth="1"/>
+    <col min="9" max="9" width="7.5703125" style="6" customWidth="1"/>
+    <col min="10" max="10" width="8.140625" style="6" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" style="6" customWidth="1"/>
+    <col min="12" max="12" width="7.85546875" style="10" customWidth="1"/>
+    <col min="13" max="13" width="5.7109375" style="6" customWidth="1"/>
+    <col min="14" max="14" width="8.5703125" style="6" customWidth="1"/>
+    <col min="15" max="15" width="34.140625" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>80</v>
       </c>
@@ -1976,7 +1980,7 @@
       </c>
       <c r="U1" s="8"/>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>13</v>
       </c>
@@ -2039,7 +2043,7 @@
       </c>
       <c r="U2" s="2"/>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>79</v>
       </c>
@@ -2075,7 +2079,7 @@
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>101</v>
       </c>
@@ -2111,7 +2115,7 @@
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>18</v>
       </c>
@@ -2149,7 +2153,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>19</v>
       </c>
@@ -2187,7 +2191,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="15">
+    <row r="7" spans="1:21" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>17</v>
       </c>
@@ -2229,7 +2233,7 @@
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>160</v>
       </c>
@@ -2265,9 +2269,9 @@
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>158</v>
@@ -2293,7 +2297,7 @@
         <v>9000</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L9" s="27">
         <v>1E+36</v>
@@ -2311,7 +2315,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>103</v>
       </c>
@@ -2339,7 +2343,7 @@
         <v>9000</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L10" s="27">
         <v>1E+36</v>
@@ -2357,7 +2361,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
         <v>45</v>
       </c>
@@ -2385,7 +2389,7 @@
         <v>9000</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L11" s="27">
         <v>1E+36</v>
@@ -2401,7 +2405,7 @@
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
         <v>52</v>
       </c>
@@ -2447,7 +2451,7 @@
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
         <v>53</v>
       </c>
@@ -2493,15 +2497,15 @@
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
         <v>219</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>220</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>221</v>
       </c>
       <c r="D14" s="22"/>
       <c r="E14" s="18" t="s">
@@ -2526,7 +2530,7 @@
       </c>
       <c r="M14" s="11"/>
       <c r="N14" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
@@ -2535,9 +2539,9 @@
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>158</v>
@@ -2546,7 +2550,7 @@
         <v>84</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E15" s="18" t="s">
         <v>126</v>
@@ -2573,7 +2577,7 @@
         <v>11</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
@@ -2581,7 +2585,7 @@
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
         <v>56</v>
       </c>
@@ -2627,7 +2631,7 @@
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
         <v>59</v>
       </c>
@@ -2673,7 +2677,7 @@
       <c r="S17" s="3"/>
       <c r="T17" s="3"/>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
         <v>65</v>
       </c>
@@ -2701,7 +2705,7 @@
         <v>1600</v>
       </c>
       <c r="K18" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L18" s="27">
         <v>1E+36</v>
@@ -2719,7 +2723,7 @@
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
         <v>28</v>
       </c>
@@ -2765,7 +2769,7 @@
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
         <v>72</v>
       </c>
@@ -2811,7 +2815,7 @@
       <c r="S20" s="3"/>
       <c r="T20" s="3"/>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
         <v>34</v>
       </c>
@@ -2857,7 +2861,7 @@
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
         <v>37</v>
       </c>
@@ -2903,7 +2907,7 @@
       <c r="S22" s="3"/>
       <c r="T22" s="3"/>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
         <v>40</v>
       </c>
@@ -2949,7 +2953,7 @@
       <c r="S23" s="3"/>
       <c r="T23" s="3"/>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" s="13" t="s">
         <v>67</v>
       </c>
@@ -2993,7 +2997,7 @@
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" s="13" t="s">
         <v>68</v>
       </c>
@@ -3037,7 +3041,7 @@
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="13" t="s">
         <v>63</v>
       </c>
@@ -3083,7 +3087,7 @@
       <c r="S26" s="3"/>
       <c r="T26" s="3"/>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" s="13" t="s">
         <v>27</v>
       </c>
@@ -3129,7 +3133,7 @@
       <c r="S27" s="3"/>
       <c r="T27" s="3"/>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="13" t="s">
         <v>64</v>
       </c>
@@ -3175,7 +3179,7 @@
       <c r="S28" s="3"/>
       <c r="T28" s="3"/>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" s="13" t="s">
         <v>74</v>
       </c>
@@ -3217,7 +3221,7 @@
       <c r="S29" s="3"/>
       <c r="T29" s="3"/>
     </row>
-    <row r="30" spans="1:20">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" s="13" t="s">
         <v>76</v>
       </c>
@@ -3243,7 +3247,7 @@
         <v>1</v>
       </c>
       <c r="K30" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="L30" s="27">
         <v>1E+36</v>
@@ -3259,7 +3263,7 @@
       <c r="S30" s="3"/>
       <c r="T30" s="3"/>
     </row>
-    <row r="31" spans="1:20">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" s="25" t="s">
         <v>194</v>
       </c>
@@ -3301,15 +3305,15 @@
       <c r="S31" s="3"/>
       <c r="T31" s="3"/>
     </row>
-    <row r="32" spans="1:20">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" s="25" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>158</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D32" s="22"/>
       <c r="E32" s="29" t="s">
@@ -3343,7 +3347,7 @@
       <c r="S32" s="3"/>
       <c r="T32" s="3"/>
     </row>
-    <row r="33" spans="1:20">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" s="13" t="s">
         <v>78</v>
       </c>
@@ -3369,7 +3373,7 @@
         <v>100</v>
       </c>
       <c r="K33" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L33" s="27">
         <v>1E+36</v>
@@ -3385,7 +3389,7 @@
       <c r="S33" s="3"/>
       <c r="T33" s="3"/>
     </row>
-    <row r="34" spans="1:20">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" s="25" t="s">
         <v>186</v>
       </c>
@@ -3427,7 +3431,7 @@
       <c r="S34" s="3"/>
       <c r="T34" s="3"/>
     </row>
-    <row r="35" spans="1:20">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" s="25" t="s">
         <v>190</v>
       </c>
@@ -3469,7 +3473,7 @@
       <c r="S35" s="3"/>
       <c r="T35" s="3"/>
     </row>
-    <row r="36" spans="1:20" ht="12.6" customHeight="1">
+    <row r="36" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="25" t="s">
         <v>186</v>
       </c>
@@ -3511,7 +3515,7 @@
       <c r="S36" s="3"/>
       <c r="T36" s="3"/>
     </row>
-    <row r="37" spans="1:20" ht="12.6" customHeight="1">
+    <row r="37" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="25" t="s">
         <v>192</v>
       </c>
@@ -3553,15 +3557,15 @@
       <c r="S37" s="3"/>
       <c r="T37" s="3"/>
     </row>
-    <row r="38" spans="1:20" ht="12.6" customHeight="1">
+    <row r="38" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C38" s="28" t="s">
         <v>226</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C38" s="28" t="s">
-        <v>227</v>
       </c>
       <c r="D38" s="22"/>
       <c r="E38" s="18" t="s">
@@ -3579,7 +3583,7 @@
         <v>100</v>
       </c>
       <c r="K38" s="30" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L38" s="27">
         <v>1E+36</v>
@@ -3595,7 +3599,7 @@
       <c r="S38" s="3"/>
       <c r="T38" s="3"/>
     </row>
-    <row r="39" spans="1:20" ht="12.6" customHeight="1">
+    <row r="39" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="26" t="s">
         <v>197</v>
       </c>
@@ -3637,15 +3641,15 @@
       <c r="S39" s="3"/>
       <c r="T39" s="3"/>
     </row>
-    <row r="40" spans="1:20" ht="12.6" customHeight="1">
+    <row r="40" spans="1:20" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="26" t="s">
+        <v>232</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C40" s="31" t="s">
         <v>233</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C40" s="31" t="s">
-        <v>234</v>
       </c>
       <c r="D40" s="22"/>
       <c r="E40" s="32" t="s">
@@ -3663,7 +3667,7 @@
         <v>500</v>
       </c>
       <c r="K40" s="33" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="L40" s="27">
         <v>1E+36</v>
@@ -3679,7 +3683,7 @@
       <c r="S40" s="3"/>
       <c r="T40" s="3"/>
     </row>
-    <row r="41" spans="1:20">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41" s="13" t="s">
         <v>63</v>
       </c>
@@ -3721,7 +3725,7 @@
       <c r="S41" s="3"/>
       <c r="T41" s="3"/>
     </row>
-    <row r="42" spans="1:20">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42" s="13" t="s">
         <v>105</v>
       </c>
@@ -3763,7 +3767,7 @@
       <c r="S42" s="3"/>
       <c r="T42" s="3"/>
     </row>
-    <row r="43" spans="1:20">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" s="13" t="s">
         <v>110</v>
       </c>
@@ -3805,7 +3809,7 @@
       <c r="S43" s="3"/>
       <c r="T43" s="3"/>
     </row>
-    <row r="44" spans="1:20">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A44" s="13" t="s">
         <v>112</v>
       </c>
@@ -3847,7 +3851,7 @@
       <c r="S44" s="3"/>
       <c r="T44" s="3"/>
     </row>
-    <row r="45" spans="1:20">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A45" s="13" t="s">
         <v>114</v>
       </c>
@@ -3889,7 +3893,7 @@
       <c r="S45" s="3"/>
       <c r="T45" s="3"/>
     </row>
-    <row r="46" spans="1:20">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46" s="13" t="s">
         <v>116</v>
       </c>
@@ -3931,7 +3935,7 @@
       <c r="S46" s="3"/>
       <c r="T46" s="3"/>
     </row>
-    <row r="47" spans="1:20">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47" s="13" t="s">
         <v>118</v>
       </c>
@@ -3973,7 +3977,7 @@
       <c r="S47" s="3"/>
       <c r="T47" s="3"/>
     </row>
-    <row r="48" spans="1:20">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48" s="13" t="s">
         <v>122</v>
       </c>
@@ -4015,7 +4019,7 @@
       <c r="S48" s="3"/>
       <c r="T48" s="3"/>
     </row>
-    <row r="49" spans="1:20">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A49" s="13" t="s">
         <v>124</v>
       </c>
@@ -4057,7 +4061,7 @@
       <c r="S49" s="3"/>
       <c r="T49" s="3"/>
     </row>
-    <row r="50" spans="1:20">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50" s="13" t="s">
         <v>128</v>
       </c>
@@ -4099,7 +4103,7 @@
       <c r="S50" s="3"/>
       <c r="T50" s="3"/>
     </row>
-    <row r="51" spans="1:20">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A51" s="13" t="s">
         <v>130</v>
       </c>
@@ -4141,7 +4145,7 @@
       <c r="S51" s="3"/>
       <c r="T51" s="3"/>
     </row>
-    <row r="52" spans="1:20">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A52" s="13" t="s">
         <v>132</v>
       </c>
@@ -4183,7 +4187,7 @@
       <c r="S52" s="3"/>
       <c r="T52" s="3"/>
     </row>
-    <row r="53" spans="1:20">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A53" s="13" t="s">
         <v>133</v>
       </c>
@@ -4225,7 +4229,7 @@
       <c r="S53" s="3"/>
       <c r="T53" s="3"/>
     </row>
-    <row r="54" spans="1:20">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A54" s="13" t="s">
         <v>137</v>
       </c>
@@ -4267,7 +4271,7 @@
       <c r="S54" s="3"/>
       <c r="T54" s="3"/>
     </row>
-    <row r="55" spans="1:20">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A55" s="13" t="s">
         <v>139</v>
       </c>
@@ -4309,7 +4313,7 @@
       <c r="S55" s="3"/>
       <c r="T55" s="3"/>
     </row>
-    <row r="56" spans="1:20">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A56" s="13" t="s">
         <v>143</v>
       </c>
@@ -4342,7 +4346,7 @@
       </c>
       <c r="M56" s="11"/>
       <c r="N56" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="O56" s="3"/>
       <c r="P56" s="3"/>
@@ -4351,18 +4355,18 @@
       <c r="S56" s="3"/>
       <c r="T56" s="3"/>
     </row>
-    <row r="57" spans="1:20">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A57" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="D57" s="22" t="s">
         <v>240</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="D57" s="22" t="s">
-        <v>241</v>
       </c>
       <c r="E57" s="18" t="s">
         <v>57</v>
@@ -4395,21 +4399,21 @@
       <c r="S57" s="3"/>
       <c r="T57" s="3"/>
     </row>
-    <row r="58" spans="1:20">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A58" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C58" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="B58" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="C58" s="3" t="s">
+      <c r="D58" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="E58" s="18" t="s">
         <v>238</v>
-      </c>
-      <c r="D58" s="22" t="s">
-        <v>242</v>
-      </c>
-      <c r="E58" s="18" t="s">
-        <v>239</v>
       </c>
       <c r="F58" s="3"/>
       <c r="G58" s="3" t="s">
@@ -4439,18 +4443,18 @@
       <c r="S58" s="3"/>
       <c r="T58" s="3"/>
     </row>
-    <row r="59" spans="1:20">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A59" s="13" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>220</v>
+        <v>158</v>
       </c>
       <c r="C59" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D59" s="22" t="s">
         <v>250</v>
-      </c>
-      <c r="D59" s="22" t="s">
-        <v>251</v>
       </c>
       <c r="E59" s="18" t="s">
         <v>57</v>
@@ -4483,21 +4487,21 @@
       <c r="S59" s="3"/>
       <c r="T59" s="3"/>
     </row>
-    <row r="60" spans="1:20">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A60" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C60" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="B60" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>250</v>
-      </c>
       <c r="D60" s="22" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E60" s="18" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F60" s="3"/>
       <c r="G60" s="3" t="s">
@@ -4527,18 +4531,18 @@
       <c r="S60" s="3"/>
       <c r="T60" s="3"/>
     </row>
-    <row r="61" spans="1:20">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A61" s="13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>220</v>
+        <v>158</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D61" s="22" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E61" s="18" t="s">
         <v>57</v>
@@ -4571,21 +4575,21 @@
       <c r="S61" s="3"/>
       <c r="T61" s="3"/>
     </row>
-    <row r="62" spans="1:20">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A62" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C62" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="B62" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="C62" s="3" t="s">
+      <c r="D62" s="22" t="s">
         <v>245</v>
       </c>
-      <c r="D62" s="22" t="s">
-        <v>246</v>
-      </c>
       <c r="E62" s="18" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F62" s="3"/>
       <c r="G62" s="3" t="s">
@@ -4599,7 +4603,7 @@
         <v>100</v>
       </c>
       <c r="K62" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L62" s="27">
         <v>1E+36</v>
@@ -4615,18 +4619,18 @@
       <c r="S62" s="3"/>
       <c r="T62" s="3"/>
     </row>
-    <row r="63" spans="1:20">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A63" s="13" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>220</v>
+        <v>158</v>
       </c>
       <c r="C63" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="D63" s="22" t="s">
         <v>255</v>
-      </c>
-      <c r="D63" s="22" t="s">
-        <v>256</v>
       </c>
       <c r="E63" s="18" t="s">
         <v>57</v>
@@ -4659,21 +4663,21 @@
       <c r="S63" s="3"/>
       <c r="T63" s="3"/>
     </row>
-    <row r="64" spans="1:20">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A64" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C64" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="B64" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>255</v>
-      </c>
       <c r="D64" s="22" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E64" s="18" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F64" s="3"/>
       <c r="G64" s="3" t="s">
@@ -4703,19 +4707,19 @@
       <c r="S64" s="3"/>
       <c r="T64" s="3"/>
     </row>
-    <row r="65" spans="1:20">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A65" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C65" s="3" t="s">
         <v>258</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>259</v>
       </c>
       <c r="D65" s="22"/>
       <c r="E65" s="18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F65" s="3"/>
       <c r="G65" s="3" t="s">
@@ -4745,7 +4749,7 @@
       <c r="S65" s="3"/>
       <c r="T65" s="3"/>
     </row>
-    <row r="66" spans="1:20">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A66" s="13" t="s">
         <v>145</v>
       </c>
@@ -4787,7 +4791,7 @@
       <c r="S66" s="3"/>
       <c r="T66" s="3"/>
     </row>
-    <row r="67" spans="1:20">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A67" s="13" t="s">
         <v>148</v>
       </c>
@@ -4833,7 +4837,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="68" spans="1:20">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A68" s="14" t="s">
         <v>201</v>
       </c>
@@ -4871,7 +4875,7 @@
       <c r="S68" s="3"/>
       <c r="T68" s="3"/>
     </row>
-    <row r="69" spans="1:20">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A69" s="13" t="s">
         <v>152</v>
       </c>
@@ -4909,7 +4913,7 @@
       <c r="S69" s="3"/>
       <c r="T69" s="3"/>
     </row>
-    <row r="70" spans="1:20">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A70" s="13" t="s">
         <v>155</v>
       </c>
@@ -4947,7 +4951,7 @@
       <c r="S70" s="3"/>
       <c r="T70" s="3"/>
     </row>
-    <row r="71" spans="1:20">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A71" s="13" t="s">
         <v>182</v>
       </c>

</xml_diff>